<commit_message>
Actualización automática 2025-05-29 10:10:07
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,7 +447,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="27" customWidth="1" min="2" max="2"/>
+    <col width="33" customWidth="1" min="2" max="2"/>
     <col width="25" customWidth="1" min="3" max="3"/>
     <col width="24" customWidth="1" min="4" max="4"/>
     <col width="26" customWidth="1" min="5" max="5"/>
@@ -583,64 +583,112 @@
       </c>
     </row>
     <row r="3">
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="F3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="H3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="I3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="J3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="K3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="L3" s="3" t="inlineStr">
-        <is>
-          <t>1 de 1</t>
-        </is>
-      </c>
-      <c r="M3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="N3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="J4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="L4" s="3" t="inlineStr">
+        <is>
+          <t>1 de 2</t>
+        </is>
+      </c>
+      <c r="M4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="N4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
         </is>
       </c>
     </row>
@@ -655,7 +703,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -664,7 +712,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="27" customWidth="1" min="2" max="2"/>
+    <col width="33" customWidth="1" min="2" max="2"/>
     <col width="13" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
@@ -728,16 +776,40 @@
       </c>
     </row>
     <row r="3">
-      <c r="C3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="n">
         <v>144.53</v>
       </c>
-      <c r="F3" s="5" t="n">
+      <c r="F4" s="5" t="n">
         <v>11.52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-05-29 15:05:07
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -716,7 +716,7 @@
     <col width="13" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -796,7 +796,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0</v>
+        <v>178.33</v>
       </c>
     </row>
     <row r="4">
@@ -810,7 +810,7 @@
         <v>144.53</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>11.52</v>
+        <v>189.85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-04 16:05:06
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="VENTAS POR GRUPO" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="VENTA MENSUAL" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="CUMPLIMIENTO MENSUAL" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -68,11 +69,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -812,19 +811,126 @@
       </c>
     </row>
     <row r="4">
-      <c r="C4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5" t="n">
+      <c r="C4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <v>144.53</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="4" t="n">
         <v>189.85</v>
       </c>
-      <c r="F4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5" t="n">
+      <c r="F4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="17" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ASESOR</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>GRUPO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>PRESUPUESTO</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>POR CUMPLIR</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>CUMPLIMIENTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>605.48</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>-605.48</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>17500</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>17500</v>
+      </c>
+      <c r="F3" s="5" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-06-10 14:05:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -854,7 +854,7 @@
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="17" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -928,13 +928,13 @@
         <v>17500</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>24.31</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>17500</v>
+        <v>17475.69</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0</v>
+        <v>0.001389142857142857</v>
       </c>
     </row>
     <row r="4">
@@ -947,13 +947,13 @@
         <v>17500</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>748.04</v>
+        <v>772.3499999999999</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>16751.96</v>
+        <v>16727.65</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.04274514285714286</v>
+        <v>0.04413428571428571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-10 17:00:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -904,10 +904,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>748.04</v>
+        <v>1711.4</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-748.04</v>
+        <v>-1711.4</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -947,13 +947,13 @@
         <v>17500</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>772.3499999999999</v>
+        <v>1735.71</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>16727.65</v>
+        <v>15764.29</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.04413428571428571</v>
+        <v>0.09918342857142858</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-19 09:35:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1007,7 +1007,7 @@
     <col width="18" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
     <col width="17" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
@@ -1059,10 +1059,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>2942.59</v>
+        <v>3076.4</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-2942.59</v>
+        <v>-3076.4</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1102,13 +1102,13 @@
         <v>17500</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>3191.07</v>
+        <v>3324.88</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>14308.93</v>
+        <v>14175.12</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.1823468571428571</v>
+        <v>0.1899931428571429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-19 12:50:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1007,7 +1007,7 @@
     <col width="18" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
     <col width="17" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
@@ -1059,10 +1059,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3076.4</v>
+        <v>2942.59</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-3076.4</v>
+        <v>-2942.59</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1102,13 +1102,13 @@
         <v>17500</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>3324.88</v>
+        <v>3191.07</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>14175.12</v>
+        <v>14308.93</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.1899931428571429</v>
+        <v>0.1823468571428571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-19 13:25:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1059,10 +1059,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>2942.59</v>
+        <v>3059.12</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-2942.59</v>
+        <v>-3059.12</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1102,13 +1102,13 @@
         <v>17500</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>3191.07</v>
+        <v>3307.6</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>14308.93</v>
+        <v>14192.4</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.1823468571428571</v>
+        <v>0.1890057142857143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-19 14:50:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1007,7 +1007,7 @@
     <col width="18" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
     <col width="17" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
@@ -1059,10 +1059,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3059.12</v>
+        <v>3566</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-3059.12</v>
+        <v>-3566</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1083,13 +1083,13 @@
         <v>17500</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>248.48</v>
+        <v>321.85</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>17251.52</v>
+        <v>17178.15</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.01419885714285714</v>
+        <v>0.01839142857142857</v>
       </c>
     </row>
     <row r="4">
@@ -1102,13 +1102,13 @@
         <v>17500</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>3307.6</v>
+        <v>3887.85</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>14192.4</v>
+        <v>13612.15</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.1890057142857143</v>
+        <v>0.2221628571428571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-20 15:25:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1007,7 +1007,7 @@
     <col width="18" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
     <col width="17" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
@@ -1059,10 +1059,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3566</v>
+        <v>3788.63</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-3566</v>
+        <v>-3788.63</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1102,13 +1102,13 @@
         <v>17500</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>3887.85</v>
+        <v>4110.48</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>13612.15</v>
+        <v>13389.52</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.2221628571428571</v>
+        <v>0.2348845714285714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-23 15:15:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,7 +449,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="33" customWidth="1" min="2" max="2"/>
+    <col width="34" customWidth="1" min="2" max="2"/>
     <col width="25" customWidth="1" min="3" max="3"/>
     <col width="24" customWidth="1" min="4" max="4"/>
     <col width="26" customWidth="1" min="5" max="5"/>
@@ -628,7 +628,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -688,137 +688,197 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>LOZANO MOLINA TITO JERSON</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>0 de 3</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>1 de 3</t>
-        </is>
-      </c>
-      <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>0 de 3</t>
-        </is>
-      </c>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>0 de 3</t>
-        </is>
-      </c>
-      <c r="G5" s="3" t="inlineStr">
-        <is>
-          <t>0 de 3</t>
-        </is>
-      </c>
-      <c r="H5" s="3" t="inlineStr">
-        <is>
-          <t>0 de 3</t>
-        </is>
-      </c>
-      <c r="I5" s="3" t="inlineStr">
-        <is>
-          <t>0 de 3</t>
-        </is>
-      </c>
-      <c r="J5" s="3" t="inlineStr">
-        <is>
-          <t>0 de 3</t>
-        </is>
-      </c>
-      <c r="K5" s="3" t="inlineStr">
-        <is>
-          <t>0 de 3</t>
-        </is>
-      </c>
-      <c r="L5" s="3" t="inlineStr">
-        <is>
-          <t>0 de 3</t>
-        </is>
-      </c>
-      <c r="M5" s="3" t="inlineStr">
-        <is>
-          <t>0 de 3</t>
-        </is>
-      </c>
-      <c r="N5" s="3" t="inlineStr">
-        <is>
-          <t>0 de 3</t>
-        </is>
-      </c>
-      <c r="O5" s="3" t="inlineStr">
-        <is>
-          <t>0 de 3</t>
-        </is>
-      </c>
-      <c r="P5" s="3" t="inlineStr">
-        <is>
-          <t>0 de 3</t>
-        </is>
-      </c>
-      <c r="Q5" s="3" t="inlineStr">
-        <is>
-          <t>0 de 3</t>
-        </is>
-      </c>
-      <c r="R5" s="3" t="inlineStr">
-        <is>
-          <t>0 de 3</t>
+      <c r="C5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>0 de 4</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>1 de 4</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>0 de 4</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>0 de 4</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>0 de 4</t>
+        </is>
+      </c>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>0 de 4</t>
+        </is>
+      </c>
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>0 de 4</t>
+        </is>
+      </c>
+      <c r="J6" s="3" t="inlineStr">
+        <is>
+          <t>0 de 4</t>
+        </is>
+      </c>
+      <c r="K6" s="3" t="inlineStr">
+        <is>
+          <t>0 de 4</t>
+        </is>
+      </c>
+      <c r="L6" s="3" t="inlineStr">
+        <is>
+          <t>0 de 4</t>
+        </is>
+      </c>
+      <c r="M6" s="3" t="inlineStr">
+        <is>
+          <t>0 de 4</t>
+        </is>
+      </c>
+      <c r="N6" s="3" t="inlineStr">
+        <is>
+          <t>0 de 4</t>
+        </is>
+      </c>
+      <c r="O6" s="3" t="inlineStr">
+        <is>
+          <t>0 de 4</t>
+        </is>
+      </c>
+      <c r="P6" s="3" t="inlineStr">
+        <is>
+          <t>0 de 4</t>
+        </is>
+      </c>
+      <c r="Q6" s="3" t="inlineStr">
+        <is>
+          <t>0 de 4</t>
+        </is>
+      </c>
+      <c r="R6" s="3" t="inlineStr">
+        <is>
+          <t>0 de 4</t>
         </is>
       </c>
     </row>
@@ -833,7 +893,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -842,7 +902,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="33" customWidth="1" min="2" max="2"/>
+    <col width="34" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
@@ -922,17 +982,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>144.53</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>11.52</v>
+        <v>0</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0</v>
@@ -949,39 +1009,66 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>LOZANO MOLINA TITO JERSON</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>144.53</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>11.52</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="n">
+      <c r="C5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="n">
         <v>178.33</v>
       </c>
-      <c r="F4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4" t="n">
+      <c r="F5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="n">
         <v>144.53</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E6" s="4" t="n">
         <v>189.85</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F6" s="4" t="n">
         <v>472.57</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G6" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-06-24 14:25:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -801,84 +801,144 @@
       </c>
     </row>
     <row r="6">
-      <c r="C6" s="3" t="inlineStr">
-        <is>
-          <t>0 de 4</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>1 de 4</t>
-        </is>
-      </c>
-      <c r="E6" s="3" t="inlineStr">
-        <is>
-          <t>0 de 4</t>
-        </is>
-      </c>
-      <c r="F6" s="3" t="inlineStr">
-        <is>
-          <t>0 de 4</t>
-        </is>
-      </c>
-      <c r="G6" s="3" t="inlineStr">
-        <is>
-          <t>0 de 4</t>
-        </is>
-      </c>
-      <c r="H6" s="3" t="inlineStr">
-        <is>
-          <t>0 de 4</t>
-        </is>
-      </c>
-      <c r="I6" s="3" t="inlineStr">
-        <is>
-          <t>0 de 4</t>
-        </is>
-      </c>
-      <c r="J6" s="3" t="inlineStr">
-        <is>
-          <t>0 de 4</t>
-        </is>
-      </c>
-      <c r="K6" s="3" t="inlineStr">
-        <is>
-          <t>0 de 4</t>
-        </is>
-      </c>
-      <c r="L6" s="3" t="inlineStr">
-        <is>
-          <t>0 de 4</t>
-        </is>
-      </c>
-      <c r="M6" s="3" t="inlineStr">
-        <is>
-          <t>0 de 4</t>
-        </is>
-      </c>
-      <c r="N6" s="3" t="inlineStr">
-        <is>
-          <t>0 de 4</t>
-        </is>
-      </c>
-      <c r="O6" s="3" t="inlineStr">
-        <is>
-          <t>0 de 4</t>
-        </is>
-      </c>
-      <c r="P6" s="3" t="inlineStr">
-        <is>
-          <t>0 de 4</t>
-        </is>
-      </c>
-      <c r="Q6" s="3" t="inlineStr">
-        <is>
-          <t>0 de 4</t>
-        </is>
-      </c>
-      <c r="R6" s="3" t="inlineStr">
-        <is>
-          <t>0 de 4</t>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>1 de 5</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="K7" s="3" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="L7" s="3" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="M7" s="3" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="N7" s="3" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="O7" s="3" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="P7" s="3" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="Q7" s="3" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="R7" s="3" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
         </is>
       </c>
     </row>
@@ -893,7 +953,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1056,19 +1116,46 @@
       </c>
     </row>
     <row r="6">
-      <c r="C6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4" t="n">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4" t="n">
         <v>144.53</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E7" s="4" t="n">
         <v>189.85</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="F7" s="4" t="n">
         <v>472.57</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G7" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-06-24 15:25:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,14 +568,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
+          <t>AREVALO PEÑA JORGE LUIS</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>472.57</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>0</v>
@@ -628,14 +628,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>472.57</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>0</v>
@@ -688,7 +688,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -748,7 +748,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -808,137 +808,197 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>1 de 5</t>
-        </is>
-      </c>
-      <c r="E7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="F7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="G7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="H7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="I7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="J7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="K7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="L7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="M7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="N7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="O7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="P7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="Q7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="R7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
+      <c r="C7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>1 de 6</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="K8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="L8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="M8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="N8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="O8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="P8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="Q8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="R8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
         </is>
       </c>
     </row>
@@ -953,7 +1013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1015,7 +1075,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
+          <t>AREVALO PEÑA JORGE LUIS</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -1028,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>472.57</v>
+        <v>0</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>0</v>
@@ -1042,7 +1102,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -1055,7 +1115,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0</v>
+        <v>472.57</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>0</v>
@@ -1069,17 +1129,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>144.53</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>11.52</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>0</v>
@@ -1096,17 +1156,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0</v>
+        <v>144.53</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>178.33</v>
+        <v>11.52</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0</v>
@@ -1123,39 +1183,66 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>178.33</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4" t="n">
+      <c r="C7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="n">
         <v>144.53</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="E8" s="4" t="n">
         <v>189.85</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="F8" s="4" t="n">
         <v>472.57</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G8" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-06-24 16:40:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1320,10 +1320,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3799.07</v>
+        <v>3809.51</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-3799.07</v>
+        <v>-3809.51</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1363,13 +1363,13 @@
         <v>17500</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>4120.92</v>
+        <v>4131.360000000001</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>13379.08</v>
+        <v>13368.64</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.2354811428571429</v>
+        <v>0.2360777142857143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-24 16:45:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1320,10 +1320,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3809.51</v>
+        <v>3819.95</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-3809.51</v>
+        <v>-3819.95</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1363,13 +1363,13 @@
         <v>17500</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>4131.360000000001</v>
+        <v>4141.8</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>13368.64</v>
+        <v>13358.2</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.2360777142857143</v>
+        <v>0.2366742857142857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-24 17:00:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1344,13 +1344,13 @@
         <v>17500</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>321.85</v>
+        <v>548.46</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>17178.15</v>
+        <v>16951.54</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.01839142857142857</v>
+        <v>0.03134057142857143</v>
       </c>
     </row>
     <row r="4">
@@ -1363,13 +1363,13 @@
         <v>17500</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>4141.8</v>
+        <v>4368.41</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>13358.2</v>
+        <v>13131.59</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.2366742857142857</v>
+        <v>0.2496234285714286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-30 09:40:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -457,7 +457,7 @@
     <col width="15" customWidth="1" min="7" max="7"/>
     <col width="14" customWidth="1" min="8" max="8"/>
     <col width="13" customWidth="1" min="9" max="9"/>
-    <col width="9" customWidth="1" min="10" max="10"/>
+    <col width="11" customWidth="1" min="10" max="10"/>
     <col width="25" customWidth="1" min="11" max="11"/>
     <col width="24" customWidth="1" min="12" max="12"/>
     <col width="17" customWidth="1" min="13" max="13"/>
@@ -695,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0</v>
+        <v>434.83</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>0</v>
@@ -893,7 +893,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>0</v>
+        <v>36.74</v>
       </c>
       <c r="K7" s="2" t="n">
         <v>0</v>
@@ -905,7 +905,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="2" t="n">
-        <v>0</v>
+        <v>100.71</v>
       </c>
       <c r="O7" s="2" t="n">
         <v>0</v>
@@ -914,7 +914,7 @@
         <v>0</v>
       </c>
       <c r="Q7" s="2" t="n">
-        <v>0</v>
+        <v>21.58</v>
       </c>
       <c r="R7" s="2" t="n">
         <v>0</v>
@@ -928,72 +928,72 @@
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
+          <t>2 de 6</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
           <t>1 de 6</t>
         </is>
       </c>
-      <c r="E8" s="3" t="inlineStr">
+      <c r="K8" s="3" t="inlineStr">
         <is>
           <t>0 de 6</t>
         </is>
       </c>
-      <c r="F8" s="3" t="inlineStr">
+      <c r="L8" s="3" t="inlineStr">
         <is>
           <t>0 de 6</t>
         </is>
       </c>
-      <c r="G8" s="3" t="inlineStr">
+      <c r="M8" s="3" t="inlineStr">
         <is>
           <t>0 de 6</t>
         </is>
       </c>
-      <c r="H8" s="3" t="inlineStr">
+      <c r="N8" s="3" t="inlineStr">
+        <is>
+          <t>1 de 6</t>
+        </is>
+      </c>
+      <c r="O8" s="3" t="inlineStr">
         <is>
           <t>0 de 6</t>
         </is>
       </c>
-      <c r="I8" s="3" t="inlineStr">
+      <c r="P8" s="3" t="inlineStr">
         <is>
           <t>0 de 6</t>
         </is>
       </c>
-      <c r="J8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="K8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="L8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="M8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="N8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="O8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="P8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
       <c r="Q8" s="3" t="inlineStr">
         <is>
-          <t>0 de 6</t>
+          <t>1 de 6</t>
         </is>
       </c>
       <c r="R8" s="3" t="inlineStr">
@@ -1142,7 +1142,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0</v>
+        <v>434.83</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>0</v>
@@ -1223,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0</v>
+        <v>159.03</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>0</v>
@@ -1240,7 +1240,7 @@
         <v>189.85</v>
       </c>
       <c r="F8" s="4" t="n">
-        <v>472.57</v>
+        <v>1066.43</v>
       </c>
       <c r="G8" s="4" t="n">
         <v>0</v>
@@ -1320,10 +1320,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>4430.59</v>
+        <v>5043.87</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-4430.59</v>
+        <v>-5043.87</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1363,13 +1363,13 @@
         <v>17500</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>5025.37</v>
+        <v>5638.65</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>12474.63</v>
+        <v>11861.35</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.287164</v>
+        <v>0.3222085714285714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-01 11:50:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,7 +568,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AREVALO PEÑA JORGE LUIS</t>
+          <t>ANGULO PARRALES CARMEN</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -628,7 +628,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
+          <t>AREVALO PEÑA JORGE LUIS</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -688,7 +688,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -748,7 +748,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -808,7 +808,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -868,137 +868,197 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="C8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="E8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="F8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="G8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="H8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="I8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="J8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="K8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="L8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="M8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="N8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="O8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="P8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="Q8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="R8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
+      <c r="C8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="M9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="N9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="O9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="P9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="Q9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="R9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
         </is>
       </c>
     </row>
@@ -1013,7 +1073,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1075,7 +1135,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AREVALO PEÑA JORGE LUIS</t>
+          <t>ANGULO PARRALES CARMEN</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -1102,7 +1162,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
+          <t>AREVALO PEÑA JORGE LUIS</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -1112,7 +1172,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>472.57</v>
+        <v>0</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0</v>
@@ -1129,7 +1189,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -1139,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>434.83</v>
+        <v>472.57</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>0</v>
@@ -1156,17 +1216,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>144.53</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>11.52</v>
+        <v>0</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>10.44</v>
+        <v>434.83</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0</v>
@@ -1183,17 +1243,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0</v>
+        <v>144.53</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>178.33</v>
+        <v>11.52</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
@@ -1210,39 +1270,66 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>178.33</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="n">
+      <c r="C8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="n">
         <v>159.03</v>
       </c>
-      <c r="F7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="C8" s="4" t="n">
+      <c r="F8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" s="4" t="n">
         <v>144.53</v>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="D9" s="4" t="n">
         <v>189.85</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="E9" s="4" t="n">
         <v>1076.87</v>
       </c>
-      <c r="F8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4" t="n">
+      <c r="F9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-07-01 14:25:07
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -602,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>0</v>
+        <v>66.2</v>
       </c>
       <c r="N2" s="2" t="n">
         <v>0</v>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="M9" s="3" t="inlineStr">
         <is>
-          <t>0 de 7</t>
+          <t>1 de 7</t>
         </is>
       </c>
       <c r="N9" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0</v>
+        <v>66.2</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>0</v>
@@ -1327,7 +1327,7 @@
         <v>1076.87</v>
       </c>
       <c r="F9" s="4" t="n">
-        <v>0</v>
+        <v>66.2</v>
       </c>
       <c r="G9" s="4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Actualización automática 2025-07-01 14:40:07
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -981,84 +981,144 @@
       </c>
     </row>
     <row r="9">
-      <c r="C9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="D9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="E9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="F9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="G9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="H9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="I9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="J9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="K9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="L9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="M9" s="3" t="inlineStr">
-        <is>
-          <t>1 de 7</t>
-        </is>
-      </c>
-      <c r="N9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="O9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="P9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="Q9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="R9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="G10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="L10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="M10" s="3" t="inlineStr">
+        <is>
+          <t>1 de 8</t>
+        </is>
+      </c>
+      <c r="N10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="O10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="P10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="Q10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="R10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
         </is>
       </c>
     </row>
@@ -1073,7 +1133,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1317,19 +1377,46 @@
       </c>
     </row>
     <row r="9">
-      <c r="C9" s="4" t="n">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" s="4" t="n">
         <v>144.53</v>
       </c>
-      <c r="D9" s="4" t="n">
+      <c r="D10" s="4" t="n">
         <v>189.85</v>
       </c>
-      <c r="E9" s="4" t="n">
+      <c r="E10" s="4" t="n">
         <v>1076.87</v>
       </c>
-      <c r="F9" s="4" t="n">
+      <c r="F10" s="4" t="n">
         <v>66.2</v>
       </c>
-      <c r="G9" s="4" t="n">
+      <c r="G10" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-07-02 14:35:07
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1010,7 +1010,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>0</v>
+        <v>43.86</v>
       </c>
       <c r="J9" s="2" t="n">
         <v>0</v>
@@ -1073,7 +1073,7 @@
       </c>
       <c r="I10" s="3" t="inlineStr">
         <is>
-          <t>0 de 8</t>
+          <t>1 de 8</t>
         </is>
       </c>
       <c r="J10" s="3" t="inlineStr">
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0</v>
+        <v>43.86</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>0</v>
@@ -1414,7 +1414,7 @@
         <v>1076.87</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>66.2</v>
+        <v>110.06</v>
       </c>
       <c r="G10" s="4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Actualización automática 2025-07-03 17:10:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1494,10 +1494,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>-42.54</v>
+        <v>61.86</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>42.54</v>
+        <v>-61.86</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1537,13 +1537,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>289.21</v>
+        <v>393.61</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>13434.13</v>
+        <v>13329.73</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.02107431572780387</v>
+        <v>0.02868179320777595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-08 11:40:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,7 +449,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="34" customWidth="1" min="2" max="2"/>
+    <col width="36" customWidth="1" min="2" max="2"/>
     <col width="25" customWidth="1" min="3" max="3"/>
     <col width="24" customWidth="1" min="4" max="4"/>
     <col width="26" customWidth="1" min="5" max="5"/>
@@ -568,7 +568,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ANGULO PARRALES CARMEN</t>
+          <t>ALCIVAR BUSTAMANTE ERNESTO EDUARDO</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -602,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>66.2</v>
+        <v>0</v>
       </c>
       <c r="N2" s="2" t="n">
         <v>0</v>
@@ -628,7 +628,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AREVALO PEÑA JORGE LUIS</t>
+          <t>ANGULO PARRALES CARMEN</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -662,7 +662,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>0</v>
+        <v>66.2</v>
       </c>
       <c r="N3" s="2" t="n">
         <v>0</v>
@@ -688,7 +688,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
+          <t>AREVALO PEÑA JORGE LUIS</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -748,7 +748,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -808,7 +808,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -868,7 +868,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -928,7 +928,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -988,137 +988,197 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2" t="n">
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="n">
         <v>43.86</v>
       </c>
-      <c r="J9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="C10" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
-        </is>
-      </c>
-      <c r="D10" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
-        </is>
-      </c>
-      <c r="E10" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
-        </is>
-      </c>
-      <c r="F10" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
-        </is>
-      </c>
-      <c r="G10" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
-        </is>
-      </c>
-      <c r="H10" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
-        </is>
-      </c>
-      <c r="I10" s="3" t="inlineStr">
-        <is>
-          <t>1 de 8</t>
-        </is>
-      </c>
-      <c r="J10" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
-        </is>
-      </c>
-      <c r="K10" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
-        </is>
-      </c>
-      <c r="L10" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
-        </is>
-      </c>
-      <c r="M10" s="3" t="inlineStr">
-        <is>
-          <t>1 de 8</t>
-        </is>
-      </c>
-      <c r="N10" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
-        </is>
-      </c>
-      <c r="O10" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
-        </is>
-      </c>
-      <c r="P10" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
-        </is>
-      </c>
-      <c r="Q10" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
-        </is>
-      </c>
-      <c r="R10" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
+      <c r="J10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>0 de 9</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>0 de 9</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>0 de 9</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>0 de 9</t>
+        </is>
+      </c>
+      <c r="G11" s="3" t="inlineStr">
+        <is>
+          <t>0 de 9</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>0 de 9</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>1 de 9</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>0 de 9</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>0 de 9</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>0 de 9</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="inlineStr">
+        <is>
+          <t>1 de 9</t>
+        </is>
+      </c>
+      <c r="N11" s="3" t="inlineStr">
+        <is>
+          <t>0 de 9</t>
+        </is>
+      </c>
+      <c r="O11" s="3" t="inlineStr">
+        <is>
+          <t>0 de 9</t>
+        </is>
+      </c>
+      <c r="P11" s="3" t="inlineStr">
+        <is>
+          <t>0 de 9</t>
+        </is>
+      </c>
+      <c r="Q11" s="3" t="inlineStr">
+        <is>
+          <t>0 de 9</t>
+        </is>
+      </c>
+      <c r="R11" s="3" t="inlineStr">
+        <is>
+          <t>0 de 9</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1193,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1142,7 +1202,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="34" customWidth="1" min="2" max="2"/>
+    <col width="36" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
@@ -1195,7 +1255,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ANGULO PARRALES CARMEN</t>
+          <t>ALCIVAR BUSTAMANTE ERNESTO EDUARDO</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -1208,7 +1268,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>66.2</v>
+        <v>0</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>0</v>
@@ -1222,7 +1282,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AREVALO PEÑA JORGE LUIS</t>
+          <t>ANGULO PARRALES CARMEN</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -1235,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0</v>
+        <v>66.2</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>0</v>
@@ -1249,7 +1309,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
+          <t>AREVALO PEÑA JORGE LUIS</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -1259,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>472.57</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>0</v>
@@ -1276,7 +1336,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -1286,7 +1346,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>434.83</v>
+        <v>472.57</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0</v>
@@ -1303,17 +1363,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>144.53</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>11.52</v>
+        <v>0</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>10.44</v>
+        <v>434.83</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
@@ -1330,17 +1390,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0</v>
+        <v>144.53</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>178.33</v>
+        <v>11.52</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0</v>
@@ -1357,17 +1417,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0</v>
+        <v>178.33</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>159.03</v>
+        <v>0</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0</v>
@@ -1384,39 +1444,66 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>159.03</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2" t="n">
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2" t="n">
         <v>43.86</v>
       </c>
-      <c r="G9" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="C10" s="4" t="n">
+      <c r="G10" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" s="4" t="n">
         <v>144.53</v>
       </c>
-      <c r="D10" s="4" t="n">
+      <c r="D11" s="4" t="n">
         <v>189.85</v>
       </c>
-      <c r="E10" s="4" t="n">
+      <c r="E11" s="4" t="n">
         <v>1076.87</v>
       </c>
-      <c r="F10" s="4" t="n">
+      <c r="F11" s="4" t="n">
         <v>110.06</v>
       </c>
-      <c r="G10" s="4" t="n">
+      <c r="G11" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-07-08 15:05:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1581,10 +1581,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>925.91</v>
+        <v>906.49</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-925.91</v>
+        <v>-906.49</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1624,13 +1624,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>1478.34</v>
+        <v>1458.92</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>12245</v>
+        <v>12264.42</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.1077245043845011</v>
+        <v>0.1063093969835332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-08 16:45:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1101,84 +1101,144 @@
       </c>
     </row>
     <row r="11">
-      <c r="C11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="D11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="E11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="F11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="G11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="H11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="I11" s="3" t="inlineStr">
-        <is>
-          <t>1 de 9</t>
-        </is>
-      </c>
-      <c r="J11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="K11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="L11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="M11" s="3" t="inlineStr">
-        <is>
-          <t>1 de 9</t>
-        </is>
-      </c>
-      <c r="N11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="O11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="P11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="Q11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="R11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>VEHINVER SA</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>1 de 10</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>1 de 10</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="O12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="P12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="Q12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="R12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
         </is>
       </c>
     </row>
@@ -1193,7 +1253,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1491,19 +1551,46 @@
       </c>
     </row>
     <row r="11">
-      <c r="C11" s="4" t="n">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>VEHINVER SA</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="4" t="n">
         <v>144.53</v>
       </c>
-      <c r="D11" s="4" t="n">
+      <c r="D12" s="4" t="n">
         <v>189.85</v>
       </c>
-      <c r="E11" s="4" t="n">
+      <c r="E12" s="4" t="n">
         <v>1076.87</v>
       </c>
-      <c r="F11" s="4" t="n">
+      <c r="F12" s="4" t="n">
         <v>110.06</v>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="G12" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-07-09 08:30:07
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1668,10 +1668,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>906.49</v>
+        <v>1184.9</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-906.49</v>
+        <v>-1184.9</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1711,13 +1711,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>1458.92</v>
+        <v>1737.33</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>12264.42</v>
+        <v>11986.01</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.1063093969835332</v>
+        <v>0.1265967322823744</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-09 14:35:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -608,7 +608,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>0</v>
+        <v>30.31</v>
       </c>
       <c r="P2" s="2" t="n">
         <v>0</v>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="O12" s="3" t="inlineStr">
         <is>
-          <t>0 de 10</t>
+          <t>1 de 10</t>
         </is>
       </c>
       <c r="P12" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0</v>
+        <v>30.31</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>0</v>
@@ -1588,7 +1588,7 @@
         <v>1076.87</v>
       </c>
       <c r="F12" s="4" t="n">
-        <v>110.06</v>
+        <v>140.37</v>
       </c>
       <c r="G12" s="4" t="n">
         <v>0</v>
@@ -1668,10 +1668,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>1460.22</v>
+        <v>1769.08</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-1460.22</v>
+        <v>-1769.08</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1692,13 +1692,13 @@
         <v>13723.34</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>809.04</v>
+        <v>911.6799999999999</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>12914.3</v>
+        <v>12811.66</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.05895357835628935</v>
+        <v>0.06643280717376382</v>
       </c>
     </row>
     <row r="4">
@@ -1711,13 +1711,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>2269.26</v>
+        <v>2680.76</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>11454.08</v>
+        <v>11042.58</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.165357704465531</v>
+        <v>0.1953431161801719</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-10 08:45:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1118,7 +1118,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0</v>
+        <v>565.27</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>0</v>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>0 de 10</t>
+          <t>1 de 10</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
@@ -1266,7 +1266,7 @@
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -1571,7 +1571,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0</v>
+        <v>565.27</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>0</v>
@@ -1588,7 +1588,7 @@
         <v>1076.87</v>
       </c>
       <c r="F12" s="4" t="n">
-        <v>140.37</v>
+        <v>705.64</v>
       </c>
       <c r="G12" s="4" t="n">
         <v>0</v>
@@ -1668,10 +1668,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>1490.67</v>
+        <v>2055.94</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-1490.67</v>
+        <v>-2055.94</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1711,13 +1711,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>2402.35</v>
+        <v>2967.62</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>11320.99</v>
+        <v>10755.72</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.1750557808813306</v>
+        <v>0.2162461907961181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-10 13:40:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1692,13 +1692,13 @@
         <v>13723.34</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>911.6799999999999</v>
+        <v>809.04</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>12811.66</v>
+        <v>12914.3</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.06643280717376382</v>
+        <v>0.05895357835628935</v>
       </c>
     </row>
     <row r="4">
@@ -1711,13 +1711,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>2967.62</v>
+        <v>2864.98</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>10755.72</v>
+        <v>10858.36</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.2162461907961181</v>
+        <v>0.2087669619786437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-10 17:05:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1668,10 +1668,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>2055.94</v>
+        <v>2626.18</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-2055.94</v>
+        <v>-2626.18</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1692,13 +1692,13 @@
         <v>13723.34</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>809.04</v>
+        <v>821.23</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>12914.3</v>
+        <v>12902.11</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.05895357835628935</v>
+        <v>0.05984184608120181</v>
       </c>
     </row>
     <row r="4">
@@ -1711,13 +1711,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>2864.98</v>
+        <v>3447.41</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>10858.36</v>
+        <v>10275.93</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.2087669619786437</v>
+        <v>0.2512077963527829</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-14 14:50:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -988,7 +988,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1070,7 +1070,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>43.86</v>
+        <v>0</v>
       </c>
       <c r="J10" s="2" t="n">
         <v>0</v>
@@ -1108,137 +1108,197 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>43.86</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>VEHINVER SA</t>
         </is>
       </c>
-      <c r="C11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="n">
+      <c r="C12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="n">
         <v>565.27</v>
       </c>
-      <c r="F11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="C12" s="3" t="inlineStr">
-        <is>
-          <t>0 de 10</t>
-        </is>
-      </c>
-      <c r="D12" s="3" t="inlineStr">
-        <is>
-          <t>0 de 10</t>
-        </is>
-      </c>
-      <c r="E12" s="3" t="inlineStr">
-        <is>
-          <t>1 de 10</t>
-        </is>
-      </c>
-      <c r="F12" s="3" t="inlineStr">
-        <is>
-          <t>0 de 10</t>
-        </is>
-      </c>
-      <c r="G12" s="3" t="inlineStr">
-        <is>
-          <t>0 de 10</t>
-        </is>
-      </c>
-      <c r="H12" s="3" t="inlineStr">
-        <is>
-          <t>0 de 10</t>
-        </is>
-      </c>
-      <c r="I12" s="3" t="inlineStr">
-        <is>
-          <t>1 de 10</t>
-        </is>
-      </c>
-      <c r="J12" s="3" t="inlineStr">
-        <is>
-          <t>0 de 10</t>
-        </is>
-      </c>
-      <c r="K12" s="3" t="inlineStr">
-        <is>
-          <t>0 de 10</t>
-        </is>
-      </c>
-      <c r="L12" s="3" t="inlineStr">
-        <is>
-          <t>0 de 10</t>
-        </is>
-      </c>
-      <c r="M12" s="3" t="inlineStr">
-        <is>
-          <t>1 de 10</t>
-        </is>
-      </c>
-      <c r="N12" s="3" t="inlineStr">
-        <is>
-          <t>0 de 10</t>
-        </is>
-      </c>
-      <c r="O12" s="3" t="inlineStr">
-        <is>
-          <t>1 de 10</t>
-        </is>
-      </c>
-      <c r="P12" s="3" t="inlineStr">
-        <is>
-          <t>0 de 10</t>
-        </is>
-      </c>
-      <c r="Q12" s="3" t="inlineStr">
-        <is>
-          <t>0 de 10</t>
-        </is>
-      </c>
-      <c r="R12" s="3" t="inlineStr">
-        <is>
-          <t>0 de 10</t>
+      <c r="F12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>0 de 11</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>0 de 11</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>1 de 11</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>0 de 11</t>
+        </is>
+      </c>
+      <c r="G13" s="3" t="inlineStr">
+        <is>
+          <t>0 de 11</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>0 de 11</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>1 de 11</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>0 de 11</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>0 de 11</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>0 de 11</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>1 de 11</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="inlineStr">
+        <is>
+          <t>0 de 11</t>
+        </is>
+      </c>
+      <c r="O13" s="3" t="inlineStr">
+        <is>
+          <t>1 de 11</t>
+        </is>
+      </c>
+      <c r="P13" s="3" t="inlineStr">
+        <is>
+          <t>0 de 11</t>
+        </is>
+      </c>
+      <c r="Q13" s="3" t="inlineStr">
+        <is>
+          <t>0 de 11</t>
+        </is>
+      </c>
+      <c r="R13" s="3" t="inlineStr">
+        <is>
+          <t>0 de 11</t>
         </is>
       </c>
     </row>
@@ -1253,7 +1313,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1504,7 +1564,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1514,7 +1574,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>159.03</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
@@ -1531,7 +1591,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1541,10 +1601,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0</v>
+        <v>159.03</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>43.86</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0</v>
@@ -1558,39 +1618,66 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>43.86</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>VEHINVER SA</t>
         </is>
       </c>
-      <c r="C11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2" t="n">
+      <c r="C12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2" t="n">
         <v>565.27</v>
       </c>
-      <c r="G11" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="C12" s="4" t="n">
+      <c r="G12" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" s="4" t="n">
         <v>144.53</v>
       </c>
-      <c r="D12" s="4" t="n">
+      <c r="D13" s="4" t="n">
         <v>189.85</v>
       </c>
-      <c r="E12" s="4" t="n">
+      <c r="E13" s="4" t="n">
         <v>1076.87</v>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="F13" s="4" t="n">
         <v>705.64</v>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="G13" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-07-14 16:55:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1755,10 +1755,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>2626.18</v>
+        <v>2879.62</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-2626.18</v>
+        <v>-2879.62</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1779,13 +1779,13 @@
         <v>13723.34</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>821.23</v>
+        <v>943.51</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>12902.11</v>
+        <v>12779.83</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.05984184608120181</v>
+        <v>0.06875221338245646</v>
       </c>
     </row>
     <row r="4">
@@ -1798,13 +1798,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>3447.41</v>
+        <v>3823.13</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>10275.93</v>
+        <v>9900.209999999999</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.2512077963527829</v>
+        <v>0.2785859710536939</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-15 10:55:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1755,10 +1755,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3456.76</v>
+        <v>3592.67</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-3456.76</v>
+        <v>-3592.67</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1798,13 +1798,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>4400.27</v>
+        <v>4536.18</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>9323.07</v>
+        <v>9187.16</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.320641330754758</v>
+        <v>0.3305448965047867</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-15 11:10:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1779,13 +1779,13 @@
         <v>13723.34</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>943.51</v>
+        <v>1166.29</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>12779.83</v>
+        <v>12557.05</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.06875221338245646</v>
+        <v>0.08498587078655778</v>
       </c>
     </row>
     <row r="4">
@@ -1798,13 +1798,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>4536.18</v>
+        <v>4758.96</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>9187.16</v>
+        <v>8964.379999999999</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.3305448965047867</v>
+        <v>0.3467785539088881</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-16 11:20:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1755,10 +1755,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3592.67</v>
+        <v>5182.43</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-3592.67</v>
+        <v>-5182.43</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1798,13 +1798,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>4924.47</v>
+        <v>6514.23</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>8798.870000000001</v>
+        <v>7209.110000000001</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.3588390289827404</v>
+        <v>0.4746825481260393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-17 15:55:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1705,7 +1705,7 @@
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="17" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1779,13 +1779,13 @@
         <v>13723.34</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>1331.8</v>
+        <v>5114.65</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>12391.54</v>
+        <v>8608.690000000001</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.09704634586041007</v>
+        <v>0.3726971713883063</v>
       </c>
     </row>
     <row r="4">
@@ -1798,13 +1798,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>6378.320000000001</v>
+        <v>10161.17</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>7345.02</v>
+        <v>3562.17</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.4647789823760106</v>
+        <v>0.7404298079039068</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-21 14:45:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -868,7 +868,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>FERNANDEZ MEZA JONATHAN ALEXIS</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -928,7 +928,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -988,7 +988,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1570,17 +1570,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>FERNANDEZ MEZA JONATHAN ALEXIS</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0</v>
+        <v>144.53</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0</v>
+        <v>11.52</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0</v>
@@ -1597,17 +1597,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>144.53</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>11.52</v>
+        <v>178.33</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0</v>
@@ -1624,14 +1624,14 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>178.33</v>
+        <v>0</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Actualización automática 2025-07-21 15:25:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1019,7 +1019,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>0</v>
+        <v>238.35</v>
       </c>
       <c r="M9" s="2" t="n">
         <v>0</v>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="L14" s="3" t="inlineStr">
         <is>
-          <t>1 de 12</t>
+          <t>2 de 12</t>
         </is>
       </c>
       <c r="M14" s="3" t="inlineStr">
@@ -1637,7 +1637,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0</v>
+        <v>238.35</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>0</v>
@@ -1762,7 +1762,7 @@
         <v>1076.87</v>
       </c>
       <c r="F14" s="4" t="n">
-        <v>1013.72</v>
+        <v>1252.07</v>
       </c>
       <c r="G14" s="4" t="n">
         <v>0</v>
@@ -1842,10 +1842,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>5161.07</v>
+        <v>5399.42</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-5161.07</v>
+        <v>-5399.42</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1885,13 +1885,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>10275.72</v>
+        <v>10514.07</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>3447.620000000001</v>
+        <v>3209.27</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.7487769012499872</v>
+        <v>0.766145122105843</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-22 15:30:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -868,7 +868,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -928,7 +928,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -988,7 +988,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1019,7 +1019,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="M9" s="2" t="n">
         <v>0</v>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>308.08</v>
+        <v>238.35</v>
       </c>
       <c r="M10" s="2" t="n">
         <v>0</v>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1139,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>0</v>
+        <v>308.08</v>
       </c>
       <c r="M11" s="2" t="n">
         <v>0</v>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1190,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>43.86</v>
+        <v>0</v>
       </c>
       <c r="J12" s="2" t="n">
         <v>0</v>
@@ -1228,137 +1228,197 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>43.86</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>VEHINVER SA</t>
         </is>
       </c>
-      <c r="C13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="n">
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="n">
         <v>565.27</v>
       </c>
-      <c r="F13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="C14" s="3" t="inlineStr">
-        <is>
-          <t>0 de 12</t>
-        </is>
-      </c>
-      <c r="D14" s="3" t="inlineStr">
-        <is>
-          <t>0 de 12</t>
-        </is>
-      </c>
-      <c r="E14" s="3" t="inlineStr">
-        <is>
-          <t>1 de 12</t>
-        </is>
-      </c>
-      <c r="F14" s="3" t="inlineStr">
-        <is>
-          <t>0 de 12</t>
-        </is>
-      </c>
-      <c r="G14" s="3" t="inlineStr">
-        <is>
-          <t>0 de 12</t>
-        </is>
-      </c>
-      <c r="H14" s="3" t="inlineStr">
-        <is>
-          <t>0 de 12</t>
-        </is>
-      </c>
-      <c r="I14" s="3" t="inlineStr">
-        <is>
-          <t>1 de 12</t>
-        </is>
-      </c>
-      <c r="J14" s="3" t="inlineStr">
-        <is>
-          <t>0 de 12</t>
-        </is>
-      </c>
-      <c r="K14" s="3" t="inlineStr">
-        <is>
-          <t>0 de 12</t>
-        </is>
-      </c>
-      <c r="L14" s="3" t="inlineStr">
-        <is>
-          <t>2 de 12</t>
-        </is>
-      </c>
-      <c r="M14" s="3" t="inlineStr">
-        <is>
-          <t>1 de 12</t>
-        </is>
-      </c>
-      <c r="N14" s="3" t="inlineStr">
-        <is>
-          <t>0 de 12</t>
-        </is>
-      </c>
-      <c r="O14" s="3" t="inlineStr">
-        <is>
-          <t>1 de 12</t>
-        </is>
-      </c>
-      <c r="P14" s="3" t="inlineStr">
-        <is>
-          <t>0 de 12</t>
-        </is>
-      </c>
-      <c r="Q14" s="3" t="inlineStr">
-        <is>
-          <t>0 de 12</t>
-        </is>
-      </c>
-      <c r="R14" s="3" t="inlineStr">
-        <is>
-          <t>0 de 12</t>
+      <c r="F14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>0 de 13</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>0 de 13</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>1 de 13</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>0 de 13</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>0 de 13</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>0 de 13</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>1 de 13</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>0 de 13</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>0 de 13</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>2 de 13</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>1 de 13</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>0 de 13</t>
+        </is>
+      </c>
+      <c r="O15" s="3" t="inlineStr">
+        <is>
+          <t>1 de 13</t>
+        </is>
+      </c>
+      <c r="P15" s="3" t="inlineStr">
+        <is>
+          <t>0 de 13</t>
+        </is>
+      </c>
+      <c r="Q15" s="3" t="inlineStr">
+        <is>
+          <t>0 de 13</t>
+        </is>
+      </c>
+      <c r="R15" s="3" t="inlineStr">
+        <is>
+          <t>0 de 13</t>
         </is>
       </c>
     </row>
@@ -1373,7 +1433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1543,7 +1603,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -1553,7 +1613,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>434.83</v>
+        <v>0</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
@@ -1570,17 +1630,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>144.53</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>11.52</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>10.44</v>
+        <v>434.83</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0</v>
@@ -1597,17 +1657,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0</v>
+        <v>144.53</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>178.33</v>
+        <v>11.52</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0</v>
@@ -1624,20 +1684,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>0</v>
+        <v>178.33</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>0</v>
@@ -1651,7 +1711,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1664,7 +1724,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>308.08</v>
+        <v>238.35</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0</v>
@@ -1678,7 +1738,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1688,10 +1748,10 @@
         <v>0</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>159.03</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0</v>
+        <v>308.08</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>0</v>
@@ -1705,7 +1765,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1715,10 +1775,10 @@
         <v>0</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0</v>
+        <v>159.03</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>43.86</v>
+        <v>0</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>0</v>
@@ -1732,39 +1792,66 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>43.86</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>VEHINVER SA</t>
         </is>
       </c>
-      <c r="C13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2" t="n">
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="n">
         <v>565.27</v>
       </c>
-      <c r="G13" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="C14" s="4" t="n">
+      <c r="G14" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" s="4" t="n">
         <v>144.53</v>
       </c>
-      <c r="D14" s="4" t="n">
+      <c r="D15" s="4" t="n">
         <v>189.85</v>
       </c>
-      <c r="E14" s="4" t="n">
+      <c r="E15" s="4" t="n">
         <v>1076.87</v>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="F15" s="4" t="n">
         <v>1252.07</v>
       </c>
-      <c r="G14" s="4" t="n">
+      <c r="G15" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-07-24 09:45:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1929,10 +1929,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>5399.42</v>
+        <v>5596.5</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-5399.42</v>
+        <v>-5596.5</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1972,13 +1972,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>18171.67</v>
+        <v>18368.75</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-4448.33</v>
+        <v>-4645.41</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>1.324143393663642</v>
+        <v>1.338504329121045</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-24 10:40:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1878,7 +1878,7 @@
     <col width="13" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="24" customWidth="1" min="5" max="5"/>
     <col width="23" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -1953,13 +1953,13 @@
         <v>13723.34</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>12772.25</v>
+        <v>13968.27</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>951.0900000000001</v>
+        <v>-244.9300000000003</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.930695442946105</v>
+        <v>1.017847695969057</v>
       </c>
     </row>
     <row r="4">
@@ -1972,13 +1972,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>18368.75</v>
+        <v>19564.77</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-4645.41</v>
+        <v>-5841.43</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>1.338504329121045</v>
+        <v>1.425656582143997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-25 09:55:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1929,10 +1929,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>5596.5</v>
+        <v>5874.91</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-5596.5</v>
+        <v>-5874.91</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -1972,13 +1972,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>19564.77</v>
+        <v>19843.18</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-5841.43</v>
+        <v>-6119.84</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>1.425656582143997</v>
+        <v>1.445943917442838</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-28 15:10:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -868,7 +868,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -928,7 +928,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -988,7 +988,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
         <v>0</v>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1139,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>308.08</v>
+        <v>238.35</v>
       </c>
       <c r="M11" s="2" t="n">
         <v>0</v>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1199,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>0</v>
+        <v>308.08</v>
       </c>
       <c r="M12" s="2" t="n">
         <v>0</v>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1250,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>43.86</v>
+        <v>0</v>
       </c>
       <c r="J13" s="2" t="n">
         <v>0</v>
@@ -1288,137 +1288,197 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>43.86</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>VEHINVER SA</t>
         </is>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="n">
+      <c r="C15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="n">
         <v>565.27</v>
       </c>
-      <c r="F14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R14" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="C15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="D15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="E15" s="3" t="inlineStr">
-        <is>
-          <t>1 de 13</t>
-        </is>
-      </c>
-      <c r="F15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="G15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="H15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="I15" s="3" t="inlineStr">
-        <is>
-          <t>1 de 13</t>
-        </is>
-      </c>
-      <c r="J15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="K15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="L15" s="3" t="inlineStr">
-        <is>
-          <t>2 de 13</t>
-        </is>
-      </c>
-      <c r="M15" s="3" t="inlineStr">
-        <is>
-          <t>1 de 13</t>
-        </is>
-      </c>
-      <c r="N15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="O15" s="3" t="inlineStr">
-        <is>
-          <t>1 de 13</t>
-        </is>
-      </c>
-      <c r="P15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="Q15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="R15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
+      <c r="F15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>1 de 14</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>1 de 14</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>2 de 14</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>1 de 14</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="O16" s="3" t="inlineStr">
+        <is>
+          <t>1 de 14</t>
+        </is>
+      </c>
+      <c r="P16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="Q16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="R16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
         </is>
       </c>
     </row>
@@ -1433,7 +1493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1603,7 +1663,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -1630,7 +1690,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -1640,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>434.83</v>
+        <v>0</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0</v>
@@ -1657,17 +1717,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>144.53</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>11.52</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>10.44</v>
+        <v>434.83</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0</v>
@@ -1684,17 +1744,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0</v>
+        <v>144.53</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>178.33</v>
+        <v>11.52</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
@@ -1711,20 +1771,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0</v>
+        <v>178.33</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0</v>
@@ -1738,7 +1798,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1751,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>308.08</v>
+        <v>238.35</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>0</v>
@@ -1765,7 +1825,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1775,10 +1835,10 @@
         <v>0</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>159.03</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0</v>
+        <v>308.08</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>0</v>
@@ -1792,7 +1852,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1802,10 +1862,10 @@
         <v>0</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>0</v>
+        <v>159.03</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>43.86</v>
+        <v>0</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>0</v>
@@ -1819,39 +1879,66 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>43.86</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>VEHINVER SA</t>
         </is>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2" t="n">
+      <c r="C15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="n">
         <v>565.27</v>
       </c>
-      <c r="G14" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="C15" s="4" t="n">
+      <c r="G15" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" s="4" t="n">
         <v>144.53</v>
       </c>
-      <c r="D15" s="4" t="n">
+      <c r="D16" s="4" t="n">
         <v>189.85</v>
       </c>
-      <c r="E15" s="4" t="n">
+      <c r="E16" s="4" t="n">
         <v>1076.87</v>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="F16" s="4" t="n">
         <v>1252.07</v>
       </c>
-      <c r="G15" s="4" t="n">
+      <c r="G16" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-07-28 15:20:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -988,7 +988,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1108,7 +1108,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1139,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="M11" s="2" t="n">
         <v>0</v>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1199,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>308.08</v>
+        <v>238.35</v>
       </c>
       <c r="M12" s="2" t="n">
         <v>0</v>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1259,7 +1259,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>0</v>
+        <v>308.08</v>
       </c>
       <c r="M13" s="2" t="n">
         <v>0</v>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1310,7 +1310,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>43.86</v>
+        <v>0</v>
       </c>
       <c r="J14" s="2" t="n">
         <v>0</v>
@@ -1348,137 +1348,197 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>43.86</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>VEHINVER SA</t>
         </is>
       </c>
-      <c r="C15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="n">
+      <c r="C16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="n">
         <v>565.27</v>
       </c>
-      <c r="F15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R15" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="C16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="D16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="E16" s="3" t="inlineStr">
-        <is>
-          <t>1 de 14</t>
-        </is>
-      </c>
-      <c r="F16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="G16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="H16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="I16" s="3" t="inlineStr">
-        <is>
-          <t>1 de 14</t>
-        </is>
-      </c>
-      <c r="J16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="K16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="L16" s="3" t="inlineStr">
-        <is>
-          <t>2 de 14</t>
-        </is>
-      </c>
-      <c r="M16" s="3" t="inlineStr">
-        <is>
-          <t>1 de 14</t>
-        </is>
-      </c>
-      <c r="N16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="O16" s="3" t="inlineStr">
-        <is>
-          <t>1 de 14</t>
-        </is>
-      </c>
-      <c r="P16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="Q16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="R16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
+      <c r="F16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>1 de 15</t>
+        </is>
+      </c>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>1 de 15</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>2 de 15</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>1 de 15</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="O17" s="3" t="inlineStr">
+        <is>
+          <t>1 de 15</t>
+        </is>
+      </c>
+      <c r="P17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="Q17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="R17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
         </is>
       </c>
     </row>
@@ -1493,7 +1553,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1744,17 +1804,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>144.53</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>11.52</v>
+        <v>0</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
@@ -1771,17 +1831,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0</v>
+        <v>144.53</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>178.33</v>
+        <v>11.52</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0</v>
@@ -1798,20 +1858,20 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0</v>
+        <v>178.33</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>0</v>
@@ -1825,7 +1885,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1838,7 +1898,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>308.08</v>
+        <v>238.35</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>0</v>
@@ -1852,7 +1912,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1862,10 +1922,10 @@
         <v>0</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>159.03</v>
+        <v>0</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0</v>
+        <v>308.08</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>0</v>
@@ -1879,7 +1939,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1889,10 +1949,10 @@
         <v>0</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>0</v>
+        <v>159.03</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>43.86</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>0</v>
@@ -1906,39 +1966,66 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>43.86</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>VEHINVER SA</t>
         </is>
       </c>
-      <c r="C15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2" t="n">
+      <c r="C16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2" t="n">
         <v>565.27</v>
       </c>
-      <c r="G15" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="C16" s="4" t="n">
+      <c r="G16" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" s="4" t="n">
         <v>144.53</v>
       </c>
-      <c r="D16" s="4" t="n">
+      <c r="D17" s="4" t="n">
         <v>189.85</v>
       </c>
-      <c r="E16" s="4" t="n">
+      <c r="E17" s="4" t="n">
         <v>1076.87</v>
       </c>
-      <c r="F16" s="4" t="n">
+      <c r="F17" s="4" t="n">
         <v>1252.07</v>
       </c>
-      <c r="G16" s="4" t="n">
+      <c r="G17" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-07-28 16:00:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2103,10 +2103,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>5874.91</v>
+        <v>6005.41</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-5874.91</v>
+        <v>-6005.41</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -2127,13 +2127,13 @@
         <v>13723.34</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>13968.27</v>
+        <v>14195.66</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>-244.9300000000003</v>
+        <v>-472.3199999999997</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>1.017847695969057</v>
+        <v>1.034417277426632</v>
       </c>
     </row>
     <row r="4">
@@ -2146,13 +2146,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>19843.18</v>
+        <v>20201.07</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-6119.84</v>
+        <v>-6477.73</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>1.445943917442838</v>
+        <v>1.472022845750379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-29 13:30:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>0</v>
+        <v>24.39</v>
       </c>
       <c r="N7" s="2" t="n">
         <v>0</v>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="M19" s="3" t="inlineStr">
         <is>
-          <t>1 de 17</t>
+          <t>2 de 17</t>
         </is>
       </c>
       <c r="N19" s="3" t="inlineStr">
@@ -1883,7 +1883,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0</v>
+        <v>24.39</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>0</v>
@@ -2197,7 +2197,7 @@
         <v>1076.87</v>
       </c>
       <c r="F19" s="4" t="n">
-        <v>1619.87</v>
+        <v>1644.26</v>
       </c>
       <c r="G19" s="4" t="n">
         <v>0</v>
@@ -2301,13 +2301,13 @@
         <v>13723.34</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>14195.66</v>
+        <v>14220.05</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>-472.3199999999997</v>
+        <v>-496.7099999999991</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>1.034417277426632</v>
+        <v>1.036194541562039</v>
       </c>
     </row>
     <row r="4">
@@ -2320,13 +2320,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>20568.87</v>
+        <v>20593.26</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-6845.53</v>
+        <v>-6869.919999999999</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>1.49882390147005</v>
+        <v>1.500601165605457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-29 14:25:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1415,7 +1415,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>0</v>
+        <v>413.5</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>0</v>
@@ -1588,7 +1588,7 @@
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>0 de 17</t>
+          <t>1 de 17</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr">
@@ -2126,7 +2126,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>0</v>
+        <v>413.5</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>0</v>
@@ -2197,7 +2197,7 @@
         <v>1076.87</v>
       </c>
       <c r="F19" s="4" t="n">
-        <v>1644.26</v>
+        <v>2057.76</v>
       </c>
       <c r="G19" s="4" t="n">
         <v>0</v>
@@ -2277,10 +2277,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>6373.21</v>
+        <v>6786.71</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-6373.21</v>
+        <v>-6786.71</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -2320,13 +2320,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>20593.26</v>
+        <v>21006.76</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-6869.919999999999</v>
+        <v>-7283.419999999999</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>1.500601165605457</v>
+        <v>1.530732314436573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-29 14:45:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1673,7 +1673,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1682,7 +1682,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="36" customWidth="1" min="2" max="2"/>
+    <col width="56" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
@@ -1870,7 +1870,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
+          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -1883,7 +1883,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>24.39</v>
+        <v>0</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>0</v>
@@ -1897,7 +1897,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -1910,7 +1910,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0</v>
+        <v>24.39</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>0</v>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1934,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>434.83</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
@@ -1951,7 +1951,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1961,10 +1961,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0</v>
+        <v>434.83</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0</v>
@@ -1978,20 +1978,20 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>144.53</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>11.52</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>0</v>
@@ -2005,17 +2005,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0</v>
+        <v>144.53</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>178.33</v>
+        <v>11.52</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>0</v>
@@ -2032,20 +2032,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>0</v>
+        <v>178.33</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>0</v>
@@ -2059,7 +2059,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -2072,7 +2072,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>308.08</v>
+        <v>238.35</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>0</v>
@@ -2086,7 +2086,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -2096,10 +2096,10 @@
         <v>0</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>159.03</v>
+        <v>0</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>0</v>
+        <v>308.08</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>0</v>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -2123,10 +2123,10 @@
         <v>0</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>0</v>
+        <v>159.03</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>413.5</v>
+        <v>0</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>0</v>
@@ -2140,7 +2140,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -2153,7 +2153,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>43.86</v>
+        <v>413.5</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>0</v>
@@ -2167,39 +2167,66 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>43.86</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>VEHINVER SA</t>
         </is>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2" t="n">
+      <c r="C19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="n">
         <v>565.27</v>
       </c>
-      <c r="G18" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="C19" s="4" t="n">
+      <c r="G19" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" s="4" t="n">
         <v>144.53</v>
       </c>
-      <c r="D19" s="4" t="n">
+      <c r="D20" s="4" t="n">
         <v>189.85</v>
       </c>
-      <c r="E19" s="4" t="n">
+      <c r="E20" s="4" t="n">
         <v>1076.87</v>
       </c>
-      <c r="F19" s="4" t="n">
+      <c r="F20" s="4" t="n">
         <v>2057.76</v>
       </c>
-      <c r="G19" s="4" t="n">
+      <c r="G20" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-07-29 14:50:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,7 +449,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="36" customWidth="1" min="2" max="2"/>
+    <col width="56" customWidth="1" min="2" max="2"/>
     <col width="25" customWidth="1" min="3" max="3"/>
     <col width="24" customWidth="1" min="4" max="4"/>
     <col width="26" customWidth="1" min="5" max="5"/>
@@ -868,7 +868,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
+          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>24.39</v>
+        <v>0</v>
       </c>
       <c r="N7" s="2" t="n">
         <v>0</v>
@@ -928,7 +928,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -962,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>0</v>
+        <v>24.39</v>
       </c>
       <c r="N8" s="2" t="n">
         <v>0</v>
@@ -988,7 +988,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
         <v>0</v>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1139,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="M11" s="2" t="n">
         <v>0</v>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1259,7 +1259,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
         <v>0</v>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>308.08</v>
+        <v>238.35</v>
       </c>
       <c r="M14" s="2" t="n">
         <v>0</v>
@@ -1348,7 +1348,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1379,7 +1379,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>0</v>
+        <v>308.08</v>
       </c>
       <c r="M15" s="2" t="n">
         <v>0</v>
@@ -1408,14 +1408,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>413.5</v>
+        <v>0</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>0</v>
@@ -1468,14 +1468,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0</v>
+        <v>413.5</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>0</v>
@@ -1490,7 +1490,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>43.86</v>
+        <v>0</v>
       </c>
       <c r="J17" s="2" t="n">
         <v>0</v>
@@ -1528,137 +1528,197 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>43.86</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>VEHINVER SA</t>
         </is>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2" t="n">
+      <c r="C19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="n">
         <v>565.27</v>
       </c>
-      <c r="F18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R18" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="C19" s="3" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="D19" s="3" t="inlineStr">
-        <is>
-          <t>1 de 17</t>
-        </is>
-      </c>
-      <c r="E19" s="3" t="inlineStr">
-        <is>
-          <t>1 de 17</t>
-        </is>
-      </c>
-      <c r="F19" s="3" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="G19" s="3" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="H19" s="3" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="I19" s="3" t="inlineStr">
-        <is>
-          <t>1 de 17</t>
-        </is>
-      </c>
-      <c r="J19" s="3" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="K19" s="3" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="L19" s="3" t="inlineStr">
-        <is>
-          <t>3 de 17</t>
-        </is>
-      </c>
-      <c r="M19" s="3" t="inlineStr">
-        <is>
-          <t>2 de 17</t>
-        </is>
-      </c>
-      <c r="N19" s="3" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="O19" s="3" t="inlineStr">
-        <is>
-          <t>1 de 17</t>
-        </is>
-      </c>
-      <c r="P19" s="3" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="Q19" s="3" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
-        </is>
-      </c>
-      <c r="R19" s="3" t="inlineStr">
-        <is>
-          <t>0 de 17</t>
+      <c r="F19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>0 de 18</t>
+        </is>
+      </c>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>1 de 18</t>
+        </is>
+      </c>
+      <c r="E20" s="3" t="inlineStr">
+        <is>
+          <t>1 de 18</t>
+        </is>
+      </c>
+      <c r="F20" s="3" t="inlineStr">
+        <is>
+          <t>0 de 18</t>
+        </is>
+      </c>
+      <c r="G20" s="3" t="inlineStr">
+        <is>
+          <t>0 de 18</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>0 de 18</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>1 de 18</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>0 de 18</t>
+        </is>
+      </c>
+      <c r="K20" s="3" t="inlineStr">
+        <is>
+          <t>0 de 18</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>3 de 18</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="inlineStr">
+        <is>
+          <t>2 de 18</t>
+        </is>
+      </c>
+      <c r="N20" s="3" t="inlineStr">
+        <is>
+          <t>0 de 18</t>
+        </is>
+      </c>
+      <c r="O20" s="3" t="inlineStr">
+        <is>
+          <t>1 de 18</t>
+        </is>
+      </c>
+      <c r="P20" s="3" t="inlineStr">
+        <is>
+          <t>0 de 18</t>
+        </is>
+      </c>
+      <c r="Q20" s="3" t="inlineStr">
+        <is>
+          <t>0 de 18</t>
+        </is>
+      </c>
+      <c r="R20" s="3" t="inlineStr">
+        <is>
+          <t>0 de 18</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-07-31 16:05:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2364,10 +2364,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>6311.23</v>
+        <v>6396.51</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-6311.23</v>
+        <v>-6396.51</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -2407,13 +2407,13 @@
         <v>13723.34</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>20639.36</v>
+        <v>20724.64</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-6916.019999999999</v>
+        <v>-7001.299999999999</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>1.503960406140196</v>
+        <v>1.510174636786671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-05 09:05:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="M6" s="2" t="n">
         <v>0</v>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="L20" s="3" t="inlineStr">
         <is>
-          <t>0 de 18</t>
+          <t>1 de 18</t>
         </is>
       </c>
       <c r="M20" s="3" t="inlineStr">
@@ -1916,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>0</v>
@@ -2284,7 +2284,7 @@
         <v>2057.76</v>
       </c>
       <c r="F20" s="4" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="G20" s="4" t="n">
         <v>0</v>
@@ -2364,10 +2364,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>68536.67999999999</v>
+        <v>68904.48</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-68536.67999999999</v>
+        <v>-68904.48</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -2407,13 +2407,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>68536.67999999999</v>
+        <v>68904.48</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-53065.12069999999</v>
+        <v>-53432.9207</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>4.429849549812344</v>
+        <v>4.453622202126711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-05 09:20:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2364,10 +2364,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>68904.48</v>
+        <v>69594.61</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-68904.48</v>
+        <v>-69594.61</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -2407,13 +2407,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>68904.48</v>
+        <v>69594.61</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-53432.9207</v>
+        <v>-54123.0507</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>4.453622202126711</v>
+        <v>4.498228565752903</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-05 12:50:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -688,7 +688,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AREVALO PEÑA JORGE LUIS</t>
+          <t>ARCE CANDO DENISSE YAJAIRA</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -748,7 +748,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
+          <t>AREVALO PEÑA JORGE LUIS</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -808,7 +808,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
+          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="M6" s="2" t="n">
         <v>0</v>
@@ -868,7 +868,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
+          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -899,7 +899,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="M7" s="2" t="n">
         <v>0</v>
@@ -928,7 +928,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
+          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -988,7 +988,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1108,7 +1108,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -1468,7 +1468,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1588,137 +1588,197 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>VEHINVER SA</t>
         </is>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R19" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="C20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="D20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="E20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="F20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="G20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="H20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="I20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="J20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="K20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="L20" s="3" t="inlineStr">
-        <is>
-          <t>1 de 18</t>
-        </is>
-      </c>
-      <c r="M20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="N20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="O20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="P20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="Q20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="R20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
+      <c r="C20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="E21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="F21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="G21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>1 de 19</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="O21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="P21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="Q21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="R21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
         </is>
       </c>
     </row>
@@ -1733,7 +1793,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1849,7 +1909,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AREVALO PEÑA JORGE LUIS</t>
+          <t>ARCE CANDO DENISSE YAJAIRA</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -1876,14 +1936,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
+          <t>AREVALO PEÑA JORGE LUIS</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>472.57</v>
+        <v>0</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>0</v>
@@ -1903,20 +1963,20 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
+          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0</v>
+        <v>472.57</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>0</v>
@@ -1930,7 +1990,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
+          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -1943,7 +2003,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>0</v>
@@ -1957,7 +2017,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
+          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -1967,7 +2027,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>24.39</v>
+        <v>0</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0</v>
@@ -1984,7 +2044,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1994,7 +2054,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>0</v>
+        <v>24.39</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
@@ -2011,14 +2071,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>434.83</v>
+        <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>0</v>
@@ -2038,17 +2098,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0</v>
+        <v>434.83</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>0</v>
@@ -2065,17 +2125,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>11.52</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>0</v>
@@ -2092,14 +2152,14 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>178.33</v>
+        <v>11.52</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>0</v>
@@ -2119,17 +2179,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0</v>
+        <v>178.33</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>0</v>
@@ -2146,7 +2206,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -2156,7 +2216,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>308.08</v>
+        <v>238.35</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>0</v>
@@ -2173,17 +2233,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>159.03</v>
+        <v>0</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>0</v>
+        <v>308.08</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>0</v>
@@ -2200,17 +2260,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0</v>
+        <v>159.03</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>413.5</v>
+        <v>0</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>0</v>
@@ -2227,7 +2287,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -2237,7 +2297,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>43.86</v>
+        <v>413.5</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>0</v>
@@ -2254,39 +2314,66 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>43.86</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>VEHINVER SA</t>
         </is>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="n">
+      <c r="C20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="n">
         <v>565.27</v>
       </c>
-      <c r="F19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="C20" s="4" t="n">
+      <c r="F20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" s="4" t="n">
         <v>189.85</v>
       </c>
-      <c r="D20" s="4" t="n">
+      <c r="D21" s="4" t="n">
         <v>1076.87</v>
       </c>
-      <c r="E20" s="4" t="n">
+      <c r="E21" s="4" t="n">
         <v>2057.76</v>
       </c>
-      <c r="F20" s="4" t="n">
+      <c r="F21" s="4" t="n">
         <v>367.8</v>
       </c>
-      <c r="G20" s="4" t="n">
+      <c r="G21" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-08-05 17:25:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2451,10 +2451,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>69594.61</v>
+        <v>69974.77</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-69594.61</v>
+        <v>-69974.77</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -2494,13 +2494,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>69594.61</v>
+        <v>69974.77</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-54123.0507</v>
+        <v>-54503.2107</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>4.498228565752903</v>
+        <v>4.522800103283707</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-06 14:55:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -722,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>0</v>
+        <v>95.56</v>
       </c>
       <c r="N4" s="2" t="n">
         <v>0</v>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="M21" s="3" t="inlineStr">
         <is>
-          <t>0 de 19</t>
+          <t>1 de 19</t>
         </is>
       </c>
       <c r="N21" s="3" t="inlineStr">
@@ -1922,7 +1922,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0</v>
+        <v>95.56</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>0</v>
@@ -2371,7 +2371,7 @@
         <v>2057.76</v>
       </c>
       <c r="F21" s="4" t="n">
-        <v>367.8</v>
+        <v>463.36</v>
       </c>
       <c r="G21" s="4" t="n">
         <v>0</v>
@@ -2401,7 +2401,7 @@
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="17" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2475,13 +2475,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>95.56</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>15471.5593</v>
+        <v>15375.9993</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0</v>
+        <v>0.006176494440350301</v>
       </c>
     </row>
     <row r="4">
@@ -2494,13 +2494,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>69974.77</v>
+        <v>70070.33</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-54503.2107</v>
+        <v>-54598.77070000001</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>4.522800103283707</v>
+        <v>4.528976597724057</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-07 09:05:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2451,10 +2451,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>69974.77</v>
+        <v>70069.27</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-69974.77</v>
+        <v>-70069.27</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -2494,13 +2494,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>70070.33</v>
+        <v>70164.83</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-54598.77070000001</v>
+        <v>-54693.27070000001</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>4.528976597724057</v>
+        <v>4.535084579354583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-08 14:20:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2451,10 +2451,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>70357.72</v>
+        <v>70642.84</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-70357.72</v>
+        <v>-70642.84</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -2494,13 +2494,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>70453.28</v>
+        <v>70738.39999999999</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-54981.72070000001</v>
+        <v>-55266.8407</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>4.553728466141095</v>
+        <v>4.572157119289197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-08 15:00:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2475,13 +2475,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>95.56</v>
+        <v>102.38</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>15375.9993</v>
+        <v>15369.1793</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.006176494440350301</v>
+        <v>0.006617303273368185</v>
       </c>
     </row>
     <row r="4">
@@ -2494,13 +2494,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>70738.39999999999</v>
+        <v>70745.22</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-55266.8407</v>
+        <v>-55273.66069999999</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>4.572157119289197</v>
+        <v>4.572597928122216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-15 15:45:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2562,13 +2562,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>102.38</v>
+        <v>128.12</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>15369.1793</v>
+        <v>15343.4393</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.006617303273368185</v>
+        <v>0.008281001127016331</v>
       </c>
     </row>
     <row r="4">
@@ -2581,13 +2581,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>71088.60000000001</v>
+        <v>71114.34</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-55617.0407</v>
+        <v>-55642.7807</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>4.594792200421582</v>
+        <v>4.59645589827523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-15 16:30:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2488,7 +2488,7 @@
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="17" customWidth="1" min="5" max="5"/>
-    <col width="26" customWidth="1" min="6" max="6"/>
+    <col width="23" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2562,13 +2562,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>128.12</v>
+        <v>2848.66</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>15343.4393</v>
+        <v>12622.8993</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.008281001127016331</v>
+        <v>0.184122359276353</v>
       </c>
     </row>
     <row r="4">
@@ -2581,13 +2581,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>71114.34</v>
+        <v>73834.88</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-55642.7807</v>
+        <v>-58363.3207</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>4.59645589827523</v>
+        <v>4.772297256424568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-18 15:25:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2488,7 +2488,7 @@
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="17" customWidth="1" min="5" max="5"/>
-    <col width="23" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2562,13 +2562,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>2848.66</v>
+        <v>3237.89</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>12622.8993</v>
+        <v>12233.6693</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.184122359276353</v>
+        <v>0.2092801337742344</v>
       </c>
     </row>
     <row r="4">
@@ -2581,13 +2581,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>73834.88</v>
+        <v>74224.11</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-58363.3207</v>
+        <v>-58752.5507</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>4.772297256424568</v>
+        <v>4.797455030922449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-20 10:35:10
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1055,7 +1055,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0</v>
+        <v>354.43</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>0</v>
@@ -1768,7 +1768,7 @@
       </c>
       <c r="D22" s="3" t="inlineStr">
         <is>
-          <t>0 de 20</t>
+          <t>1 de 20</t>
         </is>
       </c>
       <c r="E22" s="3" t="inlineStr">
@@ -2144,7 +2144,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0</v>
+        <v>354.43</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0</v>
@@ -2458,7 +2458,7 @@
         <v>2057.76</v>
       </c>
       <c r="F22" s="4" t="n">
-        <v>701.71</v>
+        <v>1056.14</v>
       </c>
       <c r="G22" s="4" t="n">
         <v>0</v>
@@ -2538,10 +2538,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>71369.11</v>
+        <v>71723.53999999999</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-71369.11</v>
+        <v>-71723.53999999999</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -2581,13 +2581,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>74607</v>
+        <v>74961.42999999999</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-59135.4407</v>
+        <v>-59489.87069999999</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>4.822203021255912</v>
+        <v>4.845111507280329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-22 15:40:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2538,10 +2538,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>71726.64999999999</v>
+        <v>71864.49000000001</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-71726.64999999999</v>
+        <v>-71864.49000000001</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -2581,13 +2581,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>74964.53999999999</v>
+        <v>75102.38</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-59492.98069999999</v>
+        <v>-59630.8207</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>4.845312521278963</v>
+        <v>4.85422177194512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-25 14:55:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2562,13 +2562,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>3237.89</v>
+        <v>3293.63</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>12233.6693</v>
+        <v>12177.9293</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.2092801337742344</v>
+        <v>0.2128828734153512</v>
       </c>
     </row>
     <row r="4">
@@ -2581,13 +2581,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>75102.38</v>
+        <v>75158.12000000001</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-59630.8207</v>
+        <v>-59686.5607</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>4.85422177194512</v>
+        <v>4.857824511586237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-27 12:15:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2538,10 +2538,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>72466.41</v>
+        <v>73996.77</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-72466.41</v>
+        <v>-73996.77</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -2562,13 +2562,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>3287.87</v>
+        <v>3361.24</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>12183.6893</v>
+        <v>12110.3193</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.2125105773921572</v>
+        <v>0.2172528272570432</v>
       </c>
     </row>
     <row r="4">
@@ -2581,13 +2581,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>75754.28</v>
+        <v>77358.01000000001</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-60282.72070000001</v>
+        <v>-61886.4507</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>4.896357149986814</v>
+        <v>5.000013799514054</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-29 10:50:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1559,7 +1559,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="M18" s="2" t="n">
         <v>0</v>
@@ -1868,7 +1868,7 @@
       </c>
       <c r="L23" s="3" t="inlineStr">
         <is>
-          <t>2 de 21</t>
+          <t>3 de 21</t>
         </is>
       </c>
       <c r="M23" s="3" t="inlineStr">
@@ -2420,7 +2420,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>0</v>
@@ -2545,7 +2545,7 @@
         <v>2057.76</v>
       </c>
       <c r="F23" s="4" t="n">
-        <v>1056.14</v>
+        <v>1423.94</v>
       </c>
       <c r="G23" s="4" t="n">
         <v>0</v>
@@ -2625,10 +2625,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>73996.77</v>
+        <v>74364.57000000001</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-73996.77</v>
+        <v>-74364.57000000001</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -2668,13 +2668,13 @@
         <v>15471.5593</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>77358.01000000001</v>
+        <v>77725.81000000001</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-61886.4507</v>
+        <v>-62254.2507</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>5.000013799514054</v>
+        <v>5.023786451828421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-29 14:15:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
+          <t>ARMIJO AGUILAR ROBERT LENIN</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -868,7 +868,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
+          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -899,7 +899,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="M7" s="2" t="n">
         <v>0</v>
@@ -928,7 +928,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
+          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -959,7 +959,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="M8" s="2" t="n">
         <v>0</v>
@@ -988,7 +988,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
+          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1048,14 +1048,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>354.43</v>
+        <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>0</v>
@@ -1108,14 +1108,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0</v>
+        <v>354.43</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>0</v>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -1468,7 +1468,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1499,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="M17" s="2" t="n">
         <v>0</v>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>MORALES CAIZA SERGIO IVAN</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1559,7 +1559,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="2" t="n">
-        <v>367.8</v>
+        <v>238.35</v>
       </c>
       <c r="M18" s="2" t="n">
         <v>0</v>
@@ -1588,7 +1588,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -1619,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="M19" s="2" t="n">
         <v>0</v>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -1768,137 +1768,197 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>VEHINVER SA</t>
         </is>
       </c>
-      <c r="C22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R22" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="C23" s="3" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="D23" s="3" t="inlineStr">
-        <is>
-          <t>1 de 21</t>
-        </is>
-      </c>
-      <c r="E23" s="3" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="F23" s="3" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="G23" s="3" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="H23" s="3" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="I23" s="3" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="J23" s="3" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="K23" s="3" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="L23" s="3" t="inlineStr">
-        <is>
-          <t>3 de 21</t>
-        </is>
-      </c>
-      <c r="M23" s="3" t="inlineStr">
-        <is>
-          <t>1 de 21</t>
-        </is>
-      </c>
-      <c r="N23" s="3" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="O23" s="3" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="P23" s="3" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="Q23" s="3" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="R23" s="3" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
+      <c r="C23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>1 de 22</t>
+        </is>
+      </c>
+      <c r="E24" s="3" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="F24" s="3" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="G24" s="3" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="J24" s="3" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="K24" s="3" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="L24" s="3" t="inlineStr">
+        <is>
+          <t>3 de 22</t>
+        </is>
+      </c>
+      <c r="M24" s="3" t="inlineStr">
+        <is>
+          <t>1 de 22</t>
+        </is>
+      </c>
+      <c r="N24" s="3" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="O24" s="3" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="P24" s="3" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="Q24" s="3" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="R24" s="3" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1973,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2083,14 +2143,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
+          <t>ARMIJO AGUILAR ROBERT LENIN</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>472.57</v>
+        <v>0</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>0</v>
@@ -2110,20 +2170,20 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
+          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0</v>
+        <v>472.57</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>0</v>
@@ -2137,7 +2197,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
+          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -2150,7 +2210,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>0</v>
@@ -2164,7 +2224,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
+          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -2174,7 +2234,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>24.39</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
@@ -2191,7 +2251,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -2201,10 +2261,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0</v>
+        <v>24.39</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>354.43</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0</v>
@@ -2218,20 +2278,20 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>434.83</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0</v>
+        <v>354.43</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>0</v>
@@ -2245,17 +2305,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0</v>
+        <v>434.83</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>0</v>
@@ -2272,17 +2332,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>11.52</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>0</v>
@@ -2299,14 +2359,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>178.33</v>
+        <v>11.52</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>0</v>
@@ -2326,17 +2386,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>0</v>
+        <v>178.33</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>0</v>
@@ -2353,7 +2413,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -2363,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>308.08</v>
+        <v>238.35</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>0</v>
@@ -2380,7 +2440,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -2390,10 +2450,10 @@
         <v>0</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>0</v>
+        <v>308.08</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>0</v>
@@ -2407,7 +2467,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>MORALES CAIZA SERGIO IVAN</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -2420,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>367.8</v>
+        <v>238.35</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>0</v>
@@ -2434,20 +2494,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>159.03</v>
+        <v>0</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>0</v>
@@ -2461,17 +2521,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>0</v>
+        <v>159.03</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>413.5</v>
+        <v>0</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0</v>
@@ -2488,7 +2548,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -2498,7 +2558,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>43.86</v>
+        <v>413.5</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>0</v>
@@ -2515,39 +2575,66 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>43.86</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>VEHINVER SA</t>
         </is>
       </c>
-      <c r="C22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2" t="n">
+      <c r="C23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="n">
         <v>565.27</v>
       </c>
-      <c r="F22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="C23" s="4" t="n">
+      <c r="F23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" s="4" t="n">
         <v>189.85</v>
       </c>
-      <c r="D23" s="4" t="n">
+      <c r="D24" s="4" t="n">
         <v>1076.87</v>
       </c>
-      <c r="E23" s="4" t="n">
+      <c r="E24" s="4" t="n">
         <v>2057.76</v>
       </c>
-      <c r="F23" s="4" t="n">
+      <c r="F24" s="4" t="n">
         <v>1423.94</v>
       </c>
-      <c r="G23" s="4" t="n">
+      <c r="G24" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-09-02 10:55:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -842,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>0</v>
+        <v>2697.41</v>
       </c>
       <c r="N6" s="2" t="n">
         <v>0</v>
@@ -1933,7 +1933,7 @@
       </c>
       <c r="M24" s="3" t="inlineStr">
         <is>
-          <t>0 de 22</t>
+          <t>1 de 22</t>
         </is>
       </c>
       <c r="N24" s="3" t="inlineStr">
@@ -2156,7 +2156,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0</v>
+        <v>2697.41</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>0</v>
@@ -2632,7 +2632,7 @@
         <v>1423.94</v>
       </c>
       <c r="F24" s="4" t="n">
-        <v>0</v>
+        <v>2697.41</v>
       </c>
       <c r="G24" s="4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Actualización automática 2025-09-08 10:00:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2099,7 +2099,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="2" t="n">
-        <v>0</v>
+        <v>346.56</v>
       </c>
       <c r="M27" s="2" t="n">
         <v>0</v>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="L28" s="3" t="inlineStr">
         <is>
-          <t>1 de 26</t>
+          <t>2 de 26</t>
         </is>
       </c>
       <c r="M28" s="3" t="inlineStr">
@@ -2963,7 +2963,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>0</v>
+        <v>346.56</v>
       </c>
       <c r="G27" s="2" t="n">
         <v>0</v>
@@ -2980,7 +2980,7 @@
         <v>1423.94</v>
       </c>
       <c r="F28" s="4" t="n">
-        <v>8323.9</v>
+        <v>8670.459999999999</v>
       </c>
       <c r="G28" s="4" t="n">
         <v>0</v>
@@ -3060,10 +3060,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>4083.42</v>
+        <v>4429.98</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-4083.42</v>
+        <v>-4429.98</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -3103,13 +3103,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>13777.5</v>
+        <v>14124.06</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>6222.5</v>
+        <v>5875.940000000001</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.688875</v>
+        <v>0.706203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-08 13:10:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -988,7 +988,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
+          <t>BRAVO MANZABA MARIA CECILIA</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
+          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1108,7 +1108,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
+          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>GARCIA BRAVO JOSE LUIS</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>GARCIA BRAVO JOSE LUIS</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -1468,7 +1468,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>MORALES CAIZA SERGIO IVAN</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -1982,7 +1982,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="2" t="n">
-        <v>3722.63</v>
+        <v>0</v>
       </c>
       <c r="N25" s="2" t="n">
         <v>0</v>
@@ -2008,7 +2008,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -2018,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>94.20999999999999</v>
+        <v>0</v>
       </c>
       <c r="F26" s="2" t="n">
         <v>0</v>
@@ -2042,7 +2042,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="2" t="n">
-        <v>428.61</v>
+        <v>3722.63</v>
       </c>
       <c r="N26" s="2" t="n">
         <v>0</v>
@@ -2068,137 +2068,197 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>VEHINVER SA</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>94.20999999999999</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2" t="n">
+        <v>428.61</v>
+      </c>
+      <c r="N27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L27" s="2" t="n">
+      <c r="C28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2" t="n">
         <v>346.56</v>
       </c>
-      <c r="M27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R27" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="C28" s="3" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="D28" s="3" t="inlineStr">
-        <is>
-          <t>1 de 26</t>
-        </is>
-      </c>
-      <c r="E28" s="3" t="inlineStr">
-        <is>
-          <t>1 de 26</t>
-        </is>
-      </c>
-      <c r="F28" s="3" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="G28" s="3" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="H28" s="3" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="I28" s="3" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="J28" s="3" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="K28" s="3" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="L28" s="3" t="inlineStr">
-        <is>
-          <t>2 de 26</t>
-        </is>
-      </c>
-      <c r="M28" s="3" t="inlineStr">
-        <is>
-          <t>3 de 26</t>
-        </is>
-      </c>
-      <c r="N28" s="3" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="O28" s="3" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="P28" s="3" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="Q28" s="3" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
-        </is>
-      </c>
-      <c r="R28" s="3" t="inlineStr">
-        <is>
-          <t>0 de 26</t>
+      <c r="M28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" s="3" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="D29" s="3" t="inlineStr">
+        <is>
+          <t>1 de 27</t>
+        </is>
+      </c>
+      <c r="E29" s="3" t="inlineStr">
+        <is>
+          <t>1 de 27</t>
+        </is>
+      </c>
+      <c r="F29" s="3" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="G29" s="3" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="J29" s="3" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="L29" s="3" t="inlineStr">
+        <is>
+          <t>2 de 27</t>
+        </is>
+      </c>
+      <c r="M29" s="3" t="inlineStr">
+        <is>
+          <t>3 de 27</t>
+        </is>
+      </c>
+      <c r="N29" s="3" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="O29" s="3" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="P29" s="3" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="Q29" s="3" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
+        </is>
+      </c>
+      <c r="R29" s="3" t="inlineStr">
+        <is>
+          <t>0 de 27</t>
         </is>
       </c>
     </row>
@@ -2213,7 +2273,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2464,7 +2524,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
+          <t>BRAVO MANZABA MARIA CECILIA</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -2474,7 +2534,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
@@ -2491,7 +2551,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
+          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -2501,7 +2561,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0</v>
@@ -2518,14 +2578,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
+          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>24.39</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>0</v>
@@ -2545,17 +2605,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0</v>
+        <v>24.39</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>354.43</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>0</v>
@@ -2572,17 +2632,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>434.83</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>0</v>
+        <v>354.43</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>0</v>
@@ -2599,11 +2659,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>GARCIA BRAVO JOSE LUIS</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0</v>
+        <v>434.83</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>0</v>
@@ -2626,14 +2686,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>GARCIA BRAVO JOSE LUIS</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>0</v>
@@ -2653,14 +2713,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>0</v>
@@ -2680,11 +2740,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="D17" s="2" t="n">
         <v>0</v>
@@ -2707,14 +2767,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>0</v>
@@ -2734,14 +2794,14 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>308.08</v>
+        <v>238.35</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>0</v>
@@ -2761,17 +2821,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>0</v>
+        <v>308.08</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0</v>
@@ -2788,7 +2848,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>MORALES CAIZA SERGIO IVAN</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -2798,7 +2858,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>367.8</v>
+        <v>238.35</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>0</v>
@@ -2815,17 +2875,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>159.03</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>0</v>
@@ -2842,14 +2902,14 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>0</v>
+        <v>159.03</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>413.5</v>
+        <v>0</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>0</v>
@@ -2869,14 +2929,14 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>43.86</v>
+        <v>413.5</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>0</v>
@@ -2896,20 +2956,20 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>0</v>
+        <v>43.86</v>
       </c>
       <c r="E25" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>3722.63</v>
+        <v>0</v>
       </c>
       <c r="G25" s="2" t="n">
         <v>0</v>
@@ -2923,20 +2983,20 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>565.27</v>
+        <v>0</v>
       </c>
       <c r="E26" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>522.8200000000001</v>
+        <v>3722.63</v>
       </c>
       <c r="G26" s="2" t="n">
         <v>0</v>
@@ -2950,39 +3010,66 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>VEHINVER SA</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>565.27</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>522.8200000000001</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="2" t="n">
+      <c r="C28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2" t="n">
         <v>346.56</v>
       </c>
-      <c r="G27" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="C28" s="4" t="n">
+      <c r="G28" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" s="4" t="n">
         <v>1076.87</v>
       </c>
-      <c r="D28" s="4" t="n">
+      <c r="D29" s="4" t="n">
         <v>2057.76</v>
       </c>
-      <c r="E28" s="4" t="n">
+      <c r="E29" s="4" t="n">
         <v>1423.94</v>
       </c>
-      <c r="F28" s="4" t="n">
+      <c r="F29" s="4" t="n">
         <v>8670.459999999999</v>
       </c>
-      <c r="G28" s="4" t="n">
+      <c r="G29" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-09-08 14:40:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -3147,10 +3147,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>4429.98</v>
+        <v>4661.02</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-4429.98</v>
+        <v>-4661.02</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -3190,13 +3190,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>14124.06</v>
+        <v>14355.1</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>5875.940000000001</v>
+        <v>5644.9</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.706203</v>
+        <v>0.717755</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-08 14:50:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,7 +568,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ALCIVAR BUSTAMANTE ERNESTO EDUARDO</t>
+          <t>AGUILERA ANDRADE FAUSTO ROGELIO</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -628,7 +628,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ANGULO PARRALES CARMEN</t>
+          <t>ALCIVAR BUSTAMANTE ERNESTO EDUARDO</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -688,7 +688,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ARCE CANDO DENISSE YAJAIRA</t>
+          <t>ANGULO PARRALES CARMEN</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -748,7 +748,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AREVALO PEÑA JORGE LUIS</t>
+          <t>ARCE CANDO DENISSE YAJAIRA</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -808,7 +808,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ARMIJO AGUILAR ROBERT LENIN</t>
+          <t>ARCOS GOMEZ CONSTRUCCIONES CIA. LTDA.</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -839,10 +839,10 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>1144.75</v>
+        <v>0</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>2697.41</v>
+        <v>0</v>
       </c>
       <c r="N6" s="2" t="n">
         <v>0</v>
@@ -868,14 +868,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ARQUITECKSA S.A.</t>
+          <t>AREVALO PEÑA JORGE LUIS</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>236.29</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>0</v>
@@ -928,7 +928,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
+          <t>AREVALO SAQUICELA LUIS MARCELO</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -988,7 +988,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BRAVO MANZABA MARIA CECILIA</t>
+          <t>ARMIJO AGUILAR ROBERT LENIN</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1019,10 +1019,10 @@
         <v>0</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>0</v>
+        <v>1144.75</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>0</v>
+        <v>2697.41</v>
       </c>
       <c r="N9" s="2" t="n">
         <v>0</v>
@@ -1048,14 +1048,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
+          <t>ARQUITECKSA S.A.</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0</v>
+        <v>236.29</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>0</v>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
+          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
+          <t>BRAVO MANZABA MARIA CECILIA</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>CARRION ALVAREZ MARIO ANDRES</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>GARCIA BRAVO JOSE LUIS</t>
+          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>CORREA IGLESIAS RAMIRO MARCELO</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -1468,7 +1468,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>GARCIA BRAVO JOSE LUIS</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>GRANJA VANEGAS MARCELA</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>KITCHENSCO S.A.</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -2008,7 +2008,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -2042,7 +2042,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="2" t="n">
-        <v>3722.63</v>
+        <v>0</v>
       </c>
       <c r="N26" s="2" t="n">
         <v>0</v>
@@ -2068,7 +2068,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
@@ -2078,7 +2078,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>94.20999999999999</v>
+        <v>0</v>
       </c>
       <c r="F27" s="2" t="n">
         <v>0</v>
@@ -2102,7 +2102,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="2" t="n">
-        <v>428.61</v>
+        <v>0</v>
       </c>
       <c r="N27" s="2" t="n">
         <v>0</v>
@@ -2128,137 +2128,797 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>MORALES CAIZA SERGIO IVAN</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" s="2" t="n">
+        <v>3722.63</v>
+      </c>
+      <c r="N35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>VACA PANCHI DORYS CAROLINA</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R36" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>VEHINVER SA</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>94.20999999999999</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" s="2" t="n">
+        <v>428.61</v>
+      </c>
+      <c r="N37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" s="2" t="n">
+      <c r="C39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" s="2" t="n">
         <v>346.56</v>
       </c>
-      <c r="M28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R28" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="C29" s="3" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
-      <c r="D29" s="3" t="inlineStr">
-        <is>
-          <t>1 de 27</t>
-        </is>
-      </c>
-      <c r="E29" s="3" t="inlineStr">
-        <is>
-          <t>1 de 27</t>
-        </is>
-      </c>
-      <c r="F29" s="3" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
-      <c r="G29" s="3" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
-      <c r="H29" s="3" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
-      <c r="I29" s="3" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
-      <c r="J29" s="3" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
-      <c r="K29" s="3" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
-      <c r="L29" s="3" t="inlineStr">
-        <is>
-          <t>2 de 27</t>
-        </is>
-      </c>
-      <c r="M29" s="3" t="inlineStr">
-        <is>
-          <t>3 de 27</t>
-        </is>
-      </c>
-      <c r="N29" s="3" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
-      <c r="O29" s="3" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
-      <c r="P29" s="3" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
-      <c r="Q29" s="3" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
-        </is>
-      </c>
-      <c r="R29" s="3" t="inlineStr">
-        <is>
-          <t>0 de 27</t>
+      <c r="M39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="C40" s="3" t="inlineStr">
+        <is>
+          <t>0 de 38</t>
+        </is>
+      </c>
+      <c r="D40" s="3" t="inlineStr">
+        <is>
+          <t>1 de 38</t>
+        </is>
+      </c>
+      <c r="E40" s="3" t="inlineStr">
+        <is>
+          <t>1 de 38</t>
+        </is>
+      </c>
+      <c r="F40" s="3" t="inlineStr">
+        <is>
+          <t>0 de 38</t>
+        </is>
+      </c>
+      <c r="G40" s="3" t="inlineStr">
+        <is>
+          <t>0 de 38</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>0 de 38</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>0 de 38</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>0 de 38</t>
+        </is>
+      </c>
+      <c r="K40" s="3" t="inlineStr">
+        <is>
+          <t>0 de 38</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>2 de 38</t>
+        </is>
+      </c>
+      <c r="M40" s="3" t="inlineStr">
+        <is>
+          <t>3 de 38</t>
+        </is>
+      </c>
+      <c r="N40" s="3" t="inlineStr">
+        <is>
+          <t>0 de 38</t>
+        </is>
+      </c>
+      <c r="O40" s="3" t="inlineStr">
+        <is>
+          <t>0 de 38</t>
+        </is>
+      </c>
+      <c r="P40" s="3" t="inlineStr">
+        <is>
+          <t>0 de 38</t>
+        </is>
+      </c>
+      <c r="Q40" s="3" t="inlineStr">
+        <is>
+          <t>0 de 38</t>
+        </is>
+      </c>
+      <c r="R40" s="3" t="inlineStr">
+        <is>
+          <t>0 de 38</t>
         </is>
       </c>
     </row>
@@ -2273,7 +2933,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2335,14 +2995,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ALCIVAR BUSTAMANTE ERNESTO EDUARDO</t>
+          <t>AGUILERA ANDRADE FAUSTO ROGELIO</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>30.31</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>0</v>
@@ -2362,14 +3022,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ANGULO PARRALES CARMEN</t>
+          <t>ALCIVAR BUSTAMANTE ERNESTO EDUARDO</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>66.2</v>
+        <v>30.31</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>0</v>
@@ -2389,17 +3049,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ARCE CANDO DENISSE YAJAIRA</t>
+          <t>ANGULO PARRALES CARMEN</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0</v>
+        <v>66.2</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>95.56</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>0</v>
@@ -2416,7 +3076,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AREVALO PEÑA JORGE LUIS</t>
+          <t>ARCE CANDO DENISSE YAJAIRA</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -2426,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0</v>
+        <v>95.56</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0</v>
@@ -2443,20 +3103,20 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ARMIJO AGUILAR ROBERT LENIN</t>
+          <t>ARCOS GOMEZ CONSTRUCCIONES CIA. LTDA.</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0</v>
+        <v>832</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0</v>
+        <v>594.47</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>0</v>
+        <v>142.56</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>3842.16</v>
+        <v>0</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>0</v>
@@ -2470,7 +3130,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ARQUITECKSA S.A.</t>
+          <t>AREVALO PEÑA JORGE LUIS</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -2483,7 +3143,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>236.29</v>
+        <v>0</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>0</v>
@@ -2497,11 +3157,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
+          <t>AREVALO SAQUICELA LUIS MARCELO</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>472.57</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>0</v>
@@ -2524,7 +3184,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BRAVO MANZABA MARIA CECILIA</t>
+          <t>ARMIJO AGUILAR ROBERT LENIN</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -2537,7 +3197,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0</v>
+        <v>3842.16</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>0</v>
@@ -2551,7 +3211,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
+          <t>ARQUITECKSA S.A.</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -2561,10 +3221,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0</v>
+        <v>236.29</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0</v>
@@ -2578,11 +3238,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
+          <t>AVILA TORRES RAFAEL ALEJANDRO</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0</v>
+        <v>472.57</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>0</v>
@@ -2605,14 +3265,14 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
+          <t>BRAVO MANZABA MARIA CECILIA</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>24.39</v>
+        <v>0</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>0</v>
@@ -2632,7 +3292,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -2642,7 +3302,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>354.43</v>
+        <v>367.8</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>0</v>
@@ -2659,11 +3319,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>CARRION ALVAREZ MARIO ANDRES</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>434.83</v>
+        <v>155.38</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>0</v>
@@ -2686,7 +3346,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>GARCIA BRAVO JOSE LUIS</t>
+          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -2713,14 +3373,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>CORREA IGLESIAS RAMIRO MARCELO</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>0</v>
@@ -2740,14 +3400,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0</v>
+        <v>24.39</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>0</v>
@@ -2767,7 +3427,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -2777,7 +3437,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>0</v>
+        <v>354.43</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>0</v>
@@ -2794,14 +3454,14 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>0</v>
+        <v>434.83</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>0</v>
@@ -2821,14 +3481,14 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>GARCIA BRAVO JOSE LUIS</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>308.08</v>
+        <v>0</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>0</v>
@@ -2848,7 +3508,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>GRANJA VANEGAS MARCELA</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -2858,7 +3518,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>0</v>
@@ -2875,17 +3535,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>0</v>
@@ -2902,11 +3562,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>KITCHENSCO S.A.</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>159.03</v>
+        <v>0</v>
       </c>
       <c r="D23" s="2" t="n">
         <v>0</v>
@@ -2929,14 +3589,14 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>413.5</v>
+        <v>0</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>0</v>
@@ -2956,14 +3616,14 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>43.86</v>
+        <v>0</v>
       </c>
       <c r="E25" s="2" t="n">
         <v>0</v>
@@ -2983,7 +3643,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -2996,7 +3656,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>3722.63</v>
+        <v>0</v>
       </c>
       <c r="G26" s="2" t="n">
         <v>0</v>
@@ -3010,20 +3670,20 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>565.27</v>
+        <v>238.35</v>
       </c>
       <c r="E27" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>522.8200000000001</v>
+        <v>0</v>
       </c>
       <c r="G27" s="2" t="n">
         <v>0</v>
@@ -3037,39 +3697,336 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>308.08</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>MORALES CAIZA SERGIO IVAN</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>238.35</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>367.8</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>159.03</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>413.5</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>43.86</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>3722.63</v>
+      </c>
+      <c r="G35" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>VACA PANCHI DORYS CAROLINA</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>10.44</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>VEHINVER SA</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>565.27</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <v>522.8200000000001</v>
+      </c>
+      <c r="G37" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="2" t="n">
+      <c r="C39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2" t="n">
         <v>346.56</v>
       </c>
-      <c r="G28" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="C29" s="4" t="n">
-        <v>1076.87</v>
-      </c>
-      <c r="D29" s="4" t="n">
-        <v>2057.76</v>
-      </c>
-      <c r="E29" s="4" t="n">
-        <v>1423.94</v>
-      </c>
-      <c r="F29" s="4" t="n">
+      <c r="G39" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="C40" s="4" t="n">
+        <v>2074.69</v>
+      </c>
+      <c r="D40" s="4" t="n">
+        <v>2652.23</v>
+      </c>
+      <c r="E40" s="4" t="n">
+        <v>1566.5</v>
+      </c>
+      <c r="F40" s="4" t="n">
         <v>8670.459999999999</v>
       </c>
-      <c r="G29" s="4" t="n">
+      <c r="G40" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-09-09 08:45:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -4104,10 +4104,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>4661.02</v>
+        <v>4831.58</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-4661.02</v>
+        <v>-4831.58</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -4147,13 +4147,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>14908.01</v>
+        <v>15078.57</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>5091.99</v>
+        <v>4921.43</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.7454005</v>
+        <v>0.7539285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-10 14:15:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1022,7 +1022,7 @@
         <v>1144.75</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>2697.41</v>
+        <v>2719.7</v>
       </c>
       <c r="N9" s="2" t="n">
         <v>0</v>
@@ -3197,7 +3197,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>3842.16</v>
+        <v>3864.45</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>0</v>
@@ -4024,7 +4024,7 @@
         <v>1566.5</v>
       </c>
       <c r="F40" s="4" t="n">
-        <v>9089.51</v>
+        <v>9111.799999999999</v>
       </c>
       <c r="G40" s="4" t="n">
         <v>0</v>
@@ -4054,7 +4054,7 @@
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="17" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4128,13 +4128,13 @@
         <v>20000</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>10217.27</v>
+        <v>10239.56</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>9782.73</v>
+        <v>9760.440000000001</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.5108635</v>
+        <v>0.5119779999999999</v>
       </c>
     </row>
     <row r="4">
@@ -4147,13 +4147,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>15497.62</v>
+        <v>15519.91</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>4502.379999999999</v>
+        <v>4480.09</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.774881</v>
+        <v>0.7759954999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-11 09:25:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R40"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1828,7 +1828,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>KITCHENSCO S.A.</t>
+          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+          <t>KITCHENSCO S.A.</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -2008,7 +2008,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>MORALES CAIZA SERGIO IVAN</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
@@ -2308,7 +2308,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
@@ -2368,7 +2368,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>PAREDES POVEDA TATIANA VERONICA</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
@@ -2548,7 +2548,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
@@ -2582,7 +2582,7 @@
         <v>0</v>
       </c>
       <c r="M35" s="2" t="n">
-        <v>3692.91</v>
+        <v>0</v>
       </c>
       <c r="N35" s="2" t="n">
         <v>0</v>
@@ -2608,7 +2608,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
@@ -2642,7 +2642,7 @@
         <v>0</v>
       </c>
       <c r="M36" s="2" t="n">
-        <v>0</v>
+        <v>3692.91</v>
       </c>
       <c r="N36" s="2" t="n">
         <v>0</v>
@@ -2668,7 +2668,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
@@ -2678,7 +2678,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>94.20999999999999</v>
+        <v>0</v>
       </c>
       <c r="F37" s="2" t="n">
         <v>0</v>
@@ -2702,7 +2702,7 @@
         <v>0</v>
       </c>
       <c r="M37" s="2" t="n">
-        <v>428.61</v>
+        <v>0</v>
       </c>
       <c r="N37" s="2" t="n">
         <v>0</v>
@@ -2728,7 +2728,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+          <t>VEHINVER SA</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
@@ -2738,7 +2738,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>0</v>
+        <v>94.20999999999999</v>
       </c>
       <c r="F38" s="2" t="n">
         <v>0</v>
@@ -2762,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="M38" s="2" t="n">
-        <v>0</v>
+        <v>428.61</v>
       </c>
       <c r="N38" s="2" t="n">
         <v>0</v>
@@ -2788,137 +2788,197 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L39" s="2" t="n">
+      <c r="C40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" s="2" t="n">
         <v>346.56</v>
       </c>
-      <c r="M39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R39" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="C40" s="3" t="inlineStr">
-        <is>
-          <t>0 de 38</t>
-        </is>
-      </c>
-      <c r="D40" s="3" t="inlineStr">
-        <is>
-          <t>1 de 38</t>
-        </is>
-      </c>
-      <c r="E40" s="3" t="inlineStr">
-        <is>
-          <t>1 de 38</t>
-        </is>
-      </c>
-      <c r="F40" s="3" t="inlineStr">
-        <is>
-          <t>0 de 38</t>
-        </is>
-      </c>
-      <c r="G40" s="3" t="inlineStr">
-        <is>
-          <t>0 de 38</t>
-        </is>
-      </c>
-      <c r="H40" s="3" t="inlineStr">
-        <is>
-          <t>0 de 38</t>
-        </is>
-      </c>
-      <c r="I40" s="3" t="inlineStr">
-        <is>
-          <t>0 de 38</t>
-        </is>
-      </c>
-      <c r="J40" s="3" t="inlineStr">
-        <is>
-          <t>0 de 38</t>
-        </is>
-      </c>
-      <c r="K40" s="3" t="inlineStr">
-        <is>
-          <t>0 de 38</t>
-        </is>
-      </c>
-      <c r="L40" s="3" t="inlineStr">
-        <is>
-          <t>3 de 38</t>
-        </is>
-      </c>
-      <c r="M40" s="3" t="inlineStr">
-        <is>
-          <t>3 de 38</t>
-        </is>
-      </c>
-      <c r="N40" s="3" t="inlineStr">
-        <is>
-          <t>0 de 38</t>
-        </is>
-      </c>
-      <c r="O40" s="3" t="inlineStr">
-        <is>
-          <t>0 de 38</t>
-        </is>
-      </c>
-      <c r="P40" s="3" t="inlineStr">
-        <is>
-          <t>0 de 38</t>
-        </is>
-      </c>
-      <c r="Q40" s="3" t="inlineStr">
-        <is>
-          <t>0 de 38</t>
-        </is>
-      </c>
-      <c r="R40" s="3" t="inlineStr">
-        <is>
-          <t>0 de 38</t>
+      <c r="M40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R40" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="C41" s="3" t="inlineStr">
+        <is>
+          <t>0 de 39</t>
+        </is>
+      </c>
+      <c r="D41" s="3" t="inlineStr">
+        <is>
+          <t>1 de 39</t>
+        </is>
+      </c>
+      <c r="E41" s="3" t="inlineStr">
+        <is>
+          <t>1 de 39</t>
+        </is>
+      </c>
+      <c r="F41" s="3" t="inlineStr">
+        <is>
+          <t>0 de 39</t>
+        </is>
+      </c>
+      <c r="G41" s="3" t="inlineStr">
+        <is>
+          <t>0 de 39</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>0 de 39</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>0 de 39</t>
+        </is>
+      </c>
+      <c r="J41" s="3" t="inlineStr">
+        <is>
+          <t>0 de 39</t>
+        </is>
+      </c>
+      <c r="K41" s="3" t="inlineStr">
+        <is>
+          <t>0 de 39</t>
+        </is>
+      </c>
+      <c r="L41" s="3" t="inlineStr">
+        <is>
+          <t>3 de 39</t>
+        </is>
+      </c>
+      <c r="M41" s="3" t="inlineStr">
+        <is>
+          <t>3 de 39</t>
+        </is>
+      </c>
+      <c r="N41" s="3" t="inlineStr">
+        <is>
+          <t>0 de 39</t>
+        </is>
+      </c>
+      <c r="O41" s="3" t="inlineStr">
+        <is>
+          <t>0 de 39</t>
+        </is>
+      </c>
+      <c r="P41" s="3" t="inlineStr">
+        <is>
+          <t>0 de 39</t>
+        </is>
+      </c>
+      <c r="Q41" s="3" t="inlineStr">
+        <is>
+          <t>0 de 39</t>
+        </is>
+      </c>
+      <c r="R41" s="3" t="inlineStr">
+        <is>
+          <t>0 de 39</t>
         </is>
       </c>
     </row>
@@ -2933,7 +2993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3562,7 +3622,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>KITCHENSCO S.A.</t>
+          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -3589,7 +3649,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+          <t>KITCHENSCO S.A.</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -3616,11 +3676,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="D25" s="2" t="n">
         <v>0</v>
@@ -3643,11 +3703,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="D26" s="2" t="n">
         <v>0</v>
@@ -3670,14 +3730,14 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="E27" s="2" t="n">
         <v>0</v>
@@ -3697,14 +3757,14 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>308.08</v>
+        <v>238.35</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>0</v>
@@ -3724,17 +3784,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>0</v>
+        <v>308.08</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="F29" s="2" t="n">
         <v>0</v>
@@ -3751,7 +3811,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>MORALES CAIZA SERGIO IVAN</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
@@ -3761,7 +3821,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>367.8</v>
+        <v>238.35</v>
       </c>
       <c r="F30" s="2" t="n">
         <v>0</v>
@@ -3778,17 +3838,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
-        <v>159.03</v>
+        <v>0</v>
       </c>
       <c r="D31" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="F31" s="2" t="n">
         <v>0</v>
@@ -3805,11 +3865,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>PAREDES POVEDA TATIANA VERONICA</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>0</v>
+        <v>159.03</v>
       </c>
       <c r="D32" s="2" t="n">
         <v>0</v>
@@ -3832,14 +3892,14 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>413.5</v>
+        <v>0</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>0</v>
@@ -3859,14 +3919,14 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>43.86</v>
+        <v>413.5</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>0</v>
@@ -3886,20 +3946,20 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>0</v>
+        <v>43.86</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>3692.91</v>
+        <v>0</v>
       </c>
       <c r="G35" s="2" t="n">
         <v>0</v>
@@ -3913,11 +3973,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="D36" s="2" t="n">
         <v>0</v>
@@ -3926,7 +3986,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>0</v>
+        <v>3692.91</v>
       </c>
       <c r="G36" s="2" t="n">
         <v>0</v>
@@ -3940,20 +4000,20 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>565.27</v>
+        <v>0</v>
       </c>
       <c r="E37" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>522.8200000000001</v>
+        <v>0</v>
       </c>
       <c r="G37" s="2" t="n">
         <v>0</v>
@@ -3967,20 +4027,20 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+          <t>VEHINVER SA</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>0</v>
+        <v>565.27</v>
       </c>
       <c r="E38" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>0</v>
+        <v>522.8200000000001</v>
       </c>
       <c r="G38" s="2" t="n">
         <v>0</v>
@@ -3994,39 +4054,66 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="2" t="n">
+      <c r="C40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2" t="n">
         <v>346.56</v>
       </c>
-      <c r="G39" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="C40" s="4" t="n">
+      <c r="G40" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="C41" s="4" t="n">
         <v>2074.69</v>
       </c>
-      <c r="D40" s="4" t="n">
+      <c r="D41" s="4" t="n">
         <v>2652.23</v>
       </c>
-      <c r="E40" s="4" t="n">
+      <c r="E41" s="4" t="n">
         <v>1566.5</v>
       </c>
-      <c r="F40" s="4" t="n">
+      <c r="F41" s="4" t="n">
         <v>9111.799999999999</v>
       </c>
-      <c r="G40" s="4" t="n">
+      <c r="G41" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-09-11 12:20:10
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1348,7 +1348,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
+          <t>COBO FOLLECO JORGE ERNESTO</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>CORREA IGLESIAS RAMIRO MARCELO</t>
+          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -1468,7 +1468,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
+          <t>CORREA IGLESIAS RAMIRO MARCELO</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>GARCIA BRAVO JOSE LUIS</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>GRANJA VANEGAS MARCELA</t>
+          <t>GARCIA BRAVO JOSE LUIS</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>GRANJA VANEGAS MARCELA</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>KITCHENSCO S.A.</t>
+          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+          <t>KITCHENSCO S.A.</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -2008,7 +2008,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
@@ -2308,7 +2308,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>MORALES CAIZA SERGIO IVAN</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
@@ -2368,7 +2368,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>PAREDES POVEDA TATIANA VERONICA</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
@@ -2548,7 +2548,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
@@ -2608,7 +2608,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
@@ -2642,7 +2642,7 @@
         <v>0</v>
       </c>
       <c r="M36" s="2" t="n">
-        <v>3692.91</v>
+        <v>0</v>
       </c>
       <c r="N36" s="2" t="n">
         <v>0</v>
@@ -2668,7 +2668,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
@@ -2702,7 +2702,7 @@
         <v>0</v>
       </c>
       <c r="M37" s="2" t="n">
-        <v>0</v>
+        <v>3692.91</v>
       </c>
       <c r="N37" s="2" t="n">
         <v>0</v>
@@ -2728,7 +2728,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
@@ -2738,7 +2738,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>94.20999999999999</v>
+        <v>0</v>
       </c>
       <c r="F38" s="2" t="n">
         <v>0</v>
@@ -2762,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="M38" s="2" t="n">
-        <v>428.61</v>
+        <v>0</v>
       </c>
       <c r="N38" s="2" t="n">
         <v>0</v>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+          <t>VEHINVER SA</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
@@ -2798,7 +2798,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>0</v>
+        <v>94.20999999999999</v>
       </c>
       <c r="F39" s="2" t="n">
         <v>0</v>
@@ -2822,7 +2822,7 @@
         <v>0</v>
       </c>
       <c r="M39" s="2" t="n">
-        <v>0</v>
+        <v>428.61</v>
       </c>
       <c r="N39" s="2" t="n">
         <v>0</v>
@@ -2848,137 +2848,197 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R40" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L40" s="2" t="n">
+      <c r="C41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" s="2" t="n">
         <v>346.56</v>
       </c>
-      <c r="M40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R40" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="C41" s="3" t="inlineStr">
-        <is>
-          <t>0 de 39</t>
-        </is>
-      </c>
-      <c r="D41" s="3" t="inlineStr">
-        <is>
-          <t>1 de 39</t>
-        </is>
-      </c>
-      <c r="E41" s="3" t="inlineStr">
-        <is>
-          <t>1 de 39</t>
-        </is>
-      </c>
-      <c r="F41" s="3" t="inlineStr">
-        <is>
-          <t>0 de 39</t>
-        </is>
-      </c>
-      <c r="G41" s="3" t="inlineStr">
-        <is>
-          <t>0 de 39</t>
-        </is>
-      </c>
-      <c r="H41" s="3" t="inlineStr">
-        <is>
-          <t>0 de 39</t>
-        </is>
-      </c>
-      <c r="I41" s="3" t="inlineStr">
-        <is>
-          <t>0 de 39</t>
-        </is>
-      </c>
-      <c r="J41" s="3" t="inlineStr">
-        <is>
-          <t>0 de 39</t>
-        </is>
-      </c>
-      <c r="K41" s="3" t="inlineStr">
-        <is>
-          <t>0 de 39</t>
-        </is>
-      </c>
-      <c r="L41" s="3" t="inlineStr">
-        <is>
-          <t>3 de 39</t>
-        </is>
-      </c>
-      <c r="M41" s="3" t="inlineStr">
-        <is>
-          <t>3 de 39</t>
-        </is>
-      </c>
-      <c r="N41" s="3" t="inlineStr">
-        <is>
-          <t>0 de 39</t>
-        </is>
-      </c>
-      <c r="O41" s="3" t="inlineStr">
-        <is>
-          <t>0 de 39</t>
-        </is>
-      </c>
-      <c r="P41" s="3" t="inlineStr">
-        <is>
-          <t>0 de 39</t>
-        </is>
-      </c>
-      <c r="Q41" s="3" t="inlineStr">
-        <is>
-          <t>0 de 39</t>
-        </is>
-      </c>
-      <c r="R41" s="3" t="inlineStr">
-        <is>
-          <t>0 de 39</t>
+      <c r="M41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="C42" s="3" t="inlineStr">
+        <is>
+          <t>0 de 40</t>
+        </is>
+      </c>
+      <c r="D42" s="3" t="inlineStr">
+        <is>
+          <t>1 de 40</t>
+        </is>
+      </c>
+      <c r="E42" s="3" t="inlineStr">
+        <is>
+          <t>1 de 40</t>
+        </is>
+      </c>
+      <c r="F42" s="3" t="inlineStr">
+        <is>
+          <t>0 de 40</t>
+        </is>
+      </c>
+      <c r="G42" s="3" t="inlineStr">
+        <is>
+          <t>0 de 40</t>
+        </is>
+      </c>
+      <c r="H42" s="3" t="inlineStr">
+        <is>
+          <t>0 de 40</t>
+        </is>
+      </c>
+      <c r="I42" s="3" t="inlineStr">
+        <is>
+          <t>0 de 40</t>
+        </is>
+      </c>
+      <c r="J42" s="3" t="inlineStr">
+        <is>
+          <t>0 de 40</t>
+        </is>
+      </c>
+      <c r="K42" s="3" t="inlineStr">
+        <is>
+          <t>0 de 40</t>
+        </is>
+      </c>
+      <c r="L42" s="3" t="inlineStr">
+        <is>
+          <t>3 de 40</t>
+        </is>
+      </c>
+      <c r="M42" s="3" t="inlineStr">
+        <is>
+          <t>3 de 40</t>
+        </is>
+      </c>
+      <c r="N42" s="3" t="inlineStr">
+        <is>
+          <t>0 de 40</t>
+        </is>
+      </c>
+      <c r="O42" s="3" t="inlineStr">
+        <is>
+          <t>0 de 40</t>
+        </is>
+      </c>
+      <c r="P42" s="3" t="inlineStr">
+        <is>
+          <t>0 de 40</t>
+        </is>
+      </c>
+      <c r="Q42" s="3" t="inlineStr">
+        <is>
+          <t>0 de 40</t>
+        </is>
+      </c>
+      <c r="R42" s="3" t="inlineStr">
+        <is>
+          <t>0 de 40</t>
         </is>
       </c>
     </row>
@@ -2993,7 +3053,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3406,7 +3466,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
+          <t>COBO FOLLECO JORGE ERNESTO</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -3433,7 +3493,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>CORREA IGLESIAS RAMIRO MARCELO</t>
+          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -3460,14 +3520,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
+          <t>CORREA IGLESIAS RAMIRO MARCELO</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>24.39</v>
+        <v>0</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>0</v>
@@ -3487,17 +3547,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>0</v>
+        <v>24.39</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>354.43</v>
+        <v>0</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>0</v>
@@ -3514,17 +3574,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>434.83</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>0</v>
+        <v>354.43</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>0</v>
@@ -3541,11 +3601,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>GARCIA BRAVO JOSE LUIS</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0</v>
+        <v>434.83</v>
       </c>
       <c r="D20" s="2" t="n">
         <v>0</v>
@@ -3568,7 +3628,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>GRANJA VANEGAS MARCELA</t>
+          <t>GARCIA BRAVO JOSE LUIS</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -3595,14 +3655,14 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>GRANJA VANEGAS MARCELA</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>0</v>
@@ -3622,14 +3682,14 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>0</v>
@@ -3649,7 +3709,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>KITCHENSCO S.A.</t>
+          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -3676,7 +3736,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+          <t>KITCHENSCO S.A.</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -3703,11 +3763,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="D26" s="2" t="n">
         <v>0</v>
@@ -3730,11 +3790,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="D27" s="2" t="n">
         <v>0</v>
@@ -3757,14 +3817,14 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>0</v>
@@ -3784,14 +3844,14 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>308.08</v>
+        <v>238.35</v>
       </c>
       <c r="E29" s="2" t="n">
         <v>0</v>
@@ -3811,17 +3871,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>0</v>
+        <v>308.08</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="F30" s="2" t="n">
         <v>0</v>
@@ -3838,7 +3898,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>MORALES CAIZA SERGIO IVAN</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
@@ -3848,7 +3908,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>367.8</v>
+        <v>238.35</v>
       </c>
       <c r="F31" s="2" t="n">
         <v>0</v>
@@ -3865,17 +3925,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>159.03</v>
+        <v>0</v>
       </c>
       <c r="D32" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="F32" s="2" t="n">
         <v>0</v>
@@ -3892,11 +3952,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>PAREDES POVEDA TATIANA VERONICA</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
-        <v>0</v>
+        <v>159.03</v>
       </c>
       <c r="D33" s="2" t="n">
         <v>0</v>
@@ -3919,14 +3979,14 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>413.5</v>
+        <v>0</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>0</v>
@@ -3946,14 +4006,14 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>43.86</v>
+        <v>413.5</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>0</v>
@@ -3973,20 +4033,20 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>0</v>
+        <v>43.86</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>3692.91</v>
+        <v>0</v>
       </c>
       <c r="G36" s="2" t="n">
         <v>0</v>
@@ -4000,11 +4060,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="D37" s="2" t="n">
         <v>0</v>
@@ -4013,7 +4073,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>0</v>
+        <v>3692.91</v>
       </c>
       <c r="G37" s="2" t="n">
         <v>0</v>
@@ -4027,20 +4087,20 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>565.27</v>
+        <v>0</v>
       </c>
       <c r="E38" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>522.8200000000001</v>
+        <v>0</v>
       </c>
       <c r="G38" s="2" t="n">
         <v>0</v>
@@ -4054,20 +4114,20 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+          <t>VEHINVER SA</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>0</v>
+        <v>565.27</v>
       </c>
       <c r="E39" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>0</v>
+        <v>522.8200000000001</v>
       </c>
       <c r="G39" s="2" t="n">
         <v>0</v>
@@ -4081,39 +4141,66 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="2" t="n">
+      <c r="C41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="2" t="n">
         <v>346.56</v>
       </c>
-      <c r="G40" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="C41" s="4" t="n">
+      <c r="G41" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="C42" s="4" t="n">
         <v>2074.69</v>
       </c>
-      <c r="D41" s="4" t="n">
+      <c r="D42" s="4" t="n">
         <v>2652.23</v>
       </c>
-      <c r="E41" s="4" t="n">
+      <c r="E42" s="4" t="n">
         <v>1566.5</v>
       </c>
-      <c r="F41" s="4" t="n">
+      <c r="F42" s="4" t="n">
         <v>9111.799999999999</v>
       </c>
-      <c r="G41" s="4" t="n">
+      <c r="G42" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-09-12 09:00:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1379,7 +1379,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>0</v>
+        <v>508.48</v>
       </c>
       <c r="M15" s="2" t="n">
         <v>0</v>
@@ -3008,7 +3008,7 @@
       </c>
       <c r="L42" s="3" t="inlineStr">
         <is>
-          <t>3 de 40</t>
+          <t>4 de 40</t>
         </is>
       </c>
       <c r="M42" s="3" t="inlineStr">
@@ -3479,7 +3479,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>0</v>
+        <v>508.48</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>0</v>
@@ -4198,7 +4198,7 @@
         <v>1566.5</v>
       </c>
       <c r="F42" s="4" t="n">
-        <v>9111.799999999999</v>
+        <v>9620.279999999999</v>
       </c>
       <c r="G42" s="4" t="n">
         <v>0</v>
@@ -4278,10 +4278,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>5280.35</v>
+        <v>5788.83</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-5280.35</v>
+        <v>-5788.83</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -4321,13 +4321,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>15519.91</v>
+        <v>16028.39</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>4480.09</v>
+        <v>3971.610000000001</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.7759954999999999</v>
+        <v>0.8014195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-12 15:05:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2608,7 +2608,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
@@ -2702,7 +2702,7 @@
         <v>0</v>
       </c>
       <c r="M37" s="2" t="n">
-        <v>3692.91</v>
+        <v>0</v>
       </c>
       <c r="N37" s="2" t="n">
         <v>0</v>
@@ -2728,7 +2728,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
@@ -2762,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="M38" s="2" t="n">
-        <v>0</v>
+        <v>3692.91</v>
       </c>
       <c r="N38" s="2" t="n">
         <v>0</v>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
@@ -2798,7 +2798,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>94.20999999999999</v>
+        <v>0</v>
       </c>
       <c r="F39" s="2" t="n">
         <v>0</v>
@@ -2822,7 +2822,7 @@
         <v>0</v>
       </c>
       <c r="M39" s="2" t="n">
-        <v>428.61</v>
+        <v>0</v>
       </c>
       <c r="N39" s="2" t="n">
         <v>0</v>
@@ -2848,7 +2848,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+          <t>VEHINVER SA</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
@@ -2858,7 +2858,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>0</v>
+        <v>94.20999999999999</v>
       </c>
       <c r="F40" s="2" t="n">
         <v>0</v>
@@ -2882,7 +2882,7 @@
         <v>0</v>
       </c>
       <c r="M40" s="2" t="n">
-        <v>0</v>
+        <v>428.61</v>
       </c>
       <c r="N40" s="2" t="n">
         <v>0</v>
@@ -2908,137 +2908,197 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" s="2" t="n">
+      <c r="C42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" s="2" t="n">
         <v>346.56</v>
       </c>
-      <c r="M41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R41" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="C42" s="3" t="inlineStr">
-        <is>
-          <t>0 de 40</t>
-        </is>
-      </c>
-      <c r="D42" s="3" t="inlineStr">
-        <is>
-          <t>1 de 40</t>
-        </is>
-      </c>
-      <c r="E42" s="3" t="inlineStr">
-        <is>
-          <t>1 de 40</t>
-        </is>
-      </c>
-      <c r="F42" s="3" t="inlineStr">
-        <is>
-          <t>0 de 40</t>
-        </is>
-      </c>
-      <c r="G42" s="3" t="inlineStr">
-        <is>
-          <t>0 de 40</t>
-        </is>
-      </c>
-      <c r="H42" s="3" t="inlineStr">
-        <is>
-          <t>0 de 40</t>
-        </is>
-      </c>
-      <c r="I42" s="3" t="inlineStr">
-        <is>
-          <t>0 de 40</t>
-        </is>
-      </c>
-      <c r="J42" s="3" t="inlineStr">
-        <is>
-          <t>0 de 40</t>
-        </is>
-      </c>
-      <c r="K42" s="3" t="inlineStr">
-        <is>
-          <t>0 de 40</t>
-        </is>
-      </c>
-      <c r="L42" s="3" t="inlineStr">
-        <is>
-          <t>4 de 40</t>
-        </is>
-      </c>
-      <c r="M42" s="3" t="inlineStr">
-        <is>
-          <t>3 de 40</t>
-        </is>
-      </c>
-      <c r="N42" s="3" t="inlineStr">
-        <is>
-          <t>0 de 40</t>
-        </is>
-      </c>
-      <c r="O42" s="3" t="inlineStr">
-        <is>
-          <t>0 de 40</t>
-        </is>
-      </c>
-      <c r="P42" s="3" t="inlineStr">
-        <is>
-          <t>0 de 40</t>
-        </is>
-      </c>
-      <c r="Q42" s="3" t="inlineStr">
-        <is>
-          <t>0 de 40</t>
-        </is>
-      </c>
-      <c r="R42" s="3" t="inlineStr">
-        <is>
-          <t>0 de 40</t>
+      <c r="M42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R42" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="C43" s="3" t="inlineStr">
+        <is>
+          <t>0 de 41</t>
+        </is>
+      </c>
+      <c r="D43" s="3" t="inlineStr">
+        <is>
+          <t>1 de 41</t>
+        </is>
+      </c>
+      <c r="E43" s="3" t="inlineStr">
+        <is>
+          <t>1 de 41</t>
+        </is>
+      </c>
+      <c r="F43" s="3" t="inlineStr">
+        <is>
+          <t>0 de 41</t>
+        </is>
+      </c>
+      <c r="G43" s="3" t="inlineStr">
+        <is>
+          <t>0 de 41</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>0 de 41</t>
+        </is>
+      </c>
+      <c r="I43" s="3" t="inlineStr">
+        <is>
+          <t>0 de 41</t>
+        </is>
+      </c>
+      <c r="J43" s="3" t="inlineStr">
+        <is>
+          <t>0 de 41</t>
+        </is>
+      </c>
+      <c r="K43" s="3" t="inlineStr">
+        <is>
+          <t>0 de 41</t>
+        </is>
+      </c>
+      <c r="L43" s="3" t="inlineStr">
+        <is>
+          <t>4 de 41</t>
+        </is>
+      </c>
+      <c r="M43" s="3" t="inlineStr">
+        <is>
+          <t>3 de 41</t>
+        </is>
+      </c>
+      <c r="N43" s="3" t="inlineStr">
+        <is>
+          <t>0 de 41</t>
+        </is>
+      </c>
+      <c r="O43" s="3" t="inlineStr">
+        <is>
+          <t>0 de 41</t>
+        </is>
+      </c>
+      <c r="P43" s="3" t="inlineStr">
+        <is>
+          <t>0 de 41</t>
+        </is>
+      </c>
+      <c r="Q43" s="3" t="inlineStr">
+        <is>
+          <t>0 de 41</t>
+        </is>
+      </c>
+      <c r="R43" s="3" t="inlineStr">
+        <is>
+          <t>0 de 41</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3113,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4033,14 +4093,14 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>43.86</v>
+        <v>0</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>0</v>
@@ -4060,20 +4120,20 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>0</v>
+        <v>43.86</v>
       </c>
       <c r="E37" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>3692.91</v>
+        <v>0</v>
       </c>
       <c r="G37" s="2" t="n">
         <v>0</v>
@@ -4087,11 +4147,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="D38" s="2" t="n">
         <v>0</v>
@@ -4100,7 +4160,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>0</v>
+        <v>3692.91</v>
       </c>
       <c r="G38" s="2" t="n">
         <v>0</v>
@@ -4114,20 +4174,20 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>565.27</v>
+        <v>0</v>
       </c>
       <c r="E39" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>522.8200000000001</v>
+        <v>0</v>
       </c>
       <c r="G39" s="2" t="n">
         <v>0</v>
@@ -4141,20 +4201,20 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+          <t>VEHINVER SA</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>0</v>
+        <v>565.27</v>
       </c>
       <c r="E40" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>0</v>
+        <v>522.8200000000001</v>
       </c>
       <c r="G40" s="2" t="n">
         <v>0</v>
@@ -4168,39 +4228,66 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="2" t="n">
+      <c r="C42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="2" t="n">
         <v>346.56</v>
       </c>
-      <c r="G41" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="C42" s="4" t="n">
+      <c r="G42" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="C43" s="4" t="n">
         <v>2074.69</v>
       </c>
-      <c r="D42" s="4" t="n">
+      <c r="D43" s="4" t="n">
         <v>2652.23</v>
       </c>
-      <c r="E42" s="4" t="n">
+      <c r="E43" s="4" t="n">
         <v>1566.5</v>
       </c>
-      <c r="F42" s="4" t="n">
+      <c r="F43" s="4" t="n">
         <v>9620.279999999999</v>
       </c>
-      <c r="G42" s="4" t="n">
+      <c r="G43" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-09-12 15:40:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R43"/>
+  <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
+          <t>BRITO MORALES MARIA SOLEDAD</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CARRION ALVAREZ MARIO ANDRES</t>
+          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>COBO FOLLECO JORGE ERNESTO</t>
+          <t>CARRION ALVAREZ MARIO ANDRES</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1379,7 +1379,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>508.48</v>
+        <v>0</v>
       </c>
       <c r="M15" s="2" t="n">
         <v>0</v>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
+          <t>COBO FOLLECO JORGE ERNESTO</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -1439,7 +1439,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>0</v>
+        <v>508.48</v>
       </c>
       <c r="M16" s="2" t="n">
         <v>0</v>
@@ -1468,7 +1468,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>CORREA IGLESIAS RAMIRO MARCELO</t>
+          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
+          <t>CORREA IGLESIAS RAMIRO MARCELO</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>GARCIA BRAVO JOSE LUIS</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>GRANJA VANEGAS MARCELA</t>
+          <t>GARCIA BRAVO JOSE LUIS</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>GRANJA VANEGAS MARCELA</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>KITCHENSCO S.A.</t>
+          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -2008,7 +2008,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+          <t>KITCHENSCO S.A.</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
@@ -2308,7 +2308,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
@@ -2368,7 +2368,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>MORALES CAIZA SERGIO IVAN</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>PAREDES POVEDA TATIANA VERONICA</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
@@ -2548,7 +2548,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
@@ -2608,7 +2608,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
@@ -2762,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="M38" s="2" t="n">
-        <v>3692.91</v>
+        <v>0</v>
       </c>
       <c r="N38" s="2" t="n">
         <v>0</v>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
@@ -2822,7 +2822,7 @@
         <v>0</v>
       </c>
       <c r="M39" s="2" t="n">
-        <v>0</v>
+        <v>3692.91</v>
       </c>
       <c r="N39" s="2" t="n">
         <v>0</v>
@@ -2848,7 +2848,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
@@ -2858,7 +2858,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>94.20999999999999</v>
+        <v>0</v>
       </c>
       <c r="F40" s="2" t="n">
         <v>0</v>
@@ -2882,7 +2882,7 @@
         <v>0</v>
       </c>
       <c r="M40" s="2" t="n">
-        <v>428.61</v>
+        <v>0</v>
       </c>
       <c r="N40" s="2" t="n">
         <v>0</v>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+          <t>VEHINVER SA</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
@@ -2918,7 +2918,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>0</v>
+        <v>94.20999999999999</v>
       </c>
       <c r="F41" s="2" t="n">
         <v>0</v>
@@ -2942,7 +2942,7 @@
         <v>0</v>
       </c>
       <c r="M41" s="2" t="n">
-        <v>0</v>
+        <v>428.61</v>
       </c>
       <c r="N41" s="2" t="n">
         <v>0</v>
@@ -2968,137 +2968,197 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R42" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L42" s="2" t="n">
+      <c r="C43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" s="2" t="n">
         <v>346.56</v>
       </c>
-      <c r="M42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R42" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="C43" s="3" t="inlineStr">
-        <is>
-          <t>0 de 41</t>
-        </is>
-      </c>
-      <c r="D43" s="3" t="inlineStr">
-        <is>
-          <t>1 de 41</t>
-        </is>
-      </c>
-      <c r="E43" s="3" t="inlineStr">
-        <is>
-          <t>1 de 41</t>
-        </is>
-      </c>
-      <c r="F43" s="3" t="inlineStr">
-        <is>
-          <t>0 de 41</t>
-        </is>
-      </c>
-      <c r="G43" s="3" t="inlineStr">
-        <is>
-          <t>0 de 41</t>
-        </is>
-      </c>
-      <c r="H43" s="3" t="inlineStr">
-        <is>
-          <t>0 de 41</t>
-        </is>
-      </c>
-      <c r="I43" s="3" t="inlineStr">
-        <is>
-          <t>0 de 41</t>
-        </is>
-      </c>
-      <c r="J43" s="3" t="inlineStr">
-        <is>
-          <t>0 de 41</t>
-        </is>
-      </c>
-      <c r="K43" s="3" t="inlineStr">
-        <is>
-          <t>0 de 41</t>
-        </is>
-      </c>
-      <c r="L43" s="3" t="inlineStr">
-        <is>
-          <t>4 de 41</t>
-        </is>
-      </c>
-      <c r="M43" s="3" t="inlineStr">
-        <is>
-          <t>3 de 41</t>
-        </is>
-      </c>
-      <c r="N43" s="3" t="inlineStr">
-        <is>
-          <t>0 de 41</t>
-        </is>
-      </c>
-      <c r="O43" s="3" t="inlineStr">
-        <is>
-          <t>0 de 41</t>
-        </is>
-      </c>
-      <c r="P43" s="3" t="inlineStr">
-        <is>
-          <t>0 de 41</t>
-        </is>
-      </c>
-      <c r="Q43" s="3" t="inlineStr">
-        <is>
-          <t>0 de 41</t>
-        </is>
-      </c>
-      <c r="R43" s="3" t="inlineStr">
-        <is>
-          <t>0 de 41</t>
+      <c r="M43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R43" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="C44" s="3" t="inlineStr">
+        <is>
+          <t>0 de 42</t>
+        </is>
+      </c>
+      <c r="D44" s="3" t="inlineStr">
+        <is>
+          <t>1 de 42</t>
+        </is>
+      </c>
+      <c r="E44" s="3" t="inlineStr">
+        <is>
+          <t>1 de 42</t>
+        </is>
+      </c>
+      <c r="F44" s="3" t="inlineStr">
+        <is>
+          <t>0 de 42</t>
+        </is>
+      </c>
+      <c r="G44" s="3" t="inlineStr">
+        <is>
+          <t>0 de 42</t>
+        </is>
+      </c>
+      <c r="H44" s="3" t="inlineStr">
+        <is>
+          <t>0 de 42</t>
+        </is>
+      </c>
+      <c r="I44" s="3" t="inlineStr">
+        <is>
+          <t>0 de 42</t>
+        </is>
+      </c>
+      <c r="J44" s="3" t="inlineStr">
+        <is>
+          <t>0 de 42</t>
+        </is>
+      </c>
+      <c r="K44" s="3" t="inlineStr">
+        <is>
+          <t>0 de 42</t>
+        </is>
+      </c>
+      <c r="L44" s="3" t="inlineStr">
+        <is>
+          <t>4 de 42</t>
+        </is>
+      </c>
+      <c r="M44" s="3" t="inlineStr">
+        <is>
+          <t>3 de 42</t>
+        </is>
+      </c>
+      <c r="N44" s="3" t="inlineStr">
+        <is>
+          <t>0 de 42</t>
+        </is>
+      </c>
+      <c r="O44" s="3" t="inlineStr">
+        <is>
+          <t>0 de 42</t>
+        </is>
+      </c>
+      <c r="P44" s="3" t="inlineStr">
+        <is>
+          <t>0 de 42</t>
+        </is>
+      </c>
+      <c r="Q44" s="3" t="inlineStr">
+        <is>
+          <t>0 de 42</t>
+        </is>
+      </c>
+      <c r="R44" s="3" t="inlineStr">
+        <is>
+          <t>0 de 42</t>
         </is>
       </c>
     </row>
@@ -3113,7 +3173,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3472,7 +3532,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
+          <t>BRITO MORALES MARIA SOLEDAD</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -3482,7 +3542,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>0</v>
@@ -3499,17 +3559,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CARRION ALVAREZ MARIO ANDRES</t>
+          <t>CARAVEDO PAZMIÑO  JAHAIRA PAMELA</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>155.38</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>0</v>
@@ -3526,11 +3586,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>COBO FOLLECO JORGE ERNESTO</t>
+          <t>CARRION ALVAREZ MARIO ANDRES</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>0</v>
+        <v>155.38</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>0</v>
@@ -3539,7 +3599,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>508.48</v>
+        <v>0</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>0</v>
@@ -3553,7 +3613,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
+          <t>COBO FOLLECO JORGE ERNESTO</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -3566,7 +3626,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>0</v>
+        <v>508.48</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>0</v>
@@ -3580,7 +3640,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>CORREA IGLESIAS RAMIRO MARCELO</t>
+          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -3607,14 +3667,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
+          <t>CORREA IGLESIAS RAMIRO MARCELO</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>24.39</v>
+        <v>0</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>0</v>
@@ -3634,17 +3694,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>0</v>
+        <v>24.39</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>354.43</v>
+        <v>0</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>0</v>
@@ -3661,17 +3721,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>434.83</v>
+        <v>0</v>
       </c>
       <c r="D20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>0</v>
+        <v>354.43</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0</v>
@@ -3688,11 +3748,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>GARCIA BRAVO JOSE LUIS</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>0</v>
+        <v>434.83</v>
       </c>
       <c r="D21" s="2" t="n">
         <v>0</v>
@@ -3715,7 +3775,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>GRANJA VANEGAS MARCELA</t>
+          <t>GARCIA BRAVO JOSE LUIS</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -3742,14 +3802,14 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>GRANJA VANEGAS MARCELA</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>0</v>
@@ -3769,14 +3829,14 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>0</v>
@@ -3796,7 +3856,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>KITCHENSCO S.A.</t>
+          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -3823,7 +3883,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+          <t>KITCHENSCO S.A.</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -3850,11 +3910,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="D27" s="2" t="n">
         <v>0</v>
@@ -3877,11 +3937,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="D28" s="2" t="n">
         <v>0</v>
@@ -3904,14 +3964,14 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="E29" s="2" t="n">
         <v>0</v>
@@ -3931,14 +3991,14 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>308.08</v>
+        <v>238.35</v>
       </c>
       <c r="E30" s="2" t="n">
         <v>0</v>
@@ -3958,17 +4018,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>0</v>
+        <v>308.08</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="F31" s="2" t="n">
         <v>0</v>
@@ -3985,7 +4045,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>MORALES CAIZA SERGIO IVAN</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
@@ -3995,7 +4055,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>367.8</v>
+        <v>238.35</v>
       </c>
       <c r="F32" s="2" t="n">
         <v>0</v>
@@ -4012,17 +4072,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
-        <v>159.03</v>
+        <v>0</v>
       </c>
       <c r="D33" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="F33" s="2" t="n">
         <v>0</v>
@@ -4039,11 +4099,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>PAREDES POVEDA TATIANA VERONICA</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
-        <v>0</v>
+        <v>159.03</v>
       </c>
       <c r="D34" s="2" t="n">
         <v>0</v>
@@ -4066,14 +4126,14 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>413.5</v>
+        <v>0</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>0</v>
@@ -4093,14 +4153,14 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>0</v>
+        <v>413.5</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>0</v>
@@ -4120,14 +4180,14 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>43.86</v>
+        <v>0</v>
       </c>
       <c r="E37" s="2" t="n">
         <v>0</v>
@@ -4147,20 +4207,20 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>0</v>
+        <v>43.86</v>
       </c>
       <c r="E38" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>3692.91</v>
+        <v>0</v>
       </c>
       <c r="G38" s="2" t="n">
         <v>0</v>
@@ -4174,11 +4234,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="D39" s="2" t="n">
         <v>0</v>
@@ -4187,7 +4247,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>0</v>
+        <v>3692.91</v>
       </c>
       <c r="G39" s="2" t="n">
         <v>0</v>
@@ -4201,20 +4261,20 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>565.27</v>
+        <v>0</v>
       </c>
       <c r="E40" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>522.8200000000001</v>
+        <v>0</v>
       </c>
       <c r="G40" s="2" t="n">
         <v>0</v>
@@ -4228,20 +4288,20 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+          <t>VEHINVER SA</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D41" s="2" t="n">
-        <v>0</v>
+        <v>565.27</v>
       </c>
       <c r="E41" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>0</v>
+        <v>522.8200000000001</v>
       </c>
       <c r="G41" s="2" t="n">
         <v>0</v>
@@ -4255,39 +4315,66 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="2" t="n">
+      <c r="C43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="2" t="n">
         <v>346.56</v>
       </c>
-      <c r="G42" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="C43" s="4" t="n">
+      <c r="G43" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="C44" s="4" t="n">
         <v>2074.69</v>
       </c>
-      <c r="D43" s="4" t="n">
+      <c r="D44" s="4" t="n">
         <v>2652.23</v>
       </c>
-      <c r="E43" s="4" t="n">
+      <c r="E44" s="4" t="n">
         <v>1566.5</v>
       </c>
-      <c r="F43" s="4" t="n">
+      <c r="F44" s="4" t="n">
         <v>9620.279999999999</v>
       </c>
-      <c r="G43" s="4" t="n">
+      <c r="G44" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-09-22 16:40:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R45"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>LOAIZA TINOCO JUAN PABLO</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
@@ -2308,7 +2308,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
@@ -2368,7 +2368,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>MORALES CAIZA SERGIO IVAN</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
@@ -2548,7 +2548,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>PALMA PICO OSCAR FILIDEL</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
@@ -2608,7 +2608,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>PAREDES POVEDA TATIANA VERONICA</t>
+          <t>PALMA PICO OSCAR FILIDEL</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
@@ -2848,7 +2848,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
@@ -2879,10 +2879,10 @@
         <v>0</v>
       </c>
       <c r="L40" s="2" t="n">
-        <v>853.29</v>
+        <v>0</v>
       </c>
       <c r="M40" s="2" t="n">
-        <v>5005.24</v>
+        <v>0</v>
       </c>
       <c r="N40" s="2" t="n">
         <v>0</v>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
@@ -2939,10 +2939,10 @@
         <v>0</v>
       </c>
       <c r="L41" s="2" t="n">
-        <v>0</v>
+        <v>853.29</v>
       </c>
       <c r="M41" s="2" t="n">
-        <v>0</v>
+        <v>5005.24</v>
       </c>
       <c r="N41" s="2" t="n">
         <v>0</v>
@@ -2957,7 +2957,7 @@
         <v>0</v>
       </c>
       <c r="R41" s="2" t="n">
-        <v>-10.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -2968,7 +2968,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
@@ -2978,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>94.20999999999999</v>
+        <v>0</v>
       </c>
       <c r="F42" s="2" t="n">
         <v>0</v>
@@ -3002,7 +3002,7 @@
         <v>0</v>
       </c>
       <c r="M42" s="2" t="n">
-        <v>428.61</v>
+        <v>0</v>
       </c>
       <c r="N42" s="2" t="n">
         <v>0</v>
@@ -3017,7 +3017,7 @@
         <v>0</v>
       </c>
       <c r="R42" s="2" t="n">
-        <v>0</v>
+        <v>-10.44</v>
       </c>
     </row>
     <row r="43">
@@ -3028,7 +3028,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+          <t>VEHINVER SA</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
@@ -3038,7 +3038,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>0</v>
+        <v>94.20999999999999</v>
       </c>
       <c r="F43" s="2" t="n">
         <v>0</v>
@@ -3062,7 +3062,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="2" t="n">
-        <v>0</v>
+        <v>428.61</v>
       </c>
       <c r="N43" s="2" t="n">
         <v>0</v>
@@ -3088,137 +3088,197 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R44" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L44" s="2" t="n">
+      <c r="C45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" s="2" t="n">
         <v>346.56</v>
       </c>
-      <c r="M44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R44" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="C45" s="3" t="inlineStr">
-        <is>
-          <t>0 de 43</t>
-        </is>
-      </c>
-      <c r="D45" s="3" t="inlineStr">
-        <is>
-          <t>2 de 43</t>
-        </is>
-      </c>
-      <c r="E45" s="3" t="inlineStr">
-        <is>
-          <t>1 de 43</t>
-        </is>
-      </c>
-      <c r="F45" s="3" t="inlineStr">
-        <is>
-          <t>0 de 43</t>
-        </is>
-      </c>
-      <c r="G45" s="3" t="inlineStr">
-        <is>
-          <t>0 de 43</t>
-        </is>
-      </c>
-      <c r="H45" s="3" t="inlineStr">
-        <is>
-          <t>0 de 43</t>
-        </is>
-      </c>
-      <c r="I45" s="3" t="inlineStr">
-        <is>
-          <t>0 de 43</t>
-        </is>
-      </c>
-      <c r="J45" s="3" t="inlineStr">
-        <is>
-          <t>0 de 43</t>
-        </is>
-      </c>
-      <c r="K45" s="3" t="inlineStr">
-        <is>
-          <t>0 de 43</t>
-        </is>
-      </c>
-      <c r="L45" s="3" t="inlineStr">
-        <is>
-          <t>6 de 43</t>
-        </is>
-      </c>
-      <c r="M45" s="3" t="inlineStr">
-        <is>
-          <t>3 de 43</t>
-        </is>
-      </c>
-      <c r="N45" s="3" t="inlineStr">
-        <is>
-          <t>0 de 43</t>
-        </is>
-      </c>
-      <c r="O45" s="3" t="inlineStr">
-        <is>
-          <t>0 de 43</t>
-        </is>
-      </c>
-      <c r="P45" s="3" t="inlineStr">
-        <is>
-          <t>0 de 43</t>
-        </is>
-      </c>
-      <c r="Q45" s="3" t="inlineStr">
-        <is>
-          <t>0 de 43</t>
-        </is>
-      </c>
-      <c r="R45" s="3" t="inlineStr">
-        <is>
-          <t>0 de 43</t>
+      <c r="M45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R45" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="C46" s="3" t="inlineStr">
+        <is>
+          <t>0 de 44</t>
+        </is>
+      </c>
+      <c r="D46" s="3" t="inlineStr">
+        <is>
+          <t>2 de 44</t>
+        </is>
+      </c>
+      <c r="E46" s="3" t="inlineStr">
+        <is>
+          <t>1 de 44</t>
+        </is>
+      </c>
+      <c r="F46" s="3" t="inlineStr">
+        <is>
+          <t>0 de 44</t>
+        </is>
+      </c>
+      <c r="G46" s="3" t="inlineStr">
+        <is>
+          <t>0 de 44</t>
+        </is>
+      </c>
+      <c r="H46" s="3" t="inlineStr">
+        <is>
+          <t>0 de 44</t>
+        </is>
+      </c>
+      <c r="I46" s="3" t="inlineStr">
+        <is>
+          <t>0 de 44</t>
+        </is>
+      </c>
+      <c r="J46" s="3" t="inlineStr">
+        <is>
+          <t>0 de 44</t>
+        </is>
+      </c>
+      <c r="K46" s="3" t="inlineStr">
+        <is>
+          <t>0 de 44</t>
+        </is>
+      </c>
+      <c r="L46" s="3" t="inlineStr">
+        <is>
+          <t>6 de 44</t>
+        </is>
+      </c>
+      <c r="M46" s="3" t="inlineStr">
+        <is>
+          <t>3 de 44</t>
+        </is>
+      </c>
+      <c r="N46" s="3" t="inlineStr">
+        <is>
+          <t>0 de 44</t>
+        </is>
+      </c>
+      <c r="O46" s="3" t="inlineStr">
+        <is>
+          <t>0 de 44</t>
+        </is>
+      </c>
+      <c r="P46" s="3" t="inlineStr">
+        <is>
+          <t>0 de 44</t>
+        </is>
+      </c>
+      <c r="Q46" s="3" t="inlineStr">
+        <is>
+          <t>0 de 44</t>
+        </is>
+      </c>
+      <c r="R46" s="3" t="inlineStr">
+        <is>
+          <t>0 de 44</t>
         </is>
       </c>
     </row>
@@ -3233,7 +3293,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3997,11 +4057,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>LOAIZA TINOCO JUAN PABLO</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="D28" s="2" t="n">
         <v>0</v>
@@ -4024,11 +4084,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="D29" s="2" t="n">
         <v>0</v>
@@ -4051,14 +4111,14 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="E30" s="2" t="n">
         <v>0</v>
@@ -4078,14 +4138,14 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>308.08</v>
+        <v>238.35</v>
       </c>
       <c r="E31" s="2" t="n">
         <v>0</v>
@@ -4105,17 +4165,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>0</v>
+        <v>308.08</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="F32" s="2" t="n">
         <v>0</v>
@@ -4132,7 +4192,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>MORALES CAIZA SERGIO IVAN</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
@@ -4142,7 +4202,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>367.8</v>
+        <v>238.35</v>
       </c>
       <c r="F33" s="2" t="n">
         <v>0</v>
@@ -4159,17 +4219,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
-        <v>159.03</v>
+        <v>0</v>
       </c>
       <c r="D34" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="F34" s="2" t="n">
         <v>0</v>
@@ -4186,11 +4246,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>PALMA PICO OSCAR FILIDEL</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
-        <v>0</v>
+        <v>159.03</v>
       </c>
       <c r="D35" s="2" t="n">
         <v>0</v>
@@ -4213,7 +4273,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>PAREDES POVEDA TATIANA VERONICA</t>
+          <t>PALMA PICO OSCAR FILIDEL</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
@@ -4240,14 +4300,14 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>413.5</v>
+        <v>0</v>
       </c>
       <c r="E37" s="2" t="n">
         <v>0</v>
@@ -4267,14 +4327,14 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>0</v>
+        <v>413.5</v>
       </c>
       <c r="E38" s="2" t="n">
         <v>0</v>
@@ -4294,14 +4354,14 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>43.86</v>
+        <v>0</v>
       </c>
       <c r="E39" s="2" t="n">
         <v>0</v>
@@ -4321,20 +4381,20 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>0</v>
+        <v>43.86</v>
       </c>
       <c r="E40" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>5858.53</v>
+        <v>0</v>
       </c>
       <c r="G40" s="2" t="n">
         <v>0</v>
@@ -4348,11 +4408,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="D41" s="2" t="n">
         <v>0</v>
@@ -4361,7 +4421,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>-10.44</v>
+        <v>5858.53</v>
       </c>
       <c r="G41" s="2" t="n">
         <v>0</v>
@@ -4375,20 +4435,20 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>565.27</v>
+        <v>0</v>
       </c>
       <c r="E42" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>522.8200000000001</v>
+        <v>-10.44</v>
       </c>
       <c r="G42" s="2" t="n">
         <v>0</v>
@@ -4402,20 +4462,20 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+          <t>VEHINVER SA</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>0</v>
+        <v>565.27</v>
       </c>
       <c r="E43" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>0</v>
+        <v>522.8200000000001</v>
       </c>
       <c r="G43" s="2" t="n">
         <v>0</v>
@@ -4429,39 +4489,66 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" s="2" t="n">
+      <c r="C45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="2" t="n">
         <v>346.56</v>
       </c>
-      <c r="G44" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="C45" s="4" t="n">
+      <c r="G45" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="C46" s="4" t="n">
         <v>2074.69</v>
       </c>
-      <c r="D45" s="4" t="n">
+      <c r="D46" s="4" t="n">
         <v>2652.23</v>
       </c>
-      <c r="E45" s="4" t="n">
+      <c r="E46" s="4" t="n">
         <v>1566.5</v>
       </c>
-      <c r="F45" s="4" t="n">
+      <c r="F46" s="4" t="n">
         <v>12441.86</v>
       </c>
-      <c r="G45" s="4" t="n">
+      <c r="G46" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-09-23 09:00:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2159,7 +2159,7 @@
         <v>0</v>
       </c>
       <c r="L28" s="2" t="n">
-        <v>0</v>
+        <v>551.71</v>
       </c>
       <c r="M28" s="2" t="n">
         <v>0</v>
@@ -3248,7 +3248,7 @@
       </c>
       <c r="L46" s="3" t="inlineStr">
         <is>
-          <t>6 de 44</t>
+          <t>7 de 44</t>
         </is>
       </c>
       <c r="M46" s="3" t="inlineStr">
@@ -4070,7 +4070,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>0</v>
+        <v>551.71</v>
       </c>
       <c r="G28" s="2" t="n">
         <v>0</v>
@@ -4546,7 +4546,7 @@
         <v>1566.5</v>
       </c>
       <c r="F46" s="4" t="n">
-        <v>12441.86</v>
+        <v>12993.57</v>
       </c>
       <c r="G46" s="4" t="n">
         <v>0</v>
@@ -4626,10 +4626,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>8761.92</v>
+        <v>9313.629999999999</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-8761.92</v>
+        <v>-9313.629999999999</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -4669,13 +4669,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>20313.81</v>
+        <v>20865.52</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-313.8099999999995</v>
+        <v>-865.5199999999986</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>1.0156905</v>
+        <v>1.043276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-23 14:40:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:R47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
+          <t>RAMIREZ MOREIRA MAYRA JACQUELINE</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
@@ -2848,7 +2848,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
@@ -2908,7 +2908,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
@@ -2939,10 +2939,10 @@
         <v>0</v>
       </c>
       <c r="L41" s="2" t="n">
-        <v>853.29</v>
+        <v>0</v>
       </c>
       <c r="M41" s="2" t="n">
-        <v>5005.24</v>
+        <v>0</v>
       </c>
       <c r="N41" s="2" t="n">
         <v>0</v>
@@ -2968,7 +2968,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
@@ -2999,10 +2999,10 @@
         <v>0</v>
       </c>
       <c r="L42" s="2" t="n">
-        <v>0</v>
+        <v>853.29</v>
       </c>
       <c r="M42" s="2" t="n">
-        <v>0</v>
+        <v>5005.24</v>
       </c>
       <c r="N42" s="2" t="n">
         <v>0</v>
@@ -3017,7 +3017,7 @@
         <v>0</v>
       </c>
       <c r="R42" s="2" t="n">
-        <v>-10.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -3028,7 +3028,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
@@ -3038,7 +3038,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>94.20999999999999</v>
+        <v>0</v>
       </c>
       <c r="F43" s="2" t="n">
         <v>0</v>
@@ -3062,7 +3062,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="2" t="n">
-        <v>428.61</v>
+        <v>0</v>
       </c>
       <c r="N43" s="2" t="n">
         <v>0</v>
@@ -3077,7 +3077,7 @@
         <v>0</v>
       </c>
       <c r="R43" s="2" t="n">
-        <v>0</v>
+        <v>-10.44</v>
       </c>
     </row>
     <row r="44">
@@ -3088,7 +3088,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+          <t>VEHINVER SA</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
@@ -3098,7 +3098,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>0</v>
+        <v>94.20999999999999</v>
       </c>
       <c r="F44" s="2" t="n">
         <v>0</v>
@@ -3122,7 +3122,7 @@
         <v>0</v>
       </c>
       <c r="M44" s="2" t="n">
-        <v>0</v>
+        <v>428.61</v>
       </c>
       <c r="N44" s="2" t="n">
         <v>0</v>
@@ -3148,137 +3148,197 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R45" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L45" s="2" t="n">
+      <c r="C46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" s="2" t="n">
         <v>346.56</v>
       </c>
-      <c r="M45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R45" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="C46" s="3" t="inlineStr">
-        <is>
-          <t>0 de 44</t>
-        </is>
-      </c>
-      <c r="D46" s="3" t="inlineStr">
-        <is>
-          <t>2 de 44</t>
-        </is>
-      </c>
-      <c r="E46" s="3" t="inlineStr">
-        <is>
-          <t>1 de 44</t>
-        </is>
-      </c>
-      <c r="F46" s="3" t="inlineStr">
-        <is>
-          <t>0 de 44</t>
-        </is>
-      </c>
-      <c r="G46" s="3" t="inlineStr">
-        <is>
-          <t>0 de 44</t>
-        </is>
-      </c>
-      <c r="H46" s="3" t="inlineStr">
-        <is>
-          <t>0 de 44</t>
-        </is>
-      </c>
-      <c r="I46" s="3" t="inlineStr">
-        <is>
-          <t>0 de 44</t>
-        </is>
-      </c>
-      <c r="J46" s="3" t="inlineStr">
-        <is>
-          <t>0 de 44</t>
-        </is>
-      </c>
-      <c r="K46" s="3" t="inlineStr">
-        <is>
-          <t>0 de 44</t>
-        </is>
-      </c>
-      <c r="L46" s="3" t="inlineStr">
-        <is>
-          <t>7 de 44</t>
-        </is>
-      </c>
-      <c r="M46" s="3" t="inlineStr">
-        <is>
-          <t>3 de 44</t>
-        </is>
-      </c>
-      <c r="N46" s="3" t="inlineStr">
-        <is>
-          <t>0 de 44</t>
-        </is>
-      </c>
-      <c r="O46" s="3" t="inlineStr">
-        <is>
-          <t>0 de 44</t>
-        </is>
-      </c>
-      <c r="P46" s="3" t="inlineStr">
-        <is>
-          <t>0 de 44</t>
-        </is>
-      </c>
-      <c r="Q46" s="3" t="inlineStr">
-        <is>
-          <t>0 de 44</t>
-        </is>
-      </c>
-      <c r="R46" s="3" t="inlineStr">
-        <is>
-          <t>0 de 44</t>
+      <c r="M46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R46" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="C47" s="3" t="inlineStr">
+        <is>
+          <t>0 de 45</t>
+        </is>
+      </c>
+      <c r="D47" s="3" t="inlineStr">
+        <is>
+          <t>2 de 45</t>
+        </is>
+      </c>
+      <c r="E47" s="3" t="inlineStr">
+        <is>
+          <t>1 de 45</t>
+        </is>
+      </c>
+      <c r="F47" s="3" t="inlineStr">
+        <is>
+          <t>0 de 45</t>
+        </is>
+      </c>
+      <c r="G47" s="3" t="inlineStr">
+        <is>
+          <t>0 de 45</t>
+        </is>
+      </c>
+      <c r="H47" s="3" t="inlineStr">
+        <is>
+          <t>0 de 45</t>
+        </is>
+      </c>
+      <c r="I47" s="3" t="inlineStr">
+        <is>
+          <t>0 de 45</t>
+        </is>
+      </c>
+      <c r="J47" s="3" t="inlineStr">
+        <is>
+          <t>0 de 45</t>
+        </is>
+      </c>
+      <c r="K47" s="3" t="inlineStr">
+        <is>
+          <t>0 de 45</t>
+        </is>
+      </c>
+      <c r="L47" s="3" t="inlineStr">
+        <is>
+          <t>7 de 45</t>
+        </is>
+      </c>
+      <c r="M47" s="3" t="inlineStr">
+        <is>
+          <t>3 de 45</t>
+        </is>
+      </c>
+      <c r="N47" s="3" t="inlineStr">
+        <is>
+          <t>0 de 45</t>
+        </is>
+      </c>
+      <c r="O47" s="3" t="inlineStr">
+        <is>
+          <t>0 de 45</t>
+        </is>
+      </c>
+      <c r="P47" s="3" t="inlineStr">
+        <is>
+          <t>0 de 45</t>
+        </is>
+      </c>
+      <c r="Q47" s="3" t="inlineStr">
+        <is>
+          <t>0 de 45</t>
+        </is>
+      </c>
+      <c r="R47" s="3" t="inlineStr">
+        <is>
+          <t>0 de 45</t>
         </is>
       </c>
     </row>
@@ -3293,7 +3353,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4354,7 +4414,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
+          <t>RAMIREZ MOREIRA MAYRA JACQUELINE</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
@@ -4381,14 +4441,14 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>43.86</v>
+        <v>0</v>
       </c>
       <c r="E40" s="2" t="n">
         <v>0</v>
@@ -4408,20 +4468,20 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D41" s="2" t="n">
-        <v>0</v>
+        <v>43.86</v>
       </c>
       <c r="E41" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>5858.53</v>
+        <v>0</v>
       </c>
       <c r="G41" s="2" t="n">
         <v>0</v>
@@ -4435,11 +4495,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="D42" s="2" t="n">
         <v>0</v>
@@ -4448,7 +4508,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>-10.44</v>
+        <v>5858.53</v>
       </c>
       <c r="G42" s="2" t="n">
         <v>0</v>
@@ -4462,20 +4522,20 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
-        <v>0</v>
+        <v>10.44</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>565.27</v>
+        <v>0</v>
       </c>
       <c r="E43" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>522.8200000000001</v>
+        <v>-10.44</v>
       </c>
       <c r="G43" s="2" t="n">
         <v>0</v>
@@ -4489,20 +4549,20 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+          <t>VEHINVER SA</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>0</v>
+        <v>565.27</v>
       </c>
       <c r="E44" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>0</v>
+        <v>522.8200000000001</v>
       </c>
       <c r="G44" s="2" t="n">
         <v>0</v>
@@ -4516,39 +4576,66 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" s="2" t="n">
+      <c r="C46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="2" t="n">
         <v>346.56</v>
       </c>
-      <c r="G45" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="C46" s="4" t="n">
+      <c r="G46" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="C47" s="4" t="n">
         <v>2074.69</v>
       </c>
-      <c r="D46" s="4" t="n">
+      <c r="D47" s="4" t="n">
         <v>2652.23</v>
       </c>
-      <c r="E46" s="4" t="n">
+      <c r="E47" s="4" t="n">
         <v>1566.5</v>
       </c>
-      <c r="F46" s="4" t="n">
+      <c r="F47" s="4" t="n">
         <v>12993.57</v>
       </c>
-      <c r="G46" s="4" t="n">
+      <c r="G47" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-09-24 09:50:10
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2639,7 +2639,7 @@
         <v>0</v>
       </c>
       <c r="L36" s="2" t="n">
-        <v>0</v>
+        <v>115.52</v>
       </c>
       <c r="M36" s="2" t="n">
         <v>0</v>
@@ -3308,7 +3308,7 @@
       </c>
       <c r="L47" s="3" t="inlineStr">
         <is>
-          <t>7 de 45</t>
+          <t>8 de 45</t>
         </is>
       </c>
       <c r="M47" s="3" t="inlineStr">
@@ -4346,7 +4346,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>0</v>
+        <v>115.52</v>
       </c>
       <c r="G36" s="2" t="n">
         <v>0</v>
@@ -4633,7 +4633,7 @@
         <v>1566.5</v>
       </c>
       <c r="F47" s="4" t="n">
-        <v>13038.36</v>
+        <v>13153.88</v>
       </c>
       <c r="G47" s="4" t="n">
         <v>0</v>
@@ -4713,10 +4713,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>9358.42</v>
+        <v>9473.940000000001</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-9358.42</v>
+        <v>-9473.940000000001</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -4756,13 +4756,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>20910.31</v>
+        <v>21025.83</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-910.3099999999995</v>
+        <v>-1025.83</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>1.0455155</v>
+        <v>1.0512915</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-26 09:35:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -4800,10 +4800,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>9473.940000000001</v>
+        <v>9734.82</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-9473.940000000001</v>
+        <v>-9734.82</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -4843,13 +4843,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>21191.66</v>
+        <v>21452.54</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-1191.66</v>
+        <v>-1452.539999999999</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>1.059583</v>
+        <v>1.072627</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-26 14:50:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -4800,10 +4800,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>9734.82</v>
+        <v>10579.81</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-9734.82</v>
+        <v>-10579.81</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -4843,13 +4843,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>21452.54</v>
+        <v>22297.53</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-1452.539999999999</v>
+        <v>-2297.529999999999</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>1.072627</v>
+        <v>1.1148765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-06 17:30:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1022,7 +1022,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>0</v>
+        <v>-22.29</v>
       </c>
       <c r="N9" s="2" t="n">
         <v>0</v>
@@ -3677,7 +3677,7 @@
         <v>3864.45</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0</v>
+        <v>-22.29</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>0</v>
@@ -4720,7 +4720,7 @@
         <v>13412.01</v>
       </c>
       <c r="F48" s="4" t="n">
-        <v>-10.44</v>
+        <v>-32.73</v>
       </c>
       <c r="G48" s="4" t="n">
         <v>0</v>
@@ -4824,13 +4824,13 @@
         <v>20000</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>20.74</v>
+        <v>15.17</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>19979.26</v>
+        <v>19984.83</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.001037</v>
+        <v>0.0007585</v>
       </c>
     </row>
     <row r="4">
@@ -4843,13 +4843,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>2659.91</v>
+        <v>2654.34</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>17340.09</v>
+        <v>17345.66</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.1329955</v>
+        <v>0.132717</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-14 12:30:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -5085,13 +5085,13 @@
         <v>20000</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>4471.23</v>
+        <v>5273.13</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>15528.77</v>
+        <v>14726.87</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.2235615</v>
+        <v>0.2636565</v>
       </c>
     </row>
     <row r="4">
@@ -5104,13 +5104,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>7623.889999999999</v>
+        <v>8425.790000000001</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>12376.11</v>
+        <v>11574.21</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.3811945</v>
+        <v>0.4212895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-15 12:30:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R52"/>
+  <dimension ref="A1:R53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>CORREA IGLESIAS RAMIRO MARCELO</t>
+          <t>CORONADO MONTERO LIDA VERONICA</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
+          <t>CORREA IGLESIAS RAMIRO MARCELO</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>GARCES MORALES ANA CRISTINA</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -1802,7 +1802,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="2" t="n">
-        <v>56.02</v>
+        <v>0</v>
       </c>
       <c r="N22" s="2" t="n">
         <v>0</v>
@@ -1828,7 +1828,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>GARCIA BRAVO JOSE LUIS</t>
+          <t>GARCES MORALES ANA CRISTINA</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -1862,7 +1862,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="2" t="n">
-        <v>0</v>
+        <v>56.02</v>
       </c>
       <c r="N23" s="2" t="n">
         <v>0</v>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>GAVILANES VELEZ MARIA VALERIA</t>
+          <t>GARCIA BRAVO JOSE LUIS</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>GRANJA VANEGAS MARCELA</t>
+          <t>GAVILANES VELEZ MARIA VALERIA</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -2008,7 +2008,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>GRANJA VANEGAS MARCELA</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>KITCHENSCO S.A.</t>
+          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+          <t>KITCHENSCO S.A.</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>LOAIZA TINOCO JUAN PABLO</t>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
@@ -2308,7 +2308,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>LOAIZA TINOCO JUAN PABLO</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
@@ -2342,7 +2342,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="2" t="n">
-        <v>-156.04</v>
+        <v>0</v>
       </c>
       <c r="N31" s="2" t="n">
         <v>0</v>
@@ -2357,7 +2357,7 @@
         <v>0</v>
       </c>
       <c r="R31" s="2" t="n">
-        <v>-10.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -2368,7 +2368,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
@@ -2402,7 +2402,7 @@
         <v>0</v>
       </c>
       <c r="M32" s="2" t="n">
-        <v>0</v>
+        <v>-156.04</v>
       </c>
       <c r="N32" s="2" t="n">
         <v>0</v>
@@ -2417,7 +2417,7 @@
         <v>0</v>
       </c>
       <c r="R32" s="2" t="n">
-        <v>0</v>
+        <v>-10.44</v>
       </c>
     </row>
     <row r="33">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
@@ -2548,7 +2548,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
@@ -2608,7 +2608,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>MORALES CAIZA SERGIO IVAN</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>PALMA PICO OSCAR FILIDEL</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
@@ -2759,7 +2759,7 @@
         <v>0</v>
       </c>
       <c r="L38" s="2" t="n">
-        <v>179.12</v>
+        <v>0</v>
       </c>
       <c r="M38" s="2" t="n">
         <v>0</v>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>PAREDES POVEDA TATIANA VERONICA</t>
+          <t>PALMA PICO OSCAR FILIDEL</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
@@ -2819,7 +2819,7 @@
         <v>0</v>
       </c>
       <c r="L39" s="2" t="n">
-        <v>0</v>
+        <v>179.12</v>
       </c>
       <c r="M39" s="2" t="n">
         <v>0</v>
@@ -2848,7 +2848,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
@@ -2908,7 +2908,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>RAMIREZ MOREIRA MAYRA JACQUELINE</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
@@ -2968,14 +2968,14 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ROSHANN</t>
+          <t>RAMIREZ MOREIRA MAYRA JACQUELINE</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>194.16</v>
+        <v>0</v>
       </c>
       <c r="E42" s="2" t="n">
         <v>0</v>
@@ -3028,14 +3028,14 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
+          <t>ROSHANN</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>0</v>
+        <v>194.16</v>
       </c>
       <c r="E43" s="2" t="n">
         <v>0</v>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
@@ -3148,7 +3148,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
@@ -3208,11 +3208,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>TORRES CADENA JAVIER JOSUE</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
-        <v>334.37</v>
+        <v>0</v>
       </c>
       <c r="D46" s="2" t="n">
         <v>0</v>
@@ -3268,11 +3268,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>TORRES CADENA JAVIER JOSUE</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
-        <v>0</v>
+        <v>334.37</v>
       </c>
       <c r="D47" s="2" t="n">
         <v>0</v>
@@ -3328,7 +3328,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>VERA TREJO JUAN CARLOS</t>
+          <t>VEHINVER SA</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
@@ -3448,7 +3448,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+          <t>VERA TREJO JUAN CARLOS</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
@@ -3508,137 +3508,197 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R51" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R51" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="C52" s="3" t="inlineStr">
-        <is>
-          <t>1 de 50</t>
-        </is>
-      </c>
-      <c r="D52" s="3" t="inlineStr">
-        <is>
-          <t>1 de 50</t>
-        </is>
-      </c>
-      <c r="E52" s="3" t="inlineStr">
-        <is>
-          <t>0 de 50</t>
-        </is>
-      </c>
-      <c r="F52" s="3" t="inlineStr">
-        <is>
-          <t>0 de 50</t>
-        </is>
-      </c>
-      <c r="G52" s="3" t="inlineStr">
-        <is>
-          <t>0 de 50</t>
-        </is>
-      </c>
-      <c r="H52" s="3" t="inlineStr">
-        <is>
-          <t>0 de 50</t>
-        </is>
-      </c>
-      <c r="I52" s="3" t="inlineStr">
-        <is>
-          <t>0 de 50</t>
-        </is>
-      </c>
-      <c r="J52" s="3" t="inlineStr">
-        <is>
-          <t>0 de 50</t>
-        </is>
-      </c>
-      <c r="K52" s="3" t="inlineStr">
-        <is>
-          <t>0 de 50</t>
-        </is>
-      </c>
-      <c r="L52" s="3" t="inlineStr">
-        <is>
-          <t>1 de 50</t>
-        </is>
-      </c>
-      <c r="M52" s="3" t="inlineStr">
-        <is>
-          <t>1 de 50</t>
-        </is>
-      </c>
-      <c r="N52" s="3" t="inlineStr">
-        <is>
-          <t>0 de 50</t>
-        </is>
-      </c>
-      <c r="O52" s="3" t="inlineStr">
-        <is>
-          <t>0 de 50</t>
-        </is>
-      </c>
-      <c r="P52" s="3" t="inlineStr">
-        <is>
-          <t>0 de 50</t>
-        </is>
-      </c>
-      <c r="Q52" s="3" t="inlineStr">
-        <is>
-          <t>0 de 50</t>
-        </is>
-      </c>
-      <c r="R52" s="3" t="inlineStr">
-        <is>
-          <t>0 de 50</t>
+      <c r="C52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R52" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="C53" s="3" t="inlineStr">
+        <is>
+          <t>1 de 51</t>
+        </is>
+      </c>
+      <c r="D53" s="3" t="inlineStr">
+        <is>
+          <t>1 de 51</t>
+        </is>
+      </c>
+      <c r="E53" s="3" t="inlineStr">
+        <is>
+          <t>0 de 51</t>
+        </is>
+      </c>
+      <c r="F53" s="3" t="inlineStr">
+        <is>
+          <t>0 de 51</t>
+        </is>
+      </c>
+      <c r="G53" s="3" t="inlineStr">
+        <is>
+          <t>0 de 51</t>
+        </is>
+      </c>
+      <c r="H53" s="3" t="inlineStr">
+        <is>
+          <t>0 de 51</t>
+        </is>
+      </c>
+      <c r="I53" s="3" t="inlineStr">
+        <is>
+          <t>0 de 51</t>
+        </is>
+      </c>
+      <c r="J53" s="3" t="inlineStr">
+        <is>
+          <t>0 de 51</t>
+        </is>
+      </c>
+      <c r="K53" s="3" t="inlineStr">
+        <is>
+          <t>0 de 51</t>
+        </is>
+      </c>
+      <c r="L53" s="3" t="inlineStr">
+        <is>
+          <t>1 de 51</t>
+        </is>
+      </c>
+      <c r="M53" s="3" t="inlineStr">
+        <is>
+          <t>1 de 51</t>
+        </is>
+      </c>
+      <c r="N53" s="3" t="inlineStr">
+        <is>
+          <t>0 de 51</t>
+        </is>
+      </c>
+      <c r="O53" s="3" t="inlineStr">
+        <is>
+          <t>0 de 51</t>
+        </is>
+      </c>
+      <c r="P53" s="3" t="inlineStr">
+        <is>
+          <t>0 de 51</t>
+        </is>
+      </c>
+      <c r="Q53" s="3" t="inlineStr">
+        <is>
+          <t>0 de 51</t>
+        </is>
+      </c>
+      <c r="R53" s="3" t="inlineStr">
+        <is>
+          <t>0 de 51</t>
         </is>
       </c>
     </row>
@@ -3653,7 +3713,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4147,7 +4207,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>CORREA IGLESIAS RAMIRO MARCELO</t>
+          <t>CORONADO MONTERO LIDA VERONICA</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -4174,11 +4234,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
+          <t>CORREA IGLESIAS RAMIRO MARCELO</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>24.39</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="n">
         <v>0</v>
@@ -4201,14 +4261,14 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>EQUISAB S.A.</t>
+          <t>DANIELA ELIZABETH BECERRA BECERRA</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0</v>
+        <v>24.39</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>354.43</v>
+        <v>0</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>0</v>
@@ -4228,14 +4288,14 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
+          <t>EQUISAB S.A.</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>0</v>
+        <v>354.43</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>0</v>
@@ -4255,7 +4315,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>GARCES MORALES ANA CRISTINA</t>
+          <t>FARIAS CAICEDO GABRIELA PATRICIA</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -4268,7 +4328,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>56.02</v>
+        <v>0</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>0</v>
@@ -4282,7 +4342,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>GARCIA BRAVO JOSE LUIS</t>
+          <t>GARCES MORALES ANA CRISTINA</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -4295,7 +4355,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>0</v>
+        <v>56.02</v>
       </c>
       <c r="G23" s="2" t="n">
         <v>0</v>
@@ -4309,7 +4369,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>GAVILANES VELEZ MARIA VALERIA</t>
+          <t>GARCIA BRAVO JOSE LUIS</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -4336,7 +4396,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>GRANJA VANEGAS MARCELA</t>
+          <t>GAVILANES VELEZ MARIA VALERIA</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -4363,11 +4423,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>GRANJA VANEGAS MARCELA</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>367.8</v>
+        <v>0</v>
       </c>
       <c r="D26" s="2" t="n">
         <v>0</v>
@@ -4390,17 +4450,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="D27" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>430.11</v>
+        <v>0</v>
       </c>
       <c r="F27" s="2" t="n">
         <v>0</v>
@@ -4417,7 +4477,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>KITCHENSCO S.A.</t>
+          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -4427,7 +4487,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>0</v>
+        <v>430.11</v>
       </c>
       <c r="F28" s="2" t="n">
         <v>0</v>
@@ -4444,7 +4504,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+          <t>KITCHENSCO S.A.</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
@@ -4471,7 +4531,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>LOAIZA TINOCO JUAN PABLO</t>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
@@ -4481,7 +4541,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>551.71</v>
+        <v>0</v>
       </c>
       <c r="F30" s="2" t="n">
         <v>0</v>
@@ -4498,7 +4558,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>LOAIZA TINOCO JUAN PABLO</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
@@ -4508,10 +4568,10 @@
         <v>0</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>0</v>
+        <v>551.71</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>-166.48</v>
+        <v>0</v>
       </c>
       <c r="G31" s="2" t="n">
         <v>0</v>
@@ -4525,7 +4585,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
@@ -4538,7 +4598,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>0</v>
+        <v>-166.48</v>
       </c>
       <c r="G32" s="2" t="n">
         <v>0</v>
@@ -4552,11 +4612,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="D33" s="2" t="n">
         <v>0</v>
@@ -4579,11 +4639,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
-        <v>308.08</v>
+        <v>238.35</v>
       </c>
       <c r="D34" s="2" t="n">
         <v>0</v>
@@ -4606,14 +4666,14 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
-        <v>0</v>
+        <v>308.08</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>0</v>
@@ -4633,14 +4693,14 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>MORALES CAIZA SERGIO IVAN</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>367.8</v>
+        <v>238.35</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>0</v>
@@ -4660,14 +4720,14 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="E37" s="2" t="n">
         <v>0</v>
@@ -4687,7 +4747,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>PALMA PICO OSCAR FILIDEL</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
@@ -4697,10 +4757,10 @@
         <v>0</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>115.52</v>
+        <v>0</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>179.12</v>
+        <v>0</v>
       </c>
       <c r="G38" s="2" t="n">
         <v>0</v>
@@ -4714,7 +4774,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>PAREDES POVEDA TATIANA VERONICA</t>
+          <t>PALMA PICO OSCAR FILIDEL</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
@@ -4724,10 +4784,10 @@
         <v>0</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>0</v>
+        <v>115.52</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>0</v>
+        <v>179.12</v>
       </c>
       <c r="G39" s="2" t="n">
         <v>0</v>
@@ -4741,11 +4801,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
-        <v>413.5</v>
+        <v>0</v>
       </c>
       <c r="D40" s="2" t="n">
         <v>0</v>
@@ -4768,17 +4828,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>RAMIREZ MOREIRA MAYRA JACQUELINE</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
-        <v>0</v>
+        <v>413.5</v>
       </c>
       <c r="D41" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>44.79</v>
+        <v>0</v>
       </c>
       <c r="F41" s="2" t="n">
         <v>0</v>
@@ -4795,7 +4855,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ROSHANN</t>
+          <t>RAMIREZ MOREIRA MAYRA JACQUELINE</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
@@ -4805,10 +4865,10 @@
         <v>0</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>0</v>
+        <v>44.79</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>194.16</v>
+        <v>0</v>
       </c>
       <c r="G42" s="2" t="n">
         <v>0</v>
@@ -4822,7 +4882,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
+          <t>ROSHANN</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
@@ -4835,7 +4895,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>0</v>
+        <v>194.16</v>
       </c>
       <c r="G43" s="2" t="n">
         <v>0</v>
@@ -4849,11 +4909,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
-        <v>43.86</v>
+        <v>0</v>
       </c>
       <c r="D44" s="2" t="n">
         <v>0</v>
@@ -4876,17 +4936,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
-        <v>0</v>
+        <v>43.86</v>
       </c>
       <c r="D45" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>5858.53</v>
+        <v>0</v>
       </c>
       <c r="F45" s="2" t="n">
         <v>0</v>
@@ -4903,7 +4963,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>TORRES CADENA JAVIER JOSUE</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
@@ -4913,10 +4973,10 @@
         <v>0</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>0</v>
+        <v>5858.53</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>334.37</v>
+        <v>0</v>
       </c>
       <c r="G46" s="2" t="n">
         <v>0</v>
@@ -4930,7 +4990,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>TORRES CADENA JAVIER JOSUE</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
@@ -4940,10 +5000,10 @@
         <v>0</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>-10.44</v>
+        <v>0</v>
       </c>
       <c r="F47" s="2" t="n">
-        <v>0</v>
+        <v>334.37</v>
       </c>
       <c r="G47" s="2" t="n">
         <v>0</v>
@@ -4957,17 +5017,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
-        <v>565.27</v>
+        <v>0</v>
       </c>
       <c r="D48" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>522.8200000000001</v>
+        <v>-10.44</v>
       </c>
       <c r="F48" s="2" t="n">
         <v>0</v>
@@ -4984,17 +5044,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>VERA TREJO JUAN CARLOS</t>
+          <t>VEHINVER SA</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
-        <v>0</v>
+        <v>565.27</v>
       </c>
       <c r="D49" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>165.83</v>
+        <v>522.8200000000001</v>
       </c>
       <c r="F49" s="2" t="n">
         <v>0</v>
@@ -5011,7 +5071,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+          <t>VERA TREJO JUAN CARLOS</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
@@ -5021,7 +5081,7 @@
         <v>0</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>0</v>
+        <v>165.83</v>
       </c>
       <c r="F50" s="2" t="n">
         <v>0</v>
@@ -5038,39 +5098,66 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" s="2" t="n">
+      <c r="C52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="2" t="n">
         <v>438.86</v>
       </c>
-      <c r="F51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G51" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="C52" s="4" t="n">
+      <c r="F52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="C53" s="4" t="n">
         <v>2652.23</v>
       </c>
-      <c r="D52" s="4" t="n">
+      <c r="D53" s="4" t="n">
         <v>1566.5</v>
       </c>
-      <c r="E52" s="4" t="n">
+      <c r="E53" s="4" t="n">
         <v>13412.01</v>
       </c>
-      <c r="F52" s="4" t="n">
+      <c r="F53" s="4" t="n">
         <v>574.9</v>
       </c>
-      <c r="G52" s="4" t="n">
+      <c r="G53" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-10-15 15:30:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -5235,10 +5235,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3346.82</v>
+        <v>3577.86</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-3346.82</v>
+        <v>-3577.86</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -5278,13 +5278,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>8611.43</v>
+        <v>8842.469999999999</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>11388.57</v>
+        <v>11157.53</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.4305715</v>
+        <v>0.4421234999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-15 16:30:10
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -5235,10 +5235,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3577.86</v>
+        <v>3693.38</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-3577.86</v>
+        <v>-3693.38</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -5278,13 +5278,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>8842.469999999999</v>
+        <v>8957.99</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>11157.53</v>
+        <v>11042.01</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.4421234999999999</v>
+        <v>0.4478995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-17 12:30:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -5235,10 +5235,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>6632.5</v>
+        <v>6635.38</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-6632.5</v>
+        <v>-6635.38</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -5278,13 +5278,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>17507.27</v>
+        <v>17510.15</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>2492.73</v>
+        <v>2489.849999999999</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.8753635000000001</v>
+        <v>0.8755075000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-17 16:30:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -5235,10 +5235,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>6635.38</v>
+        <v>6777.58</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-6635.38</v>
+        <v>-6777.58</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -5278,13 +5278,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>17510.15</v>
+        <v>17652.35</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>2489.849999999999</v>
+        <v>2347.65</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.8755075000000001</v>
+        <v>0.8826174999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-23 14:30:10
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -5235,10 +5235,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>7118.92</v>
+        <v>9019.719999999999</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-7118.92</v>
+        <v>-9019.719999999999</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -5278,13 +5278,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>18164.65</v>
+        <v>20065.45</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>1835.35</v>
+        <v>-65.44999999999891</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.9082325000000001</v>
+        <v>1.0032725</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-29 16:30:07
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -5235,10 +5235,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>9105</v>
+        <v>11148.57</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-9105</v>
+        <v>-11148.57</v>
       </c>
       <c r="F2" s="5" t="n">
         <v>0</v>
@@ -5259,13 +5259,13 @@
         <v>20000</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>11045.73</v>
+        <v>11759.66</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>8954.27</v>
+        <v>8240.34</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.5522865</v>
+        <v>0.587983</v>
       </c>
     </row>
     <row r="4">
@@ -5278,13 +5278,13 @@
         <v>20000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>20150.73</v>
+        <v>22908.23</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-150.7299999999996</v>
+        <v>-2908.23</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>1.0075365</v>
+        <v>1.1454115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-11-06 15:30:06
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -3398,7 +3398,7 @@
         <v>0</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>0</v>
+        <v>202.5</v>
       </c>
       <c r="F49" s="2" t="n">
         <v>0</v>
@@ -3422,7 +3422,7 @@
         <v>0</v>
       </c>
       <c r="M49" s="2" t="n">
-        <v>0</v>
+        <v>741.92</v>
       </c>
       <c r="N49" s="2" t="n">
         <v>0</v>
@@ -3633,47 +3633,47 @@
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
+          <t>1 de 51</t>
+        </is>
+      </c>
+      <c r="F53" s="3" t="inlineStr">
+        <is>
           <t>0 de 51</t>
         </is>
       </c>
-      <c r="F53" s="3" t="inlineStr">
+      <c r="G53" s="3" t="inlineStr">
         <is>
           <t>0 de 51</t>
         </is>
       </c>
-      <c r="G53" s="3" t="inlineStr">
+      <c r="H53" s="3" t="inlineStr">
         <is>
           <t>0 de 51</t>
         </is>
       </c>
-      <c r="H53" s="3" t="inlineStr">
+      <c r="I53" s="3" t="inlineStr">
         <is>
           <t>0 de 51</t>
         </is>
       </c>
-      <c r="I53" s="3" t="inlineStr">
+      <c r="J53" s="3" t="inlineStr">
         <is>
           <t>0 de 51</t>
         </is>
       </c>
-      <c r="J53" s="3" t="inlineStr">
+      <c r="K53" s="3" t="inlineStr">
         <is>
           <t>0 de 51</t>
         </is>
       </c>
-      <c r="K53" s="3" t="inlineStr">
+      <c r="L53" s="3" t="inlineStr">
         <is>
           <t>0 de 51</t>
         </is>
       </c>
-      <c r="L53" s="3" t="inlineStr">
-        <is>
-          <t>0 de 51</t>
-        </is>
-      </c>
       <c r="M53" s="3" t="inlineStr">
         <is>
-          <t>0 de 51</t>
+          <t>1 de 51</t>
         </is>
       </c>
       <c r="N53" s="3" t="inlineStr">
@@ -5057,7 +5057,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="2" t="n">
-        <v>0</v>
+        <v>944.42</v>
       </c>
       <c r="G49" s="2" t="n">
         <v>0</v>
@@ -5155,7 +5155,7 @@
         <v>574.9</v>
       </c>
       <c r="F53" s="4" t="n">
-        <v>0</v>
+        <v>944.42</v>
       </c>
       <c r="G53" s="4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Actualización automática 2025-11-14 13:30:10
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -5433,10 +5433,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>3728.12</v>
+        <v>4615</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>-3728.12</v>
+        <v>-4615</v>
       </c>
       <c r="F3" s="5" t="n">
         <v>0</v>
@@ -5476,13 +5476,13 @@
         <v>26086.41</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>12009.35</v>
+        <v>12896.23</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>14077.06</v>
+        <v>13190.18</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>0.4603680613775525</v>
+        <v>0.4943658402976875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-11-14 17:30:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -5457,13 +5457,13 @@
         <v>26000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>8281.23</v>
+        <v>8778.18</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>17718.77</v>
+        <v>17221.82</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.3185088461538461</v>
+        <v>0.3376223076923077</v>
       </c>
     </row>
     <row r="5">
@@ -5476,13 +5476,13 @@
         <v>26086.41</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>12896.23</v>
+        <v>13393.18</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>13190.18</v>
+        <v>12693.23</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>0.4943658402976875</v>
+        <v>0.5134159893983112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-11-24 11:30:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -2999,7 +2999,7 @@
         <v>0</v>
       </c>
       <c r="L42" s="2" t="n">
-        <v>0</v>
+        <v>450.22</v>
       </c>
       <c r="M42" s="2" t="n">
         <v>0</v>
@@ -3968,7 +3968,7 @@
       </c>
       <c r="L58" s="3" t="inlineStr">
         <is>
-          <t>3 de 56</t>
+          <t>4 de 56</t>
         </is>
       </c>
       <c r="M58" s="3" t="inlineStr">
@@ -5168,7 +5168,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>0</v>
+        <v>450.22</v>
       </c>
       <c r="G42" s="2" t="n">
         <v>0</v>
@@ -5590,7 +5590,7 @@
         <v>574.9</v>
       </c>
       <c r="F58" s="4" t="n">
-        <v>5493.93</v>
+        <v>5944.15</v>
       </c>
       <c r="G58" s="4" t="n">
         <v>0</v>
@@ -5694,10 +5694,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>8039.94</v>
+        <v>8490.16</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>-8039.94</v>
+        <v>-8490.16</v>
       </c>
       <c r="F3" s="5" t="n">
         <v>0</v>
@@ -5737,13 +5737,13 @@
         <v>26086.41</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>19027.07</v>
+        <v>19477.29</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>7059.340000000001</v>
+        <v>6609.120000000001</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>0.7293862973095953</v>
+        <v>0.7466450922146819</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-11-26 09:30:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -5694,10 +5694,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>8515.360000000001</v>
+        <v>8657.92</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>-8515.360000000001</v>
+        <v>-8657.92</v>
       </c>
       <c r="F3" s="5" t="n">
         <v>0</v>
@@ -5737,13 +5737,13 @@
         <v>26086.41</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>24087.84</v>
+        <v>24230.4</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>1998.57</v>
+        <v>1856.01</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>0.9233865449481167</v>
+        <v>0.9288514594380752</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-11-26 11:30:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1727,10 +1727,10 @@
         <v>0</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>495</v>
+        <v>802.8</v>
       </c>
       <c r="I21" s="2" t="n">
-        <v>553.73</v>
+        <v>682.95</v>
       </c>
       <c r="J21" s="2" t="n">
         <v>0</v>
@@ -4601,7 +4601,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>3257.68</v>
+        <v>3694.7</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>0</v>
@@ -5590,7 +5590,7 @@
         <v>574.9</v>
       </c>
       <c r="F58" s="4" t="n">
-        <v>5969.349999999999</v>
+        <v>6406.37</v>
       </c>
       <c r="G58" s="4" t="n">
         <v>0</v>
@@ -5694,10 +5694,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>8657.92</v>
+        <v>9094.940000000001</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>-8657.92</v>
+        <v>-9094.940000000001</v>
       </c>
       <c r="F3" s="5" t="n">
         <v>0</v>
@@ -5737,13 +5737,13 @@
         <v>26086.41</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>24230.4</v>
+        <v>24667.42</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>1856.01</v>
+        <v>1418.99</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>0.9288514594380752</v>
+        <v>0.9456042437422397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-11-26 16:30:11
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R57"/>
+  <dimension ref="A1:R58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2068,7 +2068,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>JAIME COELLO ALBERTO FERNANDO</t>
+          <t>GUERRERO GARCIA OLIMPIA ANNABELLE</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>JAIME COELLO ALBERTO FERNANDO</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>KITCHENSCO S.A.</t>
+          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
@@ -2308,7 +2308,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+          <t>KITCHENSCO S.A.</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
@@ -2368,7 +2368,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>LINDAO RODRIGUEZ ANTONIO COLON</t>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
@@ -2399,7 +2399,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="2" t="n">
-        <v>190.68</v>
+        <v>0</v>
       </c>
       <c r="M32" s="2" t="n">
         <v>0</v>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>LOAIZA TINOCO JUAN PABLO</t>
+          <t>LINDAO RODRIGUEZ ANTONIO COLON</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
@@ -2459,7 +2459,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="2" t="n">
-        <v>0</v>
+        <v>190.68</v>
       </c>
       <c r="M33" s="2" t="n">
         <v>0</v>
@@ -2488,7 +2488,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>LOAIZA TINOCO JUAN PABLO</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
@@ -2548,7 +2548,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
@@ -2608,7 +2608,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>MORALES CAIZA SERGIO IVAN</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
@@ -2848,7 +2848,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
@@ -2908,7 +2908,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>MUÑOZ CALDERON JUAN ADOLFO</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
@@ -2939,7 +2939,7 @@
         <v>0</v>
       </c>
       <c r="L41" s="2" t="n">
-        <v>450.22</v>
+        <v>0</v>
       </c>
       <c r="M41" s="2" t="n">
         <v>0</v>
@@ -2968,7 +2968,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>PALMA PICO OSCAR FILIDEL</t>
+          <t>MUÑOZ CALDERON JUAN ADOLFO</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
@@ -2999,7 +2999,7 @@
         <v>0</v>
       </c>
       <c r="L42" s="2" t="n">
-        <v>517.0599999999999</v>
+        <v>450.22</v>
       </c>
       <c r="M42" s="2" t="n">
         <v>0</v>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>PAREDES POVEDA TATIANA VERONICA</t>
+          <t>PALMA PICO OSCAR FILIDEL</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
@@ -3059,7 +3059,7 @@
         <v>0</v>
       </c>
       <c r="L43" s="2" t="n">
-        <v>0</v>
+        <v>517.0599999999999</v>
       </c>
       <c r="M43" s="2" t="n">
         <v>0</v>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>PERDOMO BRIONES JOSÉ ALBERTO</t>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
@@ -3098,7 +3098,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>89.67</v>
+        <v>0</v>
       </c>
       <c r="F44" s="2" t="n">
         <v>0</v>
@@ -3119,7 +3119,7 @@
         <v>0</v>
       </c>
       <c r="L44" s="2" t="n">
-        <v>413.48</v>
+        <v>0</v>
       </c>
       <c r="M44" s="2" t="n">
         <v>0</v>
@@ -3148,7 +3148,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>PERDOMO BRIONES JOSÉ ALBERTO</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
@@ -3158,7 +3158,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>0</v>
+        <v>89.67</v>
       </c>
       <c r="F45" s="2" t="n">
         <v>0</v>
@@ -3179,7 +3179,7 @@
         <v>0</v>
       </c>
       <c r="L45" s="2" t="n">
-        <v>0</v>
+        <v>413.48</v>
       </c>
       <c r="M45" s="2" t="n">
         <v>0</v>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>RAMIREZ MOREIRA MAYRA JACQUELINE</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
@@ -3268,7 +3268,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ROSHANN</t>
+          <t>RAMIREZ MOREIRA MAYRA JACQUELINE</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
@@ -3328,7 +3328,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
+          <t>ROSHANN</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
@@ -3448,7 +3448,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
@@ -3508,7 +3508,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>TORRES CADENA JAVIER JOSUE</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C51" s="2" t="n">
@@ -3568,7 +3568,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>TORRES CADENA JAVIER JOSUE</t>
         </is>
       </c>
       <c r="C52" s="2" t="n">
@@ -3628,7 +3628,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
       <c r="C53" s="2" t="n">
@@ -3638,7 +3638,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>202.5</v>
+        <v>0</v>
       </c>
       <c r="F53" s="2" t="n">
         <v>0</v>
@@ -3662,7 +3662,7 @@
         <v>0</v>
       </c>
       <c r="M53" s="2" t="n">
-        <v>741.92</v>
+        <v>0</v>
       </c>
       <c r="N53" s="2" t="n">
         <v>0</v>
@@ -3688,7 +3688,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>VERA TREJO JUAN CARLOS</t>
+          <t>VEHINVER SA</t>
         </is>
       </c>
       <c r="C54" s="2" t="n">
@@ -3698,7 +3698,7 @@
         <v>0</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>0</v>
+        <v>202.5</v>
       </c>
       <c r="F54" s="2" t="n">
         <v>0</v>
@@ -3722,7 +3722,7 @@
         <v>0</v>
       </c>
       <c r="M54" s="2" t="n">
-        <v>0</v>
+        <v>741.92</v>
       </c>
       <c r="N54" s="2" t="n">
         <v>0</v>
@@ -3748,7 +3748,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+          <t>VERA TREJO JUAN CARLOS</t>
         </is>
       </c>
       <c r="C55" s="2" t="n">
@@ -3808,137 +3808,197 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R56" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R56" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="C57" s="3" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="D57" s="3" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="E57" s="3" t="inlineStr">
-        <is>
-          <t>2 de 55</t>
-        </is>
-      </c>
-      <c r="F57" s="3" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="G57" s="3" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="H57" s="3" t="inlineStr">
-        <is>
-          <t>1 de 55</t>
-        </is>
-      </c>
-      <c r="I57" s="3" t="inlineStr">
-        <is>
-          <t>1 de 55</t>
-        </is>
-      </c>
-      <c r="J57" s="3" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="K57" s="3" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="L57" s="3" t="inlineStr">
-        <is>
-          <t>4 de 55</t>
-        </is>
-      </c>
-      <c r="M57" s="3" t="inlineStr">
-        <is>
-          <t>2 de 55</t>
-        </is>
-      </c>
-      <c r="N57" s="3" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="O57" s="3" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="P57" s="3" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="Q57" s="3" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="R57" s="3" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
+      <c r="C57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R57" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="C58" s="3" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="D58" s="3" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="E58" s="3" t="inlineStr">
+        <is>
+          <t>2 de 56</t>
+        </is>
+      </c>
+      <c r="F58" s="3" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="G58" s="3" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="H58" s="3" t="inlineStr">
+        <is>
+          <t>1 de 56</t>
+        </is>
+      </c>
+      <c r="I58" s="3" t="inlineStr">
+        <is>
+          <t>1 de 56</t>
+        </is>
+      </c>
+      <c r="J58" s="3" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="K58" s="3" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="L58" s="3" t="inlineStr">
+        <is>
+          <t>4 de 56</t>
+        </is>
+      </c>
+      <c r="M58" s="3" t="inlineStr">
+        <is>
+          <t>2 de 56</t>
+        </is>
+      </c>
+      <c r="N58" s="3" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="O58" s="3" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="P58" s="3" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="Q58" s="3" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="R58" s="3" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
         </is>
       </c>
     </row>
@@ -3953,7 +4013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4690,7 +4750,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>JAIME COELLO ALBERTO FERNANDO</t>
+          <t>GUERRERO GARCIA OLIMPIA ANNABELLE</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
@@ -4717,7 +4777,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
+          <t>JAIME COELLO ALBERTO FERNANDO</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -4744,14 +4804,14 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
+          <t>JIMENEZ CORDERO WILLIAM GUSTAVO</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>430.11</v>
+        <v>0</v>
       </c>
       <c r="E29" s="2" t="n">
         <v>0</v>
@@ -4771,14 +4831,14 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>KITCHENSCO S.A.</t>
+          <t>JUNCO SANCHEZ ARTURO ENRIQUE</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>0</v>
+        <v>430.11</v>
       </c>
       <c r="E30" s="2" t="n">
         <v>0</v>
@@ -4798,7 +4858,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+          <t>KITCHENSCO S.A.</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
@@ -4825,7 +4885,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>LINDAO RODRIGUEZ ANTONIO COLON</t>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
@@ -4838,7 +4898,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>216.76</v>
+        <v>0</v>
       </c>
       <c r="G32" s="2" t="n">
         <v>0</v>
@@ -4852,20 +4912,20 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>LOAIZA TINOCO JUAN PABLO</t>
+          <t>LINDAO RODRIGUEZ ANTONIO COLON</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>551.71</v>
+        <v>0</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>0</v>
+        <v>216.76</v>
       </c>
       <c r="G33" s="2" t="n">
         <v>0</v>
@@ -4879,17 +4939,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>LOZANO MOLINA TITO JERSON</t>
+          <t>LOAIZA TINOCO JUAN PABLO</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>0</v>
+        <v>551.71</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>-166.48</v>
+        <v>0</v>
       </c>
       <c r="F34" s="2" t="n">
         <v>0</v>
@@ -4906,7 +4966,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>MACHARE BARCO LISSETTE STEFANIA</t>
+          <t>LOZANO MOLINA TITO JERSON</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
@@ -4916,7 +4976,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>0</v>
+        <v>-166.48</v>
       </c>
       <c r="F35" s="2" t="n">
         <v>0</v>
@@ -4933,7 +4993,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
+          <t>MACHARE BARCO LISSETTE STEFANIA</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
@@ -4960,7 +5020,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
+          <t>MEZA FERNANDEZ JONATHAN ALEXIS</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
@@ -4987,11 +5047,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>MORALES CAIZA SERGIO IVAN</t>
+          <t>MORA RODRIGUEZ BYRON RIQUELME</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
-        <v>238.35</v>
+        <v>0</v>
       </c>
       <c r="D38" s="2" t="n">
         <v>0</v>
@@ -5014,11 +5074,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>MORAN MARQUEZ DAYSE MARCELA</t>
+          <t>MORALES CAIZA SERGIO IVAN</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>367.8</v>
+        <v>238.35</v>
       </c>
       <c r="D39" s="2" t="n">
         <v>0</v>
@@ -5041,11 +5101,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
+          <t>MORAN MARQUEZ DAYSE MARCELA</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
-        <v>0</v>
+        <v>367.8</v>
       </c>
       <c r="D40" s="2" t="n">
         <v>0</v>
@@ -5068,7 +5128,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>MUÑOZ CALDERON JUAN ADOLFO</t>
+          <t>MOROCHO PLAZA SHIRLEY AURELIA</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
@@ -5081,7 +5141,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>450.22</v>
+        <v>0</v>
       </c>
       <c r="G41" s="2" t="n">
         <v>0</v>
@@ -5095,20 +5155,20 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>PALMA PICO OSCAR FILIDEL</t>
+          <t>MUÑOZ CALDERON JUAN ADOLFO</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>115.52</v>
+        <v>0</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>179.12</v>
+        <v>0</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>517.0599999999999</v>
+        <v>450.22</v>
       </c>
       <c r="G42" s="2" t="n">
         <v>0</v>
@@ -5122,20 +5182,20 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>PAREDES POVEDA TATIANA VERONICA</t>
+          <t>PALMA PICO OSCAR FILIDEL</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>0</v>
+        <v>115.52</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>0</v>
+        <v>179.12</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>0</v>
+        <v>517.0599999999999</v>
       </c>
       <c r="G43" s="2" t="n">
         <v>0</v>
@@ -5149,7 +5209,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>PERDOMO BRIONES JOSÉ ALBERTO</t>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
@@ -5162,7 +5222,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>503.15</v>
+        <v>0</v>
       </c>
       <c r="G44" s="2" t="n">
         <v>0</v>
@@ -5176,7 +5236,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
+          <t>PERDOMO BRIONES JOSÉ ALBERTO</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
@@ -5189,7 +5249,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>0</v>
+        <v>503.15</v>
       </c>
       <c r="G45" s="2" t="n">
         <v>0</v>
@@ -5203,14 +5263,14 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>RAMIREZ MOREIRA MAYRA JACQUELINE</t>
+          <t>QUIJIJE MENDOZA GENESIS XIOMARA</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>44.79</v>
+        <v>0</v>
       </c>
       <c r="E46" s="2" t="n">
         <v>0</v>
@@ -5230,17 +5290,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ROSHANN</t>
+          <t>RAMIREZ MOREIRA MAYRA JACQUELINE</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>0</v>
+        <v>44.79</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>194.16</v>
+        <v>0</v>
       </c>
       <c r="F47" s="2" t="n">
         <v>0</v>
@@ -5257,7 +5317,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
+          <t>ROSHANN</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
@@ -5267,7 +5327,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>0</v>
+        <v>194.16</v>
       </c>
       <c r="F48" s="2" t="n">
         <v>0</v>
@@ -5284,7 +5344,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SOLIS OCAMPO DIMAS ABDON</t>
+          <t>SALAZAR VERA ENRIQUE WILLIAM</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
@@ -5311,14 +5371,14 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SOLIS SOLIS JUAN CARLOS</t>
+          <t>SOLIS OCAMPO DIMAS ABDON</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>5858.53</v>
+        <v>0</v>
       </c>
       <c r="E50" s="2" t="n">
         <v>0</v>
@@ -5338,17 +5398,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>TORRES CADENA JAVIER JOSUE</t>
+          <t>SOLIS SOLIS JUAN CARLOS</t>
         </is>
       </c>
       <c r="C51" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D51" s="2" t="n">
-        <v>0</v>
+        <v>5858.53</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>334.37</v>
+        <v>0</v>
       </c>
       <c r="F51" s="2" t="n">
         <v>0</v>
@@ -5365,17 +5425,17 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>TORRES CADENA JAVIER JOSUE</t>
         </is>
       </c>
       <c r="C52" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D52" s="2" t="n">
-        <v>-10.44</v>
+        <v>0</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>0</v>
+        <v>334.37</v>
       </c>
       <c r="F52" s="2" t="n">
         <v>0</v>
@@ -5392,20 +5452,20 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>VEHINVER SA</t>
+          <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
       <c r="C53" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D53" s="2" t="n">
-        <v>522.8200000000001</v>
+        <v>-10.44</v>
       </c>
       <c r="E53" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>944.42</v>
+        <v>0</v>
       </c>
       <c r="G53" s="2" t="n">
         <v>0</v>
@@ -5419,20 +5479,20 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>VERA TREJO JUAN CARLOS</t>
+          <t>VEHINVER SA</t>
         </is>
       </c>
       <c r="C54" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D54" s="2" t="n">
-        <v>165.83</v>
+        <v>522.8200000000001</v>
       </c>
       <c r="E54" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F54" s="2" t="n">
-        <v>0</v>
+        <v>944.42</v>
       </c>
       <c r="G54" s="2" t="n">
         <v>0</v>
@@ -5446,14 +5506,14 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+          <t>VERA TREJO JUAN CARLOS</t>
         </is>
       </c>
       <c r="C55" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D55" s="2" t="n">
-        <v>0</v>
+        <v>165.83</v>
       </c>
       <c r="E55" s="2" t="n">
         <v>0</v>
@@ -5473,39 +5533,66 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
           <t>ZAVALA MENOSCAL HOMERO MIGUEL</t>
         </is>
       </c>
-      <c r="C56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D56" s="2" t="n">
+      <c r="C57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" s="2" t="n">
         <v>438.86</v>
       </c>
-      <c r="E56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G56" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="C57" s="4" t="n">
+      <c r="E57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="C58" s="4" t="n">
         <v>1566.5</v>
       </c>
-      <c r="D57" s="4" t="n">
+      <c r="D58" s="4" t="n">
         <v>13412.01</v>
       </c>
-      <c r="E57" s="4" t="n">
+      <c r="E58" s="4" t="n">
         <v>574.9</v>
       </c>
-      <c r="F57" s="4" t="n">
+      <c r="F58" s="4" t="n">
         <v>6301.11</v>
       </c>
-      <c r="G57" s="4" t="n">
+      <c r="G58" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-11-28 13:30:09
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -5694,10 +5694,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>9141.17</v>
+        <v>9400.370000000001</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>-9141.17</v>
+        <v>-9400.370000000001</v>
       </c>
       <c r="F3" s="5" t="n">
         <v>0</v>
@@ -5737,13 +5737,13 @@
         <v>26086.41</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>24713.65</v>
+        <v>24972.85</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>1372.76</v>
+        <v>1113.559999999999</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>0.9473764308695601</v>
+        <v>0.957312639033121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-12-01 11:30:08
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -1667,10 +1667,10 @@
         <v>0</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>0</v>
+        <v>392.4</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>0</v>
+        <v>575.64</v>
       </c>
       <c r="J20" s="2" t="n">
         <v>0</v>
@@ -3948,12 +3948,12 @@
       </c>
       <c r="H58" s="3" t="inlineStr">
         <is>
-          <t>0 de 56</t>
+          <t>1 de 56</t>
         </is>
       </c>
       <c r="I58" s="3" t="inlineStr">
         <is>
-          <t>0 de 56</t>
+          <t>1 de 56</t>
         </is>
       </c>
       <c r="J58" s="3" t="inlineStr">
@@ -4574,7 +4574,7 @@
         <v>3669.5</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>0</v>
+        <v>968.04</v>
       </c>
       <c r="G20" s="2" t="n">
         <v>0</v>
@@ -5590,7 +5590,7 @@
         <v>6694.99</v>
       </c>
       <c r="F58" s="4" t="n">
-        <v>0</v>
+        <v>968.04</v>
       </c>
       <c r="G58" s="4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Actualización automática 2025-12-04 17:30:07
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -3176,7 +3176,7 @@
         <v>0</v>
       </c>
       <c r="K45" s="2" t="n">
-        <v>0</v>
+        <v>137.52</v>
       </c>
       <c r="L45" s="2" t="n">
         <v>0</v>
@@ -4023,7 +4023,7 @@
       </c>
       <c r="K59" s="3" t="inlineStr">
         <is>
-          <t>0 de 57</t>
+          <t>1 de 57</t>
         </is>
       </c>
       <c r="L59" s="3" t="inlineStr">
@@ -5309,7 +5309,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>0</v>
+        <v>137.52</v>
       </c>
       <c r="G45" s="2" t="n">
         <v>0</v>
@@ -5677,7 +5677,7 @@
         <v>6694.99</v>
       </c>
       <c r="F59" s="4" t="n">
-        <v>1339.9</v>
+        <v>1477.42</v>
       </c>
       <c r="G59" s="4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Actualización automática 2025-12-08 12:30:06
</commit_message>
<xml_diff>
--- a/data/OFICINA-CATAECSA.xlsx
+++ b/data/OFICINA-CATAECSA.xlsx
@@ -3776,7 +3776,7 @@
         <v>0</v>
       </c>
       <c r="K55" s="2" t="n">
-        <v>0</v>
+        <v>537.98</v>
       </c>
       <c r="L55" s="2" t="n">
         <v>0</v>
@@ -4023,7 +4023,7 @@
       </c>
       <c r="K59" s="3" t="inlineStr">
         <is>
-          <t>1 de 57</t>
+          <t>2 de 57</t>
         </is>
       </c>
       <c r="L59" s="3" t="inlineStr">
@@ -5579,7 +5579,7 @@
         <v>944.42</v>
       </c>
       <c r="F55" s="2" t="n">
-        <v>0</v>
+        <v>537.98</v>
       </c>
       <c r="G55" s="2" t="n">
         <v>0</v>
@@ -5677,7 +5677,7 @@
         <v>6694.99</v>
       </c>
       <c r="F59" s="4" t="n">
-        <v>1477.42</v>
+        <v>2015.4</v>
       </c>
       <c r="G59" s="4" t="n">
         <v>0</v>

</xml_diff>